<commit_message>
added table header, fixed column range
from 7 to 6
</commit_message>
<xml_diff>
--- a/static/Honors.xlsx
+++ b/static/Honors.xlsx
@@ -39,7 +39,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -61,11 +61,88 @@
         <color rgb="00000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -82,7 +159,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -466,7 +548,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,7 +562,6 @@
     <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -494,7 +575,6 @@
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -507,7 +587,6 @@
       <c r="D2" s="1" t="n"/>
       <c r="E2" s="1" t="n"/>
       <c r="F2" s="1" t="n"/>
-      <c r="G2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -520,7 +599,6 @@
       <c r="D3" s="1" t="n"/>
       <c r="E3" s="1" t="n"/>
       <c r="F3" s="1" t="n"/>
-      <c r="G3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -533,10 +611,9 @@
       <c r="D4" s="1" t="n"/>
       <c r="E4" s="1" t="n"/>
       <c r="F4" s="1" t="n"/>
-      <c r="G4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="G5" s="3" t="inlineStr">
+      <c r="F5" s="3" t="inlineStr">
         <is>
           <t>July 08, 2021</t>
         </is>
@@ -553,7 +630,6 @@
       <c r="D7" s="4" t="n"/>
       <c r="E7" s="4" t="n"/>
       <c r="F7" s="4" t="n"/>
-      <c r="G7" s="4" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
@@ -566,7 +642,6 @@
       <c r="D8" s="4" t="n"/>
       <c r="E8" s="4" t="n"/>
       <c r="F8" s="4" t="n"/>
-      <c r="G8" s="4" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
@@ -579,7 +654,6 @@
       <c r="D9" s="4" t="n"/>
       <c r="E9" s="4" t="n"/>
       <c r="F9" s="4" t="n"/>
-      <c r="G9" s="4" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -610,22 +684,48 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="n"/>
-      <c r="B19" s="6" t="n"/>
-      <c r="C19" s="6" t="n"/>
-      <c r="D19" s="6" t="n"/>
-      <c r="E19" s="6" t="n"/>
-      <c r="F19" s="6" t="n"/>
-      <c r="G19" s="6" t="n"/>
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="B19" s="6" t="inlineStr">
+        <is>
+          <t>NAME</t>
+        </is>
+      </c>
+      <c r="C19" s="6" t="inlineStr">
+        <is>
+          <t>RATING</t>
+        </is>
+      </c>
+      <c r="D19" s="7" t="n"/>
+      <c r="E19" s="8" t="n"/>
+      <c r="F19" s="6" t="inlineStr">
+        <is>
+          <t>AWARD</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="n"/>
-      <c r="B20" s="6" t="n"/>
-      <c r="C20" s="6" t="n"/>
-      <c r="D20" s="6" t="n"/>
-      <c r="E20" s="6" t="n"/>
-      <c r="F20" s="6" t="n"/>
-      <c r="G20" s="6" t="n"/>
+      <c r="B20" s="9" t="n"/>
+      <c r="C20" s="6" t="inlineStr">
+        <is>
+          <t>Sum of Grades</t>
+        </is>
+      </c>
+      <c r="D20" s="6" t="inlineStr">
+        <is>
+          <t>Total Units</t>
+        </is>
+      </c>
+      <c r="E20" s="6" t="inlineStr">
+        <is>
+          <t>Final GWA</t>
+        </is>
+      </c>
+      <c r="F20" s="9" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="6" t="n"/>
@@ -634,7 +734,6 @@
       <c r="D21" s="6" t="n"/>
       <c r="E21" s="6" t="n"/>
       <c r="F21" s="6" t="n"/>
-      <c r="G21" s="6" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="6" t="n"/>
@@ -643,7 +742,6 @@
       <c r="D22" s="6" t="n"/>
       <c r="E22" s="6" t="n"/>
       <c r="F22" s="6" t="n"/>
-      <c r="G22" s="6" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="6" t="n"/>
@@ -652,7 +750,6 @@
       <c r="D23" s="6" t="n"/>
       <c r="E23" s="6" t="n"/>
       <c r="F23" s="6" t="n"/>
-      <c r="G23" s="6" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="6" t="n"/>
@@ -661,7 +758,6 @@
       <c r="D24" s="6" t="n"/>
       <c r="E24" s="6" t="n"/>
       <c r="F24" s="6" t="n"/>
-      <c r="G24" s="6" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="6" t="n"/>
@@ -670,7 +766,6 @@
       <c r="D25" s="6" t="n"/>
       <c r="E25" s="6" t="n"/>
       <c r="F25" s="6" t="n"/>
-      <c r="G25" s="6" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="6" t="n"/>
@@ -679,7 +774,6 @@
       <c r="D26" s="6" t="n"/>
       <c r="E26" s="6" t="n"/>
       <c r="F26" s="6" t="n"/>
-      <c r="G26" s="6" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="6" t="n"/>
@@ -688,7 +782,6 @@
       <c r="D27" s="6" t="n"/>
       <c r="E27" s="6" t="n"/>
       <c r="F27" s="6" t="n"/>
-      <c r="G27" s="6" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="6" t="n"/>
@@ -697,7 +790,6 @@
       <c r="D28" s="6" t="n"/>
       <c r="E28" s="6" t="n"/>
       <c r="F28" s="6" t="n"/>
-      <c r="G28" s="6" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="6" t="n"/>
@@ -706,7 +798,6 @@
       <c r="D29" s="6" t="n"/>
       <c r="E29" s="6" t="n"/>
       <c r="F29" s="6" t="n"/>
-      <c r="G29" s="6" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="6" t="n"/>
@@ -715,7 +806,6 @@
       <c r="D30" s="6" t="n"/>
       <c r="E30" s="6" t="n"/>
       <c r="F30" s="6" t="n"/>
-      <c r="G30" s="6" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="6" t="n"/>
@@ -724,7 +814,6 @@
       <c r="D31" s="6" t="n"/>
       <c r="E31" s="6" t="n"/>
       <c r="F31" s="6" t="n"/>
-      <c r="G31" s="6" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="6" t="n"/>
@@ -733,7 +822,6 @@
       <c r="D32" s="6" t="n"/>
       <c r="E32" s="6" t="n"/>
       <c r="F32" s="6" t="n"/>
-      <c r="G32" s="6" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="6" t="n"/>
@@ -742,7 +830,6 @@
       <c r="D33" s="6" t="n"/>
       <c r="E33" s="6" t="n"/>
       <c r="F33" s="6" t="n"/>
-      <c r="G33" s="6" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="6" t="n"/>
@@ -751,7 +838,6 @@
       <c r="D34" s="6" t="n"/>
       <c r="E34" s="6" t="n"/>
       <c r="F34" s="6" t="n"/>
-      <c r="G34" s="6" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="6" t="n"/>
@@ -760,7 +846,6 @@
       <c r="D35" s="6" t="n"/>
       <c r="E35" s="6" t="n"/>
       <c r="F35" s="6" t="n"/>
-      <c r="G35" s="6" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="6" t="n"/>
@@ -769,7 +854,6 @@
       <c r="D36" s="6" t="n"/>
       <c r="E36" s="6" t="n"/>
       <c r="F36" s="6" t="n"/>
-      <c r="G36" s="6" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="6" t="n"/>
@@ -778,7 +862,6 @@
       <c r="D37" s="6" t="n"/>
       <c r="E37" s="6" t="n"/>
       <c r="F37" s="6" t="n"/>
-      <c r="G37" s="6" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="6" t="n"/>
@@ -787,7 +870,6 @@
       <c r="D38" s="6" t="n"/>
       <c r="E38" s="6" t="n"/>
       <c r="F38" s="6" t="n"/>
-      <c r="G38" s="6" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="6" t="n"/>
@@ -796,7 +878,6 @@
       <c r="D39" s="6" t="n"/>
       <c r="E39" s="6" t="n"/>
       <c r="F39" s="6" t="n"/>
-      <c r="G39" s="6" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="6" t="n"/>
@@ -805,7 +886,6 @@
       <c r="D40" s="6" t="n"/>
       <c r="E40" s="6" t="n"/>
       <c r="F40" s="6" t="n"/>
-      <c r="G40" s="6" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="6" t="n"/>
@@ -814,7 +894,6 @@
       <c r="D41" s="6" t="n"/>
       <c r="E41" s="6" t="n"/>
       <c r="F41" s="6" t="n"/>
-      <c r="G41" s="6" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="6" t="n"/>
@@ -823,7 +902,6 @@
       <c r="D42" s="6" t="n"/>
       <c r="E42" s="6" t="n"/>
       <c r="F42" s="6" t="n"/>
-      <c r="G42" s="6" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="6" t="n"/>
@@ -832,7 +910,6 @@
       <c r="D43" s="6" t="n"/>
       <c r="E43" s="6" t="n"/>
       <c r="F43" s="6" t="n"/>
-      <c r="G43" s="6" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="6" t="n"/>
@@ -841,7 +918,6 @@
       <c r="D44" s="6" t="n"/>
       <c r="E44" s="6" t="n"/>
       <c r="F44" s="6" t="n"/>
-      <c r="G44" s="6" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="6" t="n"/>
@@ -850,7 +926,6 @@
       <c r="D45" s="6" t="n"/>
       <c r="E45" s="6" t="n"/>
       <c r="F45" s="6" t="n"/>
-      <c r="G45" s="6" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="6" t="n"/>
@@ -859,7 +934,6 @@
       <c r="D46" s="6" t="n"/>
       <c r="E46" s="6" t="n"/>
       <c r="F46" s="6" t="n"/>
-      <c r="G46" s="6" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="6" t="n"/>
@@ -868,7 +942,6 @@
       <c r="D47" s="6" t="n"/>
       <c r="E47" s="6" t="n"/>
       <c r="F47" s="6" t="n"/>
-      <c r="G47" s="6" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="6" t="n"/>
@@ -877,7 +950,6 @@
       <c r="D48" s="6" t="n"/>
       <c r="E48" s="6" t="n"/>
       <c r="F48" s="6" t="n"/>
-      <c r="G48" s="6" t="n"/>
     </row>
     <row r="49">
       <c r="A49" s="6" t="n"/>
@@ -886,7 +958,6 @@
       <c r="D49" s="6" t="n"/>
       <c r="E49" s="6" t="n"/>
       <c r="F49" s="6" t="n"/>
-      <c r="G49" s="6" t="n"/>
     </row>
     <row r="50">
       <c r="A50" s="6" t="n"/>
@@ -895,7 +966,6 @@
       <c r="D50" s="6" t="n"/>
       <c r="E50" s="6" t="n"/>
       <c r="F50" s="6" t="n"/>
-      <c r="G50" s="6" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="6" t="n"/>
@@ -904,7 +974,6 @@
       <c r="D51" s="6" t="n"/>
       <c r="E51" s="6" t="n"/>
       <c r="F51" s="6" t="n"/>
-      <c r="G51" s="6" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="6" t="n"/>
@@ -913,7 +982,6 @@
       <c r="D52" s="6" t="n"/>
       <c r="E52" s="6" t="n"/>
       <c r="F52" s="6" t="n"/>
-      <c r="G52" s="6" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="6" t="n"/>
@@ -922,7 +990,6 @@
       <c r="D53" s="6" t="n"/>
       <c r="E53" s="6" t="n"/>
       <c r="F53" s="6" t="n"/>
-      <c r="G53" s="6" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="6" t="n"/>
@@ -931,7 +998,6 @@
       <c r="D54" s="6" t="n"/>
       <c r="E54" s="6" t="n"/>
       <c r="F54" s="6" t="n"/>
-      <c r="G54" s="6" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="6" t="n"/>
@@ -940,7 +1006,6 @@
       <c r="D55" s="6" t="n"/>
       <c r="E55" s="6" t="n"/>
       <c r="F55" s="6" t="n"/>
-      <c r="G55" s="6" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="6" t="n"/>
@@ -949,7 +1014,6 @@
       <c r="D56" s="6" t="n"/>
       <c r="E56" s="6" t="n"/>
       <c r="F56" s="6" t="n"/>
-      <c r="G56" s="6" t="n"/>
     </row>
     <row r="57">
       <c r="A57" s="6" t="n"/>
@@ -958,7 +1022,6 @@
       <c r="D57" s="6" t="n"/>
       <c r="E57" s="6" t="n"/>
       <c r="F57" s="6" t="n"/>
-      <c r="G57" s="6" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="6" t="n"/>
@@ -967,7 +1030,6 @@
       <c r="D58" s="6" t="n"/>
       <c r="E58" s="6" t="n"/>
       <c r="F58" s="6" t="n"/>
-      <c r="G58" s="6" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="6" t="n"/>
@@ -976,7 +1038,6 @@
       <c r="D59" s="6" t="n"/>
       <c r="E59" s="6" t="n"/>
       <c r="F59" s="6" t="n"/>
-      <c r="G59" s="6" t="n"/>
     </row>
     <row r="60">
       <c r="A60" s="6" t="n"/>
@@ -985,7 +1046,6 @@
       <c r="D60" s="6" t="n"/>
       <c r="E60" s="6" t="n"/>
       <c r="F60" s="6" t="n"/>
-      <c r="G60" s="6" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="6" t="n"/>
@@ -994,7 +1054,6 @@
       <c r="D61" s="6" t="n"/>
       <c r="E61" s="6" t="n"/>
       <c r="F61" s="6" t="n"/>
-      <c r="G61" s="6" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="6" t="n"/>
@@ -1003,7 +1062,6 @@
       <c r="D62" s="6" t="n"/>
       <c r="E62" s="6" t="n"/>
       <c r="F62" s="6" t="n"/>
-      <c r="G62" s="6" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="6" t="n"/>
@@ -1012,7 +1070,6 @@
       <c r="D63" s="6" t="n"/>
       <c r="E63" s="6" t="n"/>
       <c r="F63" s="6" t="n"/>
-      <c r="G63" s="6" t="n"/>
     </row>
     <row r="64">
       <c r="A64" s="6" t="n"/>
@@ -1021,7 +1078,6 @@
       <c r="D64" s="6" t="n"/>
       <c r="E64" s="6" t="n"/>
       <c r="F64" s="6" t="n"/>
-      <c r="G64" s="6" t="n"/>
     </row>
     <row r="65">
       <c r="A65" s="6" t="n"/>
@@ -1030,7 +1086,6 @@
       <c r="D65" s="6" t="n"/>
       <c r="E65" s="6" t="n"/>
       <c r="F65" s="6" t="n"/>
-      <c r="G65" s="6" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="6" t="n"/>
@@ -1039,7 +1094,6 @@
       <c r="D66" s="6" t="n"/>
       <c r="E66" s="6" t="n"/>
       <c r="F66" s="6" t="n"/>
-      <c r="G66" s="6" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="6" t="n"/>
@@ -1048,7 +1102,6 @@
       <c r="D67" s="6" t="n"/>
       <c r="E67" s="6" t="n"/>
       <c r="F67" s="6" t="n"/>
-      <c r="G67" s="6" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="6" t="n"/>
@@ -1057,7 +1110,6 @@
       <c r="D68" s="6" t="n"/>
       <c r="E68" s="6" t="n"/>
       <c r="F68" s="6" t="n"/>
-      <c r="G68" s="6" t="n"/>
     </row>
     <row r="69">
       <c r="A69" s="6" t="n"/>
@@ -1066,7 +1118,6 @@
       <c r="D69" s="6" t="n"/>
       <c r="E69" s="6" t="n"/>
       <c r="F69" s="6" t="n"/>
-      <c r="G69" s="6" t="n"/>
     </row>
     <row r="70">
       <c r="A70" s="6" t="n"/>
@@ -1075,7 +1126,6 @@
       <c r="D70" s="6" t="n"/>
       <c r="E70" s="6" t="n"/>
       <c r="F70" s="6" t="n"/>
-      <c r="G70" s="6" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="6" t="n"/>
@@ -1084,7 +1134,6 @@
       <c r="D71" s="6" t="n"/>
       <c r="E71" s="6" t="n"/>
       <c r="F71" s="6" t="n"/>
-      <c r="G71" s="6" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="6" t="n"/>
@@ -1093,7 +1142,6 @@
       <c r="D72" s="6" t="n"/>
       <c r="E72" s="6" t="n"/>
       <c r="F72" s="6" t="n"/>
-      <c r="G72" s="6" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="6" t="n"/>
@@ -1102,7 +1150,6 @@
       <c r="D73" s="6" t="n"/>
       <c r="E73" s="6" t="n"/>
       <c r="F73" s="6" t="n"/>
-      <c r="G73" s="6" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="6" t="n"/>
@@ -1111,7 +1158,6 @@
       <c r="D74" s="6" t="n"/>
       <c r="E74" s="6" t="n"/>
       <c r="F74" s="6" t="n"/>
-      <c r="G74" s="6" t="n"/>
     </row>
     <row r="75">
       <c r="A75" s="6" t="n"/>
@@ -1120,7 +1166,6 @@
       <c r="D75" s="6" t="n"/>
       <c r="E75" s="6" t="n"/>
       <c r="F75" s="6" t="n"/>
-      <c r="G75" s="6" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="6" t="n"/>
@@ -1129,7 +1174,6 @@
       <c r="D76" s="6" t="n"/>
       <c r="E76" s="6" t="n"/>
       <c r="F76" s="6" t="n"/>
-      <c r="G76" s="6" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="6" t="n"/>
@@ -1138,7 +1182,6 @@
       <c r="D77" s="6" t="n"/>
       <c r="E77" s="6" t="n"/>
       <c r="F77" s="6" t="n"/>
-      <c r="G77" s="6" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="6" t="n"/>
@@ -1147,7 +1190,6 @@
       <c r="D78" s="6" t="n"/>
       <c r="E78" s="6" t="n"/>
       <c r="F78" s="6" t="n"/>
-      <c r="G78" s="6" t="n"/>
     </row>
     <row r="79">
       <c r="A79" s="6" t="n"/>
@@ -1156,7 +1198,6 @@
       <c r="D79" s="6" t="n"/>
       <c r="E79" s="6" t="n"/>
       <c r="F79" s="6" t="n"/>
-      <c r="G79" s="6" t="n"/>
     </row>
     <row r="80">
       <c r="A80" s="6" t="n"/>
@@ -1165,7 +1206,6 @@
       <c r="D80" s="6" t="n"/>
       <c r="E80" s="6" t="n"/>
       <c r="F80" s="6" t="n"/>
-      <c r="G80" s="6" t="n"/>
     </row>
     <row r="81">
       <c r="A81" s="6" t="n"/>
@@ -1174,7 +1214,6 @@
       <c r="D81" s="6" t="n"/>
       <c r="E81" s="6" t="n"/>
       <c r="F81" s="6" t="n"/>
-      <c r="G81" s="6" t="n"/>
     </row>
     <row r="82">
       <c r="A82" s="6" t="n"/>
@@ -1183,7 +1222,6 @@
       <c r="D82" s="6" t="n"/>
       <c r="E82" s="6" t="n"/>
       <c r="F82" s="6" t="n"/>
-      <c r="G82" s="6" t="n"/>
     </row>
     <row r="83">
       <c r="A83" s="6" t="n"/>
@@ -1192,7 +1230,6 @@
       <c r="D83" s="6" t="n"/>
       <c r="E83" s="6" t="n"/>
       <c r="F83" s="6" t="n"/>
-      <c r="G83" s="6" t="n"/>
     </row>
     <row r="84">
       <c r="A84" s="6" t="n"/>
@@ -1201,7 +1238,6 @@
       <c r="D84" s="6" t="n"/>
       <c r="E84" s="6" t="n"/>
       <c r="F84" s="6" t="n"/>
-      <c r="G84" s="6" t="n"/>
     </row>
     <row r="85">
       <c r="A85" s="6" t="n"/>
@@ -1210,7 +1246,6 @@
       <c r="D85" s="6" t="n"/>
       <c r="E85" s="6" t="n"/>
       <c r="F85" s="6" t="n"/>
-      <c r="G85" s="6" t="n"/>
     </row>
     <row r="86">
       <c r="A86" s="6" t="n"/>
@@ -1219,17 +1254,19 @@
       <c r="D86" s="6" t="n"/>
       <c r="E86" s="6" t="n"/>
       <c r="F86" s="6" t="n"/>
-      <c r="G86" s="6" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:G17"/>
+  <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:F20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperHeight="13in" paperWidth="8.5in"/>

</xml_diff>

<commit_message>
font size table data
</commit_message>
<xml_diff>
--- a/static/Honors.xlsx
+++ b/static/Honors.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,6 +29,11 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <strike val="0"/>
+      <sz val="9"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -165,6 +170,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -728,532 +736,532 @@
       <c r="F20" s="9" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="6" t="n"/>
-      <c r="B21" s="6" t="n"/>
-      <c r="C21" s="6" t="n"/>
-      <c r="D21" s="6" t="n"/>
-      <c r="E21" s="6" t="n"/>
-      <c r="F21" s="6" t="n"/>
+      <c r="A21" s="10" t="n"/>
+      <c r="B21" s="10" t="n"/>
+      <c r="C21" s="10" t="n"/>
+      <c r="D21" s="10" t="n"/>
+      <c r="E21" s="10" t="n"/>
+      <c r="F21" s="10" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="6" t="n"/>
-      <c r="B22" s="6" t="n"/>
-      <c r="C22" s="6" t="n"/>
-      <c r="D22" s="6" t="n"/>
-      <c r="E22" s="6" t="n"/>
-      <c r="F22" s="6" t="n"/>
+      <c r="A22" s="10" t="n"/>
+      <c r="B22" s="10" t="n"/>
+      <c r="C22" s="10" t="n"/>
+      <c r="D22" s="10" t="n"/>
+      <c r="E22" s="10" t="n"/>
+      <c r="F22" s="10" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="6" t="n"/>
-      <c r="B23" s="6" t="n"/>
-      <c r="C23" s="6" t="n"/>
-      <c r="D23" s="6" t="n"/>
-      <c r="E23" s="6" t="n"/>
-      <c r="F23" s="6" t="n"/>
+      <c r="A23" s="10" t="n"/>
+      <c r="B23" s="10" t="n"/>
+      <c r="C23" s="10" t="n"/>
+      <c r="D23" s="10" t="n"/>
+      <c r="E23" s="10" t="n"/>
+      <c r="F23" s="10" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="n"/>
-      <c r="B24" s="6" t="n"/>
-      <c r="C24" s="6" t="n"/>
-      <c r="D24" s="6" t="n"/>
-      <c r="E24" s="6" t="n"/>
-      <c r="F24" s="6" t="n"/>
+      <c r="A24" s="10" t="n"/>
+      <c r="B24" s="10" t="n"/>
+      <c r="C24" s="10" t="n"/>
+      <c r="D24" s="10" t="n"/>
+      <c r="E24" s="10" t="n"/>
+      <c r="F24" s="10" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="6" t="n"/>
-      <c r="B25" s="6" t="n"/>
-      <c r="C25" s="6" t="n"/>
-      <c r="D25" s="6" t="n"/>
-      <c r="E25" s="6" t="n"/>
-      <c r="F25" s="6" t="n"/>
+      <c r="A25" s="10" t="n"/>
+      <c r="B25" s="10" t="n"/>
+      <c r="C25" s="10" t="n"/>
+      <c r="D25" s="10" t="n"/>
+      <c r="E25" s="10" t="n"/>
+      <c r="F25" s="10" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="6" t="n"/>
-      <c r="B26" s="6" t="n"/>
-      <c r="C26" s="6" t="n"/>
-      <c r="D26" s="6" t="n"/>
-      <c r="E26" s="6" t="n"/>
-      <c r="F26" s="6" t="n"/>
+      <c r="A26" s="10" t="n"/>
+      <c r="B26" s="10" t="n"/>
+      <c r="C26" s="10" t="n"/>
+      <c r="D26" s="10" t="n"/>
+      <c r="E26" s="10" t="n"/>
+      <c r="F26" s="10" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="6" t="n"/>
-      <c r="B27" s="6" t="n"/>
-      <c r="C27" s="6" t="n"/>
-      <c r="D27" s="6" t="n"/>
-      <c r="E27" s="6" t="n"/>
-      <c r="F27" s="6" t="n"/>
+      <c r="A27" s="10" t="n"/>
+      <c r="B27" s="10" t="n"/>
+      <c r="C27" s="10" t="n"/>
+      <c r="D27" s="10" t="n"/>
+      <c r="E27" s="10" t="n"/>
+      <c r="F27" s="10" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="6" t="n"/>
-      <c r="B28" s="6" t="n"/>
-      <c r="C28" s="6" t="n"/>
-      <c r="D28" s="6" t="n"/>
-      <c r="E28" s="6" t="n"/>
-      <c r="F28" s="6" t="n"/>
+      <c r="A28" s="10" t="n"/>
+      <c r="B28" s="10" t="n"/>
+      <c r="C28" s="10" t="n"/>
+      <c r="D28" s="10" t="n"/>
+      <c r="E28" s="10" t="n"/>
+      <c r="F28" s="10" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="6" t="n"/>
-      <c r="B29" s="6" t="n"/>
-      <c r="C29" s="6" t="n"/>
-      <c r="D29" s="6" t="n"/>
-      <c r="E29" s="6" t="n"/>
-      <c r="F29" s="6" t="n"/>
+      <c r="A29" s="10" t="n"/>
+      <c r="B29" s="10" t="n"/>
+      <c r="C29" s="10" t="n"/>
+      <c r="D29" s="10" t="n"/>
+      <c r="E29" s="10" t="n"/>
+      <c r="F29" s="10" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="6" t="n"/>
-      <c r="B30" s="6" t="n"/>
-      <c r="C30" s="6" t="n"/>
-      <c r="D30" s="6" t="n"/>
-      <c r="E30" s="6" t="n"/>
-      <c r="F30" s="6" t="n"/>
+      <c r="A30" s="10" t="n"/>
+      <c r="B30" s="10" t="n"/>
+      <c r="C30" s="10" t="n"/>
+      <c r="D30" s="10" t="n"/>
+      <c r="E30" s="10" t="n"/>
+      <c r="F30" s="10" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="6" t="n"/>
-      <c r="B31" s="6" t="n"/>
-      <c r="C31" s="6" t="n"/>
-      <c r="D31" s="6" t="n"/>
-      <c r="E31" s="6" t="n"/>
-      <c r="F31" s="6" t="n"/>
+      <c r="A31" s="10" t="n"/>
+      <c r="B31" s="10" t="n"/>
+      <c r="C31" s="10" t="n"/>
+      <c r="D31" s="10" t="n"/>
+      <c r="E31" s="10" t="n"/>
+      <c r="F31" s="10" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="6" t="n"/>
-      <c r="B32" s="6" t="n"/>
-      <c r="C32" s="6" t="n"/>
-      <c r="D32" s="6" t="n"/>
-      <c r="E32" s="6" t="n"/>
-      <c r="F32" s="6" t="n"/>
+      <c r="A32" s="10" t="n"/>
+      <c r="B32" s="10" t="n"/>
+      <c r="C32" s="10" t="n"/>
+      <c r="D32" s="10" t="n"/>
+      <c r="E32" s="10" t="n"/>
+      <c r="F32" s="10" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="6" t="n"/>
-      <c r="B33" s="6" t="n"/>
-      <c r="C33" s="6" t="n"/>
-      <c r="D33" s="6" t="n"/>
-      <c r="E33" s="6" t="n"/>
-      <c r="F33" s="6" t="n"/>
+      <c r="A33" s="10" t="n"/>
+      <c r="B33" s="10" t="n"/>
+      <c r="C33" s="10" t="n"/>
+      <c r="D33" s="10" t="n"/>
+      <c r="E33" s="10" t="n"/>
+      <c r="F33" s="10" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="6" t="n"/>
-      <c r="B34" s="6" t="n"/>
-      <c r="C34" s="6" t="n"/>
-      <c r="D34" s="6" t="n"/>
-      <c r="E34" s="6" t="n"/>
-      <c r="F34" s="6" t="n"/>
+      <c r="A34" s="10" t="n"/>
+      <c r="B34" s="10" t="n"/>
+      <c r="C34" s="10" t="n"/>
+      <c r="D34" s="10" t="n"/>
+      <c r="E34" s="10" t="n"/>
+      <c r="F34" s="10" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="6" t="n"/>
-      <c r="B35" s="6" t="n"/>
-      <c r="C35" s="6" t="n"/>
-      <c r="D35" s="6" t="n"/>
-      <c r="E35" s="6" t="n"/>
-      <c r="F35" s="6" t="n"/>
+      <c r="A35" s="10" t="n"/>
+      <c r="B35" s="10" t="n"/>
+      <c r="C35" s="10" t="n"/>
+      <c r="D35" s="10" t="n"/>
+      <c r="E35" s="10" t="n"/>
+      <c r="F35" s="10" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="6" t="n"/>
-      <c r="B36" s="6" t="n"/>
-      <c r="C36" s="6" t="n"/>
-      <c r="D36" s="6" t="n"/>
-      <c r="E36" s="6" t="n"/>
-      <c r="F36" s="6" t="n"/>
+      <c r="A36" s="10" t="n"/>
+      <c r="B36" s="10" t="n"/>
+      <c r="C36" s="10" t="n"/>
+      <c r="D36" s="10" t="n"/>
+      <c r="E36" s="10" t="n"/>
+      <c r="F36" s="10" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="6" t="n"/>
-      <c r="B37" s="6" t="n"/>
-      <c r="C37" s="6" t="n"/>
-      <c r="D37" s="6" t="n"/>
-      <c r="E37" s="6" t="n"/>
-      <c r="F37" s="6" t="n"/>
+      <c r="A37" s="10" t="n"/>
+      <c r="B37" s="10" t="n"/>
+      <c r="C37" s="10" t="n"/>
+      <c r="D37" s="10" t="n"/>
+      <c r="E37" s="10" t="n"/>
+      <c r="F37" s="10" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="6" t="n"/>
-      <c r="B38" s="6" t="n"/>
-      <c r="C38" s="6" t="n"/>
-      <c r="D38" s="6" t="n"/>
-      <c r="E38" s="6" t="n"/>
-      <c r="F38" s="6" t="n"/>
+      <c r="A38" s="10" t="n"/>
+      <c r="B38" s="10" t="n"/>
+      <c r="C38" s="10" t="n"/>
+      <c r="D38" s="10" t="n"/>
+      <c r="E38" s="10" t="n"/>
+      <c r="F38" s="10" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="6" t="n"/>
-      <c r="B39" s="6" t="n"/>
-      <c r="C39" s="6" t="n"/>
-      <c r="D39" s="6" t="n"/>
-      <c r="E39" s="6" t="n"/>
-      <c r="F39" s="6" t="n"/>
+      <c r="A39" s="10" t="n"/>
+      <c r="B39" s="10" t="n"/>
+      <c r="C39" s="10" t="n"/>
+      <c r="D39" s="10" t="n"/>
+      <c r="E39" s="10" t="n"/>
+      <c r="F39" s="10" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="6" t="n"/>
-      <c r="B40" s="6" t="n"/>
-      <c r="C40" s="6" t="n"/>
-      <c r="D40" s="6" t="n"/>
-      <c r="E40" s="6" t="n"/>
-      <c r="F40" s="6" t="n"/>
+      <c r="A40" s="10" t="n"/>
+      <c r="B40" s="10" t="n"/>
+      <c r="C40" s="10" t="n"/>
+      <c r="D40" s="10" t="n"/>
+      <c r="E40" s="10" t="n"/>
+      <c r="F40" s="10" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="6" t="n"/>
-      <c r="B41" s="6" t="n"/>
-      <c r="C41" s="6" t="n"/>
-      <c r="D41" s="6" t="n"/>
-      <c r="E41" s="6" t="n"/>
-      <c r="F41" s="6" t="n"/>
+      <c r="A41" s="10" t="n"/>
+      <c r="B41" s="10" t="n"/>
+      <c r="C41" s="10" t="n"/>
+      <c r="D41" s="10" t="n"/>
+      <c r="E41" s="10" t="n"/>
+      <c r="F41" s="10" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="6" t="n"/>
-      <c r="B42" s="6" t="n"/>
-      <c r="C42" s="6" t="n"/>
-      <c r="D42" s="6" t="n"/>
-      <c r="E42" s="6" t="n"/>
-      <c r="F42" s="6" t="n"/>
+      <c r="A42" s="10" t="n"/>
+      <c r="B42" s="10" t="n"/>
+      <c r="C42" s="10" t="n"/>
+      <c r="D42" s="10" t="n"/>
+      <c r="E42" s="10" t="n"/>
+      <c r="F42" s="10" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="6" t="n"/>
-      <c r="B43" s="6" t="n"/>
-      <c r="C43" s="6" t="n"/>
-      <c r="D43" s="6" t="n"/>
-      <c r="E43" s="6" t="n"/>
-      <c r="F43" s="6" t="n"/>
+      <c r="A43" s="10" t="n"/>
+      <c r="B43" s="10" t="n"/>
+      <c r="C43" s="10" t="n"/>
+      <c r="D43" s="10" t="n"/>
+      <c r="E43" s="10" t="n"/>
+      <c r="F43" s="10" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="6" t="n"/>
-      <c r="B44" s="6" t="n"/>
-      <c r="C44" s="6" t="n"/>
-      <c r="D44" s="6" t="n"/>
-      <c r="E44" s="6" t="n"/>
-      <c r="F44" s="6" t="n"/>
+      <c r="A44" s="10" t="n"/>
+      <c r="B44" s="10" t="n"/>
+      <c r="C44" s="10" t="n"/>
+      <c r="D44" s="10" t="n"/>
+      <c r="E44" s="10" t="n"/>
+      <c r="F44" s="10" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="6" t="n"/>
-      <c r="B45" s="6" t="n"/>
-      <c r="C45" s="6" t="n"/>
-      <c r="D45" s="6" t="n"/>
-      <c r="E45" s="6" t="n"/>
-      <c r="F45" s="6" t="n"/>
+      <c r="A45" s="10" t="n"/>
+      <c r="B45" s="10" t="n"/>
+      <c r="C45" s="10" t="n"/>
+      <c r="D45" s="10" t="n"/>
+      <c r="E45" s="10" t="n"/>
+      <c r="F45" s="10" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="6" t="n"/>
-      <c r="B46" s="6" t="n"/>
-      <c r="C46" s="6" t="n"/>
-      <c r="D46" s="6" t="n"/>
-      <c r="E46" s="6" t="n"/>
-      <c r="F46" s="6" t="n"/>
+      <c r="A46" s="10" t="n"/>
+      <c r="B46" s="10" t="n"/>
+      <c r="C46" s="10" t="n"/>
+      <c r="D46" s="10" t="n"/>
+      <c r="E46" s="10" t="n"/>
+      <c r="F46" s="10" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="6" t="n"/>
-      <c r="B47" s="6" t="n"/>
-      <c r="C47" s="6" t="n"/>
-      <c r="D47" s="6" t="n"/>
-      <c r="E47" s="6" t="n"/>
-      <c r="F47" s="6" t="n"/>
+      <c r="A47" s="10" t="n"/>
+      <c r="B47" s="10" t="n"/>
+      <c r="C47" s="10" t="n"/>
+      <c r="D47" s="10" t="n"/>
+      <c r="E47" s="10" t="n"/>
+      <c r="F47" s="10" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="6" t="n"/>
-      <c r="B48" s="6" t="n"/>
-      <c r="C48" s="6" t="n"/>
-      <c r="D48" s="6" t="n"/>
-      <c r="E48" s="6" t="n"/>
-      <c r="F48" s="6" t="n"/>
+      <c r="A48" s="10" t="n"/>
+      <c r="B48" s="10" t="n"/>
+      <c r="C48" s="10" t="n"/>
+      <c r="D48" s="10" t="n"/>
+      <c r="E48" s="10" t="n"/>
+      <c r="F48" s="10" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="6" t="n"/>
-      <c r="B49" s="6" t="n"/>
-      <c r="C49" s="6" t="n"/>
-      <c r="D49" s="6" t="n"/>
-      <c r="E49" s="6" t="n"/>
-      <c r="F49" s="6" t="n"/>
+      <c r="A49" s="10" t="n"/>
+      <c r="B49" s="10" t="n"/>
+      <c r="C49" s="10" t="n"/>
+      <c r="D49" s="10" t="n"/>
+      <c r="E49" s="10" t="n"/>
+      <c r="F49" s="10" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="6" t="n"/>
-      <c r="B50" s="6" t="n"/>
-      <c r="C50" s="6" t="n"/>
-      <c r="D50" s="6" t="n"/>
-      <c r="E50" s="6" t="n"/>
-      <c r="F50" s="6" t="n"/>
+      <c r="A50" s="10" t="n"/>
+      <c r="B50" s="10" t="n"/>
+      <c r="C50" s="10" t="n"/>
+      <c r="D50" s="10" t="n"/>
+      <c r="E50" s="10" t="n"/>
+      <c r="F50" s="10" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" s="6" t="n"/>
-      <c r="B51" s="6" t="n"/>
-      <c r="C51" s="6" t="n"/>
-      <c r="D51" s="6" t="n"/>
-      <c r="E51" s="6" t="n"/>
-      <c r="F51" s="6" t="n"/>
+      <c r="A51" s="10" t="n"/>
+      <c r="B51" s="10" t="n"/>
+      <c r="C51" s="10" t="n"/>
+      <c r="D51" s="10" t="n"/>
+      <c r="E51" s="10" t="n"/>
+      <c r="F51" s="10" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="6" t="n"/>
-      <c r="B52" s="6" t="n"/>
-      <c r="C52" s="6" t="n"/>
-      <c r="D52" s="6" t="n"/>
-      <c r="E52" s="6" t="n"/>
-      <c r="F52" s="6" t="n"/>
+      <c r="A52" s="10" t="n"/>
+      <c r="B52" s="10" t="n"/>
+      <c r="C52" s="10" t="n"/>
+      <c r="D52" s="10" t="n"/>
+      <c r="E52" s="10" t="n"/>
+      <c r="F52" s="10" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="6" t="n"/>
-      <c r="B53" s="6" t="n"/>
-      <c r="C53" s="6" t="n"/>
-      <c r="D53" s="6" t="n"/>
-      <c r="E53" s="6" t="n"/>
-      <c r="F53" s="6" t="n"/>
+      <c r="A53" s="10" t="n"/>
+      <c r="B53" s="10" t="n"/>
+      <c r="C53" s="10" t="n"/>
+      <c r="D53" s="10" t="n"/>
+      <c r="E53" s="10" t="n"/>
+      <c r="F53" s="10" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="6" t="n"/>
-      <c r="B54" s="6" t="n"/>
-      <c r="C54" s="6" t="n"/>
-      <c r="D54" s="6" t="n"/>
-      <c r="E54" s="6" t="n"/>
-      <c r="F54" s="6" t="n"/>
+      <c r="A54" s="10" t="n"/>
+      <c r="B54" s="10" t="n"/>
+      <c r="C54" s="10" t="n"/>
+      <c r="D54" s="10" t="n"/>
+      <c r="E54" s="10" t="n"/>
+      <c r="F54" s="10" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" s="6" t="n"/>
-      <c r="B55" s="6" t="n"/>
-      <c r="C55" s="6" t="n"/>
-      <c r="D55" s="6" t="n"/>
-      <c r="E55" s="6" t="n"/>
-      <c r="F55" s="6" t="n"/>
+      <c r="A55" s="10" t="n"/>
+      <c r="B55" s="10" t="n"/>
+      <c r="C55" s="10" t="n"/>
+      <c r="D55" s="10" t="n"/>
+      <c r="E55" s="10" t="n"/>
+      <c r="F55" s="10" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="6" t="n"/>
-      <c r="B56" s="6" t="n"/>
-      <c r="C56" s="6" t="n"/>
-      <c r="D56" s="6" t="n"/>
-      <c r="E56" s="6" t="n"/>
-      <c r="F56" s="6" t="n"/>
+      <c r="A56" s="10" t="n"/>
+      <c r="B56" s="10" t="n"/>
+      <c r="C56" s="10" t="n"/>
+      <c r="D56" s="10" t="n"/>
+      <c r="E56" s="10" t="n"/>
+      <c r="F56" s="10" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="6" t="n"/>
-      <c r="B57" s="6" t="n"/>
-      <c r="C57" s="6" t="n"/>
-      <c r="D57" s="6" t="n"/>
-      <c r="E57" s="6" t="n"/>
-      <c r="F57" s="6" t="n"/>
+      <c r="A57" s="10" t="n"/>
+      <c r="B57" s="10" t="n"/>
+      <c r="C57" s="10" t="n"/>
+      <c r="D57" s="10" t="n"/>
+      <c r="E57" s="10" t="n"/>
+      <c r="F57" s="10" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="6" t="n"/>
-      <c r="B58" s="6" t="n"/>
-      <c r="C58" s="6" t="n"/>
-      <c r="D58" s="6" t="n"/>
-      <c r="E58" s="6" t="n"/>
-      <c r="F58" s="6" t="n"/>
+      <c r="A58" s="10" t="n"/>
+      <c r="B58" s="10" t="n"/>
+      <c r="C58" s="10" t="n"/>
+      <c r="D58" s="10" t="n"/>
+      <c r="E58" s="10" t="n"/>
+      <c r="F58" s="10" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" s="6" t="n"/>
-      <c r="B59" s="6" t="n"/>
-      <c r="C59" s="6" t="n"/>
-      <c r="D59" s="6" t="n"/>
-      <c r="E59" s="6" t="n"/>
-      <c r="F59" s="6" t="n"/>
+      <c r="A59" s="10" t="n"/>
+      <c r="B59" s="10" t="n"/>
+      <c r="C59" s="10" t="n"/>
+      <c r="D59" s="10" t="n"/>
+      <c r="E59" s="10" t="n"/>
+      <c r="F59" s="10" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" s="6" t="n"/>
-      <c r="B60" s="6" t="n"/>
-      <c r="C60" s="6" t="n"/>
-      <c r="D60" s="6" t="n"/>
-      <c r="E60" s="6" t="n"/>
-      <c r="F60" s="6" t="n"/>
+      <c r="A60" s="10" t="n"/>
+      <c r="B60" s="10" t="n"/>
+      <c r="C60" s="10" t="n"/>
+      <c r="D60" s="10" t="n"/>
+      <c r="E60" s="10" t="n"/>
+      <c r="F60" s="10" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" s="6" t="n"/>
-      <c r="B61" s="6" t="n"/>
-      <c r="C61" s="6" t="n"/>
-      <c r="D61" s="6" t="n"/>
-      <c r="E61" s="6" t="n"/>
-      <c r="F61" s="6" t="n"/>
+      <c r="A61" s="10" t="n"/>
+      <c r="B61" s="10" t="n"/>
+      <c r="C61" s="10" t="n"/>
+      <c r="D61" s="10" t="n"/>
+      <c r="E61" s="10" t="n"/>
+      <c r="F61" s="10" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" s="6" t="n"/>
-      <c r="B62" s="6" t="n"/>
-      <c r="C62" s="6" t="n"/>
-      <c r="D62" s="6" t="n"/>
-      <c r="E62" s="6" t="n"/>
-      <c r="F62" s="6" t="n"/>
+      <c r="A62" s="10" t="n"/>
+      <c r="B62" s="10" t="n"/>
+      <c r="C62" s="10" t="n"/>
+      <c r="D62" s="10" t="n"/>
+      <c r="E62" s="10" t="n"/>
+      <c r="F62" s="10" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" s="6" t="n"/>
-      <c r="B63" s="6" t="n"/>
-      <c r="C63" s="6" t="n"/>
-      <c r="D63" s="6" t="n"/>
-      <c r="E63" s="6" t="n"/>
-      <c r="F63" s="6" t="n"/>
+      <c r="A63" s="10" t="n"/>
+      <c r="B63" s="10" t="n"/>
+      <c r="C63" s="10" t="n"/>
+      <c r="D63" s="10" t="n"/>
+      <c r="E63" s="10" t="n"/>
+      <c r="F63" s="10" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" s="6" t="n"/>
-      <c r="B64" s="6" t="n"/>
-      <c r="C64" s="6" t="n"/>
-      <c r="D64" s="6" t="n"/>
-      <c r="E64" s="6" t="n"/>
-      <c r="F64" s="6" t="n"/>
+      <c r="A64" s="10" t="n"/>
+      <c r="B64" s="10" t="n"/>
+      <c r="C64" s="10" t="n"/>
+      <c r="D64" s="10" t="n"/>
+      <c r="E64" s="10" t="n"/>
+      <c r="F64" s="10" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" s="6" t="n"/>
-      <c r="B65" s="6" t="n"/>
-      <c r="C65" s="6" t="n"/>
-      <c r="D65" s="6" t="n"/>
-      <c r="E65" s="6" t="n"/>
-      <c r="F65" s="6" t="n"/>
+      <c r="A65" s="10" t="n"/>
+      <c r="B65" s="10" t="n"/>
+      <c r="C65" s="10" t="n"/>
+      <c r="D65" s="10" t="n"/>
+      <c r="E65" s="10" t="n"/>
+      <c r="F65" s="10" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" s="6" t="n"/>
-      <c r="B66" s="6" t="n"/>
-      <c r="C66" s="6" t="n"/>
-      <c r="D66" s="6" t="n"/>
-      <c r="E66" s="6" t="n"/>
-      <c r="F66" s="6" t="n"/>
+      <c r="A66" s="10" t="n"/>
+      <c r="B66" s="10" t="n"/>
+      <c r="C66" s="10" t="n"/>
+      <c r="D66" s="10" t="n"/>
+      <c r="E66" s="10" t="n"/>
+      <c r="F66" s="10" t="n"/>
     </row>
     <row r="67">
-      <c r="A67" s="6" t="n"/>
-      <c r="B67" s="6" t="n"/>
-      <c r="C67" s="6" t="n"/>
-      <c r="D67" s="6" t="n"/>
-      <c r="E67" s="6" t="n"/>
-      <c r="F67" s="6" t="n"/>
+      <c r="A67" s="10" t="n"/>
+      <c r="B67" s="10" t="n"/>
+      <c r="C67" s="10" t="n"/>
+      <c r="D67" s="10" t="n"/>
+      <c r="E67" s="10" t="n"/>
+      <c r="F67" s="10" t="n"/>
     </row>
     <row r="68">
-      <c r="A68" s="6" t="n"/>
-      <c r="B68" s="6" t="n"/>
-      <c r="C68" s="6" t="n"/>
-      <c r="D68" s="6" t="n"/>
-      <c r="E68" s="6" t="n"/>
-      <c r="F68" s="6" t="n"/>
+      <c r="A68" s="10" t="n"/>
+      <c r="B68" s="10" t="n"/>
+      <c r="C68" s="10" t="n"/>
+      <c r="D68" s="10" t="n"/>
+      <c r="E68" s="10" t="n"/>
+      <c r="F68" s="10" t="n"/>
     </row>
     <row r="69">
-      <c r="A69" s="6" t="n"/>
-      <c r="B69" s="6" t="n"/>
-      <c r="C69" s="6" t="n"/>
-      <c r="D69" s="6" t="n"/>
-      <c r="E69" s="6" t="n"/>
-      <c r="F69" s="6" t="n"/>
+      <c r="A69" s="10" t="n"/>
+      <c r="B69" s="10" t="n"/>
+      <c r="C69" s="10" t="n"/>
+      <c r="D69" s="10" t="n"/>
+      <c r="E69" s="10" t="n"/>
+      <c r="F69" s="10" t="n"/>
     </row>
     <row r="70">
-      <c r="A70" s="6" t="n"/>
-      <c r="B70" s="6" t="n"/>
-      <c r="C70" s="6" t="n"/>
-      <c r="D70" s="6" t="n"/>
-      <c r="E70" s="6" t="n"/>
-      <c r="F70" s="6" t="n"/>
+      <c r="A70" s="10" t="n"/>
+      <c r="B70" s="10" t="n"/>
+      <c r="C70" s="10" t="n"/>
+      <c r="D70" s="10" t="n"/>
+      <c r="E70" s="10" t="n"/>
+      <c r="F70" s="10" t="n"/>
     </row>
     <row r="71">
-      <c r="A71" s="6" t="n"/>
-      <c r="B71" s="6" t="n"/>
-      <c r="C71" s="6" t="n"/>
-      <c r="D71" s="6" t="n"/>
-      <c r="E71" s="6" t="n"/>
-      <c r="F71" s="6" t="n"/>
+      <c r="A71" s="10" t="n"/>
+      <c r="B71" s="10" t="n"/>
+      <c r="C71" s="10" t="n"/>
+      <c r="D71" s="10" t="n"/>
+      <c r="E71" s="10" t="n"/>
+      <c r="F71" s="10" t="n"/>
     </row>
     <row r="72">
-      <c r="A72" s="6" t="n"/>
-      <c r="B72" s="6" t="n"/>
-      <c r="C72" s="6" t="n"/>
-      <c r="D72" s="6" t="n"/>
-      <c r="E72" s="6" t="n"/>
-      <c r="F72" s="6" t="n"/>
+      <c r="A72" s="10" t="n"/>
+      <c r="B72" s="10" t="n"/>
+      <c r="C72" s="10" t="n"/>
+      <c r="D72" s="10" t="n"/>
+      <c r="E72" s="10" t="n"/>
+      <c r="F72" s="10" t="n"/>
     </row>
     <row r="73">
-      <c r="A73" s="6" t="n"/>
-      <c r="B73" s="6" t="n"/>
-      <c r="C73" s="6" t="n"/>
-      <c r="D73" s="6" t="n"/>
-      <c r="E73" s="6" t="n"/>
-      <c r="F73" s="6" t="n"/>
+      <c r="A73" s="10" t="n"/>
+      <c r="B73" s="10" t="n"/>
+      <c r="C73" s="10" t="n"/>
+      <c r="D73" s="10" t="n"/>
+      <c r="E73" s="10" t="n"/>
+      <c r="F73" s="10" t="n"/>
     </row>
     <row r="74">
-      <c r="A74" s="6" t="n"/>
-      <c r="B74" s="6" t="n"/>
-      <c r="C74" s="6" t="n"/>
-      <c r="D74" s="6" t="n"/>
-      <c r="E74" s="6" t="n"/>
-      <c r="F74" s="6" t="n"/>
+      <c r="A74" s="10" t="n"/>
+      <c r="B74" s="10" t="n"/>
+      <c r="C74" s="10" t="n"/>
+      <c r="D74" s="10" t="n"/>
+      <c r="E74" s="10" t="n"/>
+      <c r="F74" s="10" t="n"/>
     </row>
     <row r="75">
-      <c r="A75" s="6" t="n"/>
-      <c r="B75" s="6" t="n"/>
-      <c r="C75" s="6" t="n"/>
-      <c r="D75" s="6" t="n"/>
-      <c r="E75" s="6" t="n"/>
-      <c r="F75" s="6" t="n"/>
+      <c r="A75" s="10" t="n"/>
+      <c r="B75" s="10" t="n"/>
+      <c r="C75" s="10" t="n"/>
+      <c r="D75" s="10" t="n"/>
+      <c r="E75" s="10" t="n"/>
+      <c r="F75" s="10" t="n"/>
     </row>
     <row r="76">
-      <c r="A76" s="6" t="n"/>
-      <c r="B76" s="6" t="n"/>
-      <c r="C76" s="6" t="n"/>
-      <c r="D76" s="6" t="n"/>
-      <c r="E76" s="6" t="n"/>
-      <c r="F76" s="6" t="n"/>
+      <c r="A76" s="10" t="n"/>
+      <c r="B76" s="10" t="n"/>
+      <c r="C76" s="10" t="n"/>
+      <c r="D76" s="10" t="n"/>
+      <c r="E76" s="10" t="n"/>
+      <c r="F76" s="10" t="n"/>
     </row>
     <row r="77">
-      <c r="A77" s="6" t="n"/>
-      <c r="B77" s="6" t="n"/>
-      <c r="C77" s="6" t="n"/>
-      <c r="D77" s="6" t="n"/>
-      <c r="E77" s="6" t="n"/>
-      <c r="F77" s="6" t="n"/>
+      <c r="A77" s="10" t="n"/>
+      <c r="B77" s="10" t="n"/>
+      <c r="C77" s="10" t="n"/>
+      <c r="D77" s="10" t="n"/>
+      <c r="E77" s="10" t="n"/>
+      <c r="F77" s="10" t="n"/>
     </row>
     <row r="78">
-      <c r="A78" s="6" t="n"/>
-      <c r="B78" s="6" t="n"/>
-      <c r="C78" s="6" t="n"/>
-      <c r="D78" s="6" t="n"/>
-      <c r="E78" s="6" t="n"/>
-      <c r="F78" s="6" t="n"/>
+      <c r="A78" s="10" t="n"/>
+      <c r="B78" s="10" t="n"/>
+      <c r="C78" s="10" t="n"/>
+      <c r="D78" s="10" t="n"/>
+      <c r="E78" s="10" t="n"/>
+      <c r="F78" s="10" t="n"/>
     </row>
     <row r="79">
-      <c r="A79" s="6" t="n"/>
-      <c r="B79" s="6" t="n"/>
-      <c r="C79" s="6" t="n"/>
-      <c r="D79" s="6" t="n"/>
-      <c r="E79" s="6" t="n"/>
-      <c r="F79" s="6" t="n"/>
+      <c r="A79" s="10" t="n"/>
+      <c r="B79" s="10" t="n"/>
+      <c r="C79" s="10" t="n"/>
+      <c r="D79" s="10" t="n"/>
+      <c r="E79" s="10" t="n"/>
+      <c r="F79" s="10" t="n"/>
     </row>
     <row r="80">
-      <c r="A80" s="6" t="n"/>
-      <c r="B80" s="6" t="n"/>
-      <c r="C80" s="6" t="n"/>
-      <c r="D80" s="6" t="n"/>
-      <c r="E80" s="6" t="n"/>
-      <c r="F80" s="6" t="n"/>
+      <c r="A80" s="10" t="n"/>
+      <c r="B80" s="10" t="n"/>
+      <c r="C80" s="10" t="n"/>
+      <c r="D80" s="10" t="n"/>
+      <c r="E80" s="10" t="n"/>
+      <c r="F80" s="10" t="n"/>
     </row>
     <row r="81">
-      <c r="A81" s="6" t="n"/>
-      <c r="B81" s="6" t="n"/>
-      <c r="C81" s="6" t="n"/>
-      <c r="D81" s="6" t="n"/>
-      <c r="E81" s="6" t="n"/>
-      <c r="F81" s="6" t="n"/>
+      <c r="A81" s="10" t="n"/>
+      <c r="B81" s="10" t="n"/>
+      <c r="C81" s="10" t="n"/>
+      <c r="D81" s="10" t="n"/>
+      <c r="E81" s="10" t="n"/>
+      <c r="F81" s="10" t="n"/>
     </row>
     <row r="82">
-      <c r="A82" s="6" t="n"/>
-      <c r="B82" s="6" t="n"/>
-      <c r="C82" s="6" t="n"/>
-      <c r="D82" s="6" t="n"/>
-      <c r="E82" s="6" t="n"/>
-      <c r="F82" s="6" t="n"/>
+      <c r="A82" s="10" t="n"/>
+      <c r="B82" s="10" t="n"/>
+      <c r="C82" s="10" t="n"/>
+      <c r="D82" s="10" t="n"/>
+      <c r="E82" s="10" t="n"/>
+      <c r="F82" s="10" t="n"/>
     </row>
     <row r="83">
-      <c r="A83" s="6" t="n"/>
-      <c r="B83" s="6" t="n"/>
-      <c r="C83" s="6" t="n"/>
-      <c r="D83" s="6" t="n"/>
-      <c r="E83" s="6" t="n"/>
-      <c r="F83" s="6" t="n"/>
+      <c r="A83" s="10" t="n"/>
+      <c r="B83" s="10" t="n"/>
+      <c r="C83" s="10" t="n"/>
+      <c r="D83" s="10" t="n"/>
+      <c r="E83" s="10" t="n"/>
+      <c r="F83" s="10" t="n"/>
     </row>
     <row r="84">
-      <c r="A84" s="6" t="n"/>
-      <c r="B84" s="6" t="n"/>
-      <c r="C84" s="6" t="n"/>
-      <c r="D84" s="6" t="n"/>
-      <c r="E84" s="6" t="n"/>
-      <c r="F84" s="6" t="n"/>
+      <c r="A84" s="10" t="n"/>
+      <c r="B84" s="10" t="n"/>
+      <c r="C84" s="10" t="n"/>
+      <c r="D84" s="10" t="n"/>
+      <c r="E84" s="10" t="n"/>
+      <c r="F84" s="10" t="n"/>
     </row>
     <row r="85">
-      <c r="A85" s="6" t="n"/>
-      <c r="B85" s="6" t="n"/>
-      <c r="C85" s="6" t="n"/>
-      <c r="D85" s="6" t="n"/>
-      <c r="E85" s="6" t="n"/>
-      <c r="F85" s="6" t="n"/>
+      <c r="A85" s="10" t="n"/>
+      <c r="B85" s="10" t="n"/>
+      <c r="C85" s="10" t="n"/>
+      <c r="D85" s="10" t="n"/>
+      <c r="E85" s="10" t="n"/>
+      <c r="F85" s="10" t="n"/>
     </row>
     <row r="86">
-      <c r="A86" s="6" t="n"/>
-      <c r="B86" s="6" t="n"/>
-      <c r="C86" s="6" t="n"/>
-      <c r="D86" s="6" t="n"/>
-      <c r="E86" s="6" t="n"/>
-      <c r="F86" s="6" t="n"/>
+      <c r="A86" s="10" t="n"/>
+      <c r="B86" s="10" t="n"/>
+      <c r="C86" s="10" t="n"/>
+      <c r="D86" s="10" t="n"/>
+      <c r="E86" s="10" t="n"/>
+      <c r="F86" s="10" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>

<commit_message>
table update (width, font style, etc)
added the note at the bottom
</commit_message>
<xml_diff>
--- a/static/Honors.xlsx
+++ b/static/Honors.xlsx
@@ -32,7 +32,6 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <strike val="0"/>
       <sz val="9"/>
     </font>
   </fonts>
@@ -164,12 +163,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -556,7 +555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,12 +563,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="5" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="32" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="9" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="9" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="12" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="25" bestFit="1" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -694,7 +693,7 @@
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>NO.</t>
         </is>
       </c>
       <c r="B19" s="6" t="inlineStr">
@@ -1263,8 +1262,22 @@
       <c r="E86" s="10" t="n"/>
       <c r="F86" s="10" t="n"/>
     </row>
+    <row r="88">
+      <c r="A88" s="5" t="inlineStr">
+        <is>
+          <t>Note: Subject for verification/recommendation/approval by the University Evaluation/Review Committee</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="5" t="inlineStr">
+        <is>
+          <t>on Honor Graduates</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
@@ -1276,8 +1289,10 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A88:F88"/>
+    <mergeCell ref="A89:F89"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.5" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperHeight="13in" paperWidth="8.5in"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fixed sentence break, indention
</commit_message>
<xml_diff>
--- a/static/Honors.xlsx
+++ b/static/Honors.xlsx
@@ -146,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -161,7 +161,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="1"/>
+      <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -171,6 +171,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="6"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -622,7 +628,7 @@
     <row r="5">
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>July 08, 2021</t>
+          <t>July 09, 2021</t>
         </is>
       </c>
     </row>
@@ -679,14 +685,14 @@
     <row r="16">
       <c r="A16" s="5" t="inlineStr">
         <is>
-          <t>Herewith are the Official List of Candidates for Graduation with Honors under the different degree programs</t>
+          <t>Herewith are the Official List of Candidates for Graduation with Honors under the different</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> of the College of Social Sciences and Philosophy  for the 2nd Semester, 2019-2020 </t>
+          <t>degree programs of the College of Social Sciences and Philosophy  for the 2nd Semester, 2019-2020.</t>
         </is>
       </c>
     </row>
@@ -1263,16 +1269,16 @@
       <c r="F86" s="10" t="n"/>
     </row>
     <row r="88">
-      <c r="A88" s="5" t="inlineStr">
-        <is>
-          <t>Note: Subject for verification/recommendation/approval by the University Evaluation/Review Committee</t>
+      <c r="A88" s="11" t="inlineStr">
+        <is>
+          <t>Note: Subject for verification/recommendation/approval by the University Evaluation/Review</t>
         </is>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="5" t="inlineStr">
-        <is>
-          <t>on Honor Graduates</t>
+      <c r="A89" s="12" t="inlineStr">
+        <is>
+          <t>Committee on Honor Graduates</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed for loop for cell style
</commit_message>
<xml_diff>
--- a/static/Honors.xlsx
+++ b/static/Honors.xlsx
@@ -167,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -193,6 +193,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -204,6 +207,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="2"/>
     </xf>
@@ -212,9 +218,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -802,921 +805,2175 @@
       <c r="H20" s="9" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="10" t="n"/>
-      <c r="B21" s="10" t="n"/>
-      <c r="C21" s="10" t="n"/>
-      <c r="D21" s="10" t="n"/>
-      <c r="E21" s="10" t="n"/>
-      <c r="F21" s="10" t="n"/>
-      <c r="G21" s="10" t="n"/>
-      <c r="H21" s="10" t="n"/>
+      <c r="A21" s="10" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="B21" s="10" t="inlineStr">
+        <is>
+          <t>Bethany Jayne Ibañez Carizo</t>
+        </is>
+      </c>
+      <c r="C21" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D21" s="10" t="inlineStr"/>
+      <c r="E21" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F21" s="10" t="n">
+        <v>330.9</v>
+      </c>
+      <c r="G21" s="11" t="n">
+        <v>1.4141</v>
+      </c>
+      <c r="H21" s="10" t="inlineStr">
+        <is>
+          <t>Magna Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="10" t="n"/>
-      <c r="B22" s="10" t="n"/>
-      <c r="C22" s="10" t="n"/>
-      <c r="D22" s="10" t="n"/>
-      <c r="E22" s="10" t="n"/>
-      <c r="F22" s="10" t="n"/>
-      <c r="G22" s="10" t="n"/>
-      <c r="H22" s="10" t="n"/>
+      <c r="A22" s="10" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="B22" s="10" t="inlineStr">
+        <is>
+          <t>Arvin Joehn Misolas Pispis</t>
+        </is>
+      </c>
+      <c r="C22" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D22" s="10" t="inlineStr"/>
+      <c r="E22" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F22" s="10" t="n">
+        <v>339.5</v>
+      </c>
+      <c r="G22" s="11" t="n">
+        <v>1.4509</v>
+      </c>
+      <c r="H22" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="10" t="n"/>
-      <c r="B23" s="10" t="n"/>
-      <c r="C23" s="10" t="n"/>
-      <c r="D23" s="10" t="n"/>
-      <c r="E23" s="10" t="n"/>
-      <c r="F23" s="10" t="n"/>
-      <c r="G23" s="10" t="n"/>
-      <c r="H23" s="10" t="n"/>
+      <c r="A23" s="10" t="inlineStr">
+        <is>
+          <t>3.</t>
+        </is>
+      </c>
+      <c r="B23" s="10" t="inlineStr">
+        <is>
+          <t>Emmanuel Zaragosa Jerusalem</t>
+        </is>
+      </c>
+      <c r="C23" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D23" s="10" t="inlineStr"/>
+      <c r="E23" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F23" s="10" t="n">
+        <v>350.1</v>
+      </c>
+      <c r="G23" s="11" t="n">
+        <v>1.4962</v>
+      </c>
+      <c r="H23" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="10" t="n"/>
-      <c r="B24" s="10" t="n"/>
-      <c r="C24" s="10" t="n"/>
-      <c r="D24" s="10" t="n"/>
-      <c r="E24" s="10" t="n"/>
-      <c r="F24" s="10" t="n"/>
-      <c r="G24" s="10" t="n"/>
-      <c r="H24" s="10" t="n"/>
+      <c r="A24" s="10" t="inlineStr">
+        <is>
+          <t>4.</t>
+        </is>
+      </c>
+      <c r="B24" s="10" t="inlineStr">
+        <is>
+          <t>John Kenneth Rodriguez Rempillo</t>
+        </is>
+      </c>
+      <c r="C24" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D24" s="10" t="inlineStr"/>
+      <c r="E24" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F24" s="10" t="n">
+        <v>352.1</v>
+      </c>
+      <c r="G24" s="11" t="n">
+        <v>1.5047</v>
+      </c>
+      <c r="H24" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="10" t="n"/>
-      <c r="B25" s="10" t="n"/>
-      <c r="C25" s="10" t="n"/>
-      <c r="D25" s="10" t="n"/>
-      <c r="E25" s="10" t="n"/>
-      <c r="F25" s="10" t="n"/>
-      <c r="G25" s="10" t="n"/>
-      <c r="H25" s="10" t="n"/>
+      <c r="A25" s="10" t="inlineStr">
+        <is>
+          <t>5.</t>
+        </is>
+      </c>
+      <c r="B25" s="10" t="inlineStr">
+        <is>
+          <t>May Ann Maralit Wong</t>
+        </is>
+      </c>
+      <c r="C25" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D25" s="10" t="inlineStr"/>
+      <c r="E25" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F25" s="10" t="n">
+        <v>355.1</v>
+      </c>
+      <c r="G25" s="11" t="n">
+        <v>1.5175</v>
+      </c>
+      <c r="H25" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="10" t="n"/>
-      <c r="B26" s="10" t="n"/>
-      <c r="C26" s="10" t="n"/>
-      <c r="D26" s="10" t="n"/>
-      <c r="E26" s="10" t="n"/>
-      <c r="F26" s="10" t="n"/>
-      <c r="G26" s="10" t="n"/>
-      <c r="H26" s="10" t="n"/>
+      <c r="A26" s="10" t="inlineStr">
+        <is>
+          <t>6.</t>
+        </is>
+      </c>
+      <c r="B26" s="10" t="inlineStr">
+        <is>
+          <t>Christian Malagueño Serrano</t>
+        </is>
+      </c>
+      <c r="C26" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D26" s="10" t="inlineStr"/>
+      <c r="E26" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F26" s="10" t="n">
+        <v>355.3</v>
+      </c>
+      <c r="G26" s="11" t="n">
+        <v>1.5184</v>
+      </c>
+      <c r="H26" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="10" t="n"/>
-      <c r="B27" s="10" t="n"/>
-      <c r="C27" s="10" t="n"/>
-      <c r="D27" s="10" t="n"/>
-      <c r="E27" s="10" t="n"/>
-      <c r="F27" s="10" t="n"/>
-      <c r="G27" s="10" t="n"/>
-      <c r="H27" s="10" t="n"/>
+      <c r="A27" s="10" t="inlineStr">
+        <is>
+          <t>7.</t>
+        </is>
+      </c>
+      <c r="B27" s="10" t="inlineStr">
+        <is>
+          <t>Mark Anthony Sanchez Nobleza</t>
+        </is>
+      </c>
+      <c r="C27" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D27" s="10" t="inlineStr"/>
+      <c r="E27" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F27" s="10" t="n">
+        <v>359.6</v>
+      </c>
+      <c r="G27" s="11" t="n">
+        <v>1.5368</v>
+      </c>
+      <c r="H27" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="10" t="n"/>
-      <c r="B28" s="10" t="n"/>
-      <c r="C28" s="10" t="n"/>
-      <c r="D28" s="10" t="n"/>
-      <c r="E28" s="10" t="n"/>
-      <c r="F28" s="10" t="n"/>
-      <c r="G28" s="10" t="n"/>
-      <c r="H28" s="10" t="n"/>
+      <c r="A28" s="10" t="inlineStr">
+        <is>
+          <t>8.</t>
+        </is>
+      </c>
+      <c r="B28" s="10" t="inlineStr">
+        <is>
+          <t>Mary Dimple Navera Labalan</t>
+        </is>
+      </c>
+      <c r="C28" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D28" s="10" t="inlineStr"/>
+      <c r="E28" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F28" s="10" t="n">
+        <v>362.2</v>
+      </c>
+      <c r="G28" s="11" t="n">
+        <v>1.5479</v>
+      </c>
+      <c r="H28" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="10" t="n"/>
-      <c r="B29" s="10" t="n"/>
-      <c r="C29" s="10" t="n"/>
-      <c r="D29" s="10" t="n"/>
-      <c r="E29" s="10" t="n"/>
-      <c r="F29" s="10" t="n"/>
-      <c r="G29" s="10" t="n"/>
-      <c r="H29" s="10" t="n"/>
+      <c r="A29" s="10" t="inlineStr">
+        <is>
+          <t>9.</t>
+        </is>
+      </c>
+      <c r="B29" s="10" t="inlineStr">
+        <is>
+          <t>Julius Ian Buatin Guardian</t>
+        </is>
+      </c>
+      <c r="C29" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D29" s="10" t="inlineStr"/>
+      <c r="E29" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F29" s="10" t="n">
+        <v>366.8</v>
+      </c>
+      <c r="G29" s="11" t="n">
+        <v>1.5675</v>
+      </c>
+      <c r="H29" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="10" t="n"/>
-      <c r="B30" s="10" t="n"/>
-      <c r="C30" s="10" t="n"/>
-      <c r="D30" s="10" t="n"/>
-      <c r="E30" s="10" t="n"/>
-      <c r="F30" s="10" t="n"/>
-      <c r="G30" s="10" t="n"/>
-      <c r="H30" s="10" t="n"/>
+      <c r="A30" s="10" t="inlineStr">
+        <is>
+          <t>10.</t>
+        </is>
+      </c>
+      <c r="B30" s="10" t="inlineStr">
+        <is>
+          <t>Janne Nicole Priagola Garcia</t>
+        </is>
+      </c>
+      <c r="C30" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D30" s="10" t="inlineStr"/>
+      <c r="E30" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F30" s="10" t="n">
+        <v>378.4</v>
+      </c>
+      <c r="G30" s="11" t="n">
+        <v>1.6171</v>
+      </c>
+      <c r="H30" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="10" t="n"/>
-      <c r="B31" s="10" t="n"/>
-      <c r="C31" s="10" t="n"/>
-      <c r="D31" s="10" t="n"/>
-      <c r="E31" s="10" t="n"/>
-      <c r="F31" s="10" t="n"/>
-      <c r="G31" s="10" t="n"/>
-      <c r="H31" s="10" t="n"/>
+      <c r="A31" s="10" t="inlineStr">
+        <is>
+          <t>11.</t>
+        </is>
+      </c>
+      <c r="B31" s="10" t="inlineStr">
+        <is>
+          <t>Michael Salvador Osi Tanay</t>
+        </is>
+      </c>
+      <c r="C31" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D31" s="10" t="inlineStr"/>
+      <c r="E31" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F31" s="10" t="n">
+        <v>378.4</v>
+      </c>
+      <c r="G31" s="11" t="n">
+        <v>1.6171</v>
+      </c>
+      <c r="H31" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="10" t="n"/>
-      <c r="B32" s="10" t="n"/>
-      <c r="C32" s="10" t="n"/>
-      <c r="D32" s="10" t="n"/>
-      <c r="E32" s="10" t="n"/>
-      <c r="F32" s="10" t="n"/>
-      <c r="G32" s="10" t="n"/>
-      <c r="H32" s="10" t="n"/>
+      <c r="A32" s="10" t="inlineStr">
+        <is>
+          <t>12.</t>
+        </is>
+      </c>
+      <c r="B32" s="10" t="inlineStr">
+        <is>
+          <t>Sheila Bataller Basilla</t>
+        </is>
+      </c>
+      <c r="C32" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D32" s="10" t="inlineStr"/>
+      <c r="E32" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F32" s="10" t="n">
+        <v>378.5</v>
+      </c>
+      <c r="G32" s="11" t="n">
+        <v>1.6175</v>
+      </c>
+      <c r="H32" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="10" t="n"/>
-      <c r="B33" s="10" t="n"/>
-      <c r="C33" s="10" t="n"/>
-      <c r="D33" s="10" t="n"/>
-      <c r="E33" s="10" t="n"/>
-      <c r="F33" s="10" t="n"/>
-      <c r="G33" s="10" t="n"/>
-      <c r="H33" s="10" t="n"/>
+      <c r="A33" s="10" t="inlineStr">
+        <is>
+          <t>13.</t>
+        </is>
+      </c>
+      <c r="B33" s="10" t="inlineStr">
+        <is>
+          <t>Viviene Mae Resare Apuli</t>
+        </is>
+      </c>
+      <c r="C33" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D33" s="10" t="inlineStr"/>
+      <c r="E33" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F33" s="10" t="n">
+        <v>378.6</v>
+      </c>
+      <c r="G33" s="11" t="n">
+        <v>1.6179</v>
+      </c>
+      <c r="H33" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="10" t="n"/>
-      <c r="B34" s="10" t="n"/>
-      <c r="C34" s="10" t="n"/>
-      <c r="D34" s="10" t="n"/>
-      <c r="E34" s="10" t="n"/>
-      <c r="F34" s="10" t="n"/>
-      <c r="G34" s="10" t="n"/>
-      <c r="H34" s="10" t="n"/>
+      <c r="A34" s="10" t="inlineStr">
+        <is>
+          <t>14.</t>
+        </is>
+      </c>
+      <c r="B34" s="10" t="inlineStr">
+        <is>
+          <t>Nicole Casulla Abadesa</t>
+        </is>
+      </c>
+      <c r="C34" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D34" s="10" t="inlineStr"/>
+      <c r="E34" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F34" s="10" t="n">
+        <v>378.8</v>
+      </c>
+      <c r="G34" s="11" t="n">
+        <v>1.6188</v>
+      </c>
+      <c r="H34" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="10" t="n"/>
-      <c r="B35" s="10" t="n"/>
-      <c r="C35" s="10" t="n"/>
-      <c r="D35" s="10" t="n"/>
-      <c r="E35" s="10" t="n"/>
-      <c r="F35" s="10" t="n"/>
-      <c r="G35" s="10" t="n"/>
-      <c r="H35" s="10" t="n"/>
+      <c r="A35" s="10" t="inlineStr">
+        <is>
+          <t>15.</t>
+        </is>
+      </c>
+      <c r="B35" s="10" t="inlineStr">
+        <is>
+          <t>Carlo Pincaro Olayta</t>
+        </is>
+      </c>
+      <c r="C35" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D35" s="10" t="inlineStr"/>
+      <c r="E35" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F35" s="10" t="n">
+        <v>381.7</v>
+      </c>
+      <c r="G35" s="11" t="n">
+        <v>1.6312</v>
+      </c>
+      <c r="H35" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="10" t="n"/>
-      <c r="B36" s="10" t="n"/>
-      <c r="C36" s="10" t="n"/>
-      <c r="D36" s="10" t="n"/>
-      <c r="E36" s="10" t="n"/>
-      <c r="F36" s="10" t="n"/>
-      <c r="G36" s="10" t="n"/>
-      <c r="H36" s="10" t="n"/>
+      <c r="A36" s="10" t="inlineStr">
+        <is>
+          <t>16.</t>
+        </is>
+      </c>
+      <c r="B36" s="10" t="inlineStr">
+        <is>
+          <t>Shenaren Alapide Soneja</t>
+        </is>
+      </c>
+      <c r="C36" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D36" s="10" t="inlineStr"/>
+      <c r="E36" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F36" s="10" t="n">
+        <v>382.6</v>
+      </c>
+      <c r="G36" s="11" t="n">
+        <v>1.635</v>
+      </c>
+      <c r="H36" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="10" t="n"/>
-      <c r="B37" s="10" t="n"/>
-      <c r="C37" s="10" t="n"/>
-      <c r="D37" s="10" t="n"/>
-      <c r="E37" s="10" t="n"/>
-      <c r="F37" s="10" t="n"/>
-      <c r="G37" s="10" t="n"/>
-      <c r="H37" s="10" t="n"/>
+      <c r="A37" s="10" t="inlineStr">
+        <is>
+          <t>17.</t>
+        </is>
+      </c>
+      <c r="B37" s="10" t="inlineStr">
+        <is>
+          <t>Abby Gail Ativo Abo</t>
+        </is>
+      </c>
+      <c r="C37" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D37" s="10" t="inlineStr"/>
+      <c r="E37" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F37" s="10" t="n">
+        <v>383.1</v>
+      </c>
+      <c r="G37" s="11" t="n">
+        <v>1.6372</v>
+      </c>
+      <c r="H37" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="10" t="n"/>
-      <c r="B38" s="10" t="n"/>
-      <c r="C38" s="10" t="n"/>
-      <c r="D38" s="10" t="n"/>
-      <c r="E38" s="10" t="n"/>
-      <c r="F38" s="10" t="n"/>
-      <c r="G38" s="10" t="n"/>
-      <c r="H38" s="10" t="n"/>
+      <c r="A38" s="10" t="inlineStr">
+        <is>
+          <t>18.</t>
+        </is>
+      </c>
+      <c r="B38" s="10" t="inlineStr">
+        <is>
+          <t>Melrose Nota Razal</t>
+        </is>
+      </c>
+      <c r="C38" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D38" s="10" t="inlineStr"/>
+      <c r="E38" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F38" s="10" t="n">
+        <v>385.1</v>
+      </c>
+      <c r="G38" s="11" t="n">
+        <v>1.6457</v>
+      </c>
+      <c r="H38" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="10" t="n"/>
-      <c r="B39" s="10" t="n"/>
-      <c r="C39" s="10" t="n"/>
-      <c r="D39" s="10" t="n"/>
-      <c r="E39" s="10" t="n"/>
-      <c r="F39" s="10" t="n"/>
-      <c r="G39" s="10" t="n"/>
-      <c r="H39" s="10" t="n"/>
+      <c r="A39" s="10" t="inlineStr">
+        <is>
+          <t>19.</t>
+        </is>
+      </c>
+      <c r="B39" s="10" t="inlineStr">
+        <is>
+          <t>Noemi Sumalde Campita</t>
+        </is>
+      </c>
+      <c r="C39" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D39" s="10" t="inlineStr"/>
+      <c r="E39" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F39" s="10" t="n">
+        <v>385.1</v>
+      </c>
+      <c r="G39" s="11" t="n">
+        <v>1.6457</v>
+      </c>
+      <c r="H39" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="10" t="n"/>
-      <c r="B40" s="10" t="n"/>
-      <c r="C40" s="10" t="n"/>
-      <c r="D40" s="10" t="n"/>
-      <c r="E40" s="10" t="n"/>
-      <c r="F40" s="10" t="n"/>
-      <c r="G40" s="10" t="n"/>
-      <c r="H40" s="10" t="n"/>
+      <c r="A40" s="10" t="inlineStr">
+        <is>
+          <t>20.</t>
+        </is>
+      </c>
+      <c r="B40" s="10" t="inlineStr">
+        <is>
+          <t>Kristel Anne Bonayon Puenlabrada</t>
+        </is>
+      </c>
+      <c r="C40" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D40" s="10" t="inlineStr"/>
+      <c r="E40" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F40" s="10" t="n">
+        <v>386.8</v>
+      </c>
+      <c r="G40" s="11" t="n">
+        <v>1.653</v>
+      </c>
+      <c r="H40" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="10" t="n"/>
-      <c r="B41" s="10" t="n"/>
-      <c r="C41" s="10" t="n"/>
-      <c r="D41" s="10" t="n"/>
-      <c r="E41" s="10" t="n"/>
-      <c r="F41" s="10" t="n"/>
-      <c r="G41" s="10" t="n"/>
-      <c r="H41" s="10" t="n"/>
+      <c r="A41" s="10" t="inlineStr">
+        <is>
+          <t>21.</t>
+        </is>
+      </c>
+      <c r="B41" s="10" t="inlineStr">
+        <is>
+          <t>Shienalyn Joy Vargas Belen</t>
+        </is>
+      </c>
+      <c r="C41" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D41" s="10" t="inlineStr"/>
+      <c r="E41" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F41" s="10" t="n">
+        <v>387.4</v>
+      </c>
+      <c r="G41" s="11" t="n">
+        <v>1.6556</v>
+      </c>
+      <c r="H41" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="10" t="n"/>
-      <c r="B42" s="10" t="n"/>
-      <c r="C42" s="10" t="n"/>
-      <c r="D42" s="10" t="n"/>
-      <c r="E42" s="10" t="n"/>
-      <c r="F42" s="10" t="n"/>
-      <c r="G42" s="10" t="n"/>
-      <c r="H42" s="10" t="n"/>
+      <c r="A42" s="10" t="inlineStr">
+        <is>
+          <t>22.</t>
+        </is>
+      </c>
+      <c r="B42" s="10" t="inlineStr">
+        <is>
+          <t>Estelle Jonna Jao Estropia</t>
+        </is>
+      </c>
+      <c r="C42" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D42" s="10" t="inlineStr"/>
+      <c r="E42" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F42" s="10" t="n">
+        <v>387.5</v>
+      </c>
+      <c r="G42" s="11" t="n">
+        <v>1.656</v>
+      </c>
+      <c r="H42" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="10" t="n"/>
-      <c r="B43" s="10" t="n"/>
-      <c r="C43" s="10" t="n"/>
-      <c r="D43" s="10" t="n"/>
-      <c r="E43" s="10" t="n"/>
-      <c r="F43" s="10" t="n"/>
-      <c r="G43" s="10" t="n"/>
-      <c r="H43" s="10" t="n"/>
+      <c r="A43" s="10" t="inlineStr">
+        <is>
+          <t>23.</t>
+        </is>
+      </c>
+      <c r="B43" s="10" t="inlineStr">
+        <is>
+          <t>Rhyssa Mari Angela Gacosta Fortes</t>
+        </is>
+      </c>
+      <c r="C43" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D43" s="10" t="inlineStr"/>
+      <c r="E43" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F43" s="10" t="n">
+        <v>390.1</v>
+      </c>
+      <c r="G43" s="11" t="n">
+        <v>1.6671</v>
+      </c>
+      <c r="H43" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="10" t="n"/>
-      <c r="B44" s="10" t="n"/>
-      <c r="C44" s="10" t="n"/>
-      <c r="D44" s="10" t="n"/>
-      <c r="E44" s="10" t="n"/>
-      <c r="F44" s="10" t="n"/>
-      <c r="G44" s="10" t="n"/>
-      <c r="H44" s="10" t="n"/>
+      <c r="A44" s="10" t="inlineStr">
+        <is>
+          <t>24.</t>
+        </is>
+      </c>
+      <c r="B44" s="10" t="inlineStr">
+        <is>
+          <t>Christine May Maralit Antiquera</t>
+        </is>
+      </c>
+      <c r="C44" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D44" s="10" t="inlineStr"/>
+      <c r="E44" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F44" s="10" t="n">
+        <v>391</v>
+      </c>
+      <c r="G44" s="11" t="n">
+        <v>1.6709</v>
+      </c>
+      <c r="H44" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="10" t="n"/>
-      <c r="B45" s="10" t="n"/>
-      <c r="C45" s="10" t="n"/>
-      <c r="D45" s="10" t="n"/>
-      <c r="E45" s="10" t="n"/>
-      <c r="F45" s="10" t="n"/>
-      <c r="G45" s="10" t="n"/>
-      <c r="H45" s="10" t="n"/>
+      <c r="A45" s="10" t="inlineStr">
+        <is>
+          <t>25.</t>
+        </is>
+      </c>
+      <c r="B45" s="10" t="inlineStr">
+        <is>
+          <t>Danica Hazel Almasco Lacayanga</t>
+        </is>
+      </c>
+      <c r="C45" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D45" s="10" t="inlineStr"/>
+      <c r="E45" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F45" s="10" t="n">
+        <v>391.3</v>
+      </c>
+      <c r="G45" s="11" t="n">
+        <v>1.6722</v>
+      </c>
+      <c r="H45" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="10" t="n"/>
-      <c r="B46" s="10" t="n"/>
-      <c r="C46" s="10" t="n"/>
-      <c r="D46" s="10" t="n"/>
-      <c r="E46" s="10" t="n"/>
-      <c r="F46" s="10" t="n"/>
-      <c r="G46" s="10" t="n"/>
-      <c r="H46" s="10" t="n"/>
+      <c r="A46" s="10" t="inlineStr">
+        <is>
+          <t>26.</t>
+        </is>
+      </c>
+      <c r="B46" s="10" t="inlineStr">
+        <is>
+          <t>Krisha Mae Raro Ragas</t>
+        </is>
+      </c>
+      <c r="C46" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D46" s="10" t="inlineStr"/>
+      <c r="E46" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F46" s="10" t="n">
+        <v>391.5</v>
+      </c>
+      <c r="G46" s="11" t="n">
+        <v>1.6731</v>
+      </c>
+      <c r="H46" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="10" t="n"/>
-      <c r="B47" s="10" t="n"/>
-      <c r="C47" s="10" t="n"/>
-      <c r="D47" s="10" t="n"/>
-      <c r="E47" s="10" t="n"/>
-      <c r="F47" s="10" t="n"/>
-      <c r="G47" s="10" t="n"/>
-      <c r="H47" s="10" t="n"/>
+      <c r="A47" s="10" t="inlineStr">
+        <is>
+          <t>27.</t>
+        </is>
+      </c>
+      <c r="B47" s="10" t="inlineStr">
+        <is>
+          <t>Pia May Zara Atacador</t>
+        </is>
+      </c>
+      <c r="C47" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D47" s="10" t="inlineStr"/>
+      <c r="E47" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F47" s="10" t="n">
+        <v>393.1</v>
+      </c>
+      <c r="G47" s="11" t="n">
+        <v>1.6799</v>
+      </c>
+      <c r="H47" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" s="10" t="n"/>
-      <c r="B48" s="10" t="n"/>
-      <c r="C48" s="10" t="n"/>
-      <c r="D48" s="10" t="n"/>
-      <c r="E48" s="10" t="n"/>
-      <c r="F48" s="10" t="n"/>
-      <c r="G48" s="10" t="n"/>
-      <c r="H48" s="10" t="n"/>
+      <c r="A48" s="10" t="inlineStr">
+        <is>
+          <t>28.</t>
+        </is>
+      </c>
+      <c r="B48" s="10" t="inlineStr">
+        <is>
+          <t>Jendy Rose Federico Ferrer</t>
+        </is>
+      </c>
+      <c r="C48" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D48" s="10" t="inlineStr"/>
+      <c r="E48" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F48" s="10" t="n">
+        <v>394.2</v>
+      </c>
+      <c r="G48" s="11" t="n">
+        <v>1.6846</v>
+      </c>
+      <c r="H48" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="10" t="n"/>
-      <c r="B49" s="10" t="n"/>
-      <c r="C49" s="10" t="n"/>
-      <c r="D49" s="10" t="n"/>
-      <c r="E49" s="10" t="n"/>
-      <c r="F49" s="10" t="n"/>
-      <c r="G49" s="10" t="n"/>
-      <c r="H49" s="10" t="n"/>
+      <c r="A49" s="10" t="inlineStr">
+        <is>
+          <t>29.</t>
+        </is>
+      </c>
+      <c r="B49" s="10" t="inlineStr">
+        <is>
+          <t>Trizia Anne Morota Lolo</t>
+        </is>
+      </c>
+      <c r="C49" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D49" s="10" t="inlineStr"/>
+      <c r="E49" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F49" s="10" t="n">
+        <v>395.5</v>
+      </c>
+      <c r="G49" s="11" t="n">
+        <v>1.6902</v>
+      </c>
+      <c r="H49" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="10" t="n"/>
-      <c r="B50" s="10" t="n"/>
-      <c r="C50" s="10" t="n"/>
-      <c r="D50" s="10" t="n"/>
-      <c r="E50" s="10" t="n"/>
-      <c r="F50" s="10" t="n"/>
-      <c r="G50" s="10" t="n"/>
-      <c r="H50" s="10" t="n"/>
+      <c r="A50" s="10" t="inlineStr">
+        <is>
+          <t>30.</t>
+        </is>
+      </c>
+      <c r="B50" s="10" t="inlineStr">
+        <is>
+          <t>Geraldine Reblora Moico</t>
+        </is>
+      </c>
+      <c r="C50" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D50" s="10" t="inlineStr"/>
+      <c r="E50" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F50" s="10" t="n">
+        <v>395.7</v>
+      </c>
+      <c r="G50" s="11" t="n">
+        <v>1.691</v>
+      </c>
+      <c r="H50" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="10" t="n"/>
-      <c r="B51" s="10" t="n"/>
-      <c r="C51" s="10" t="n"/>
-      <c r="D51" s="10" t="n"/>
-      <c r="E51" s="10" t="n"/>
-      <c r="F51" s="10" t="n"/>
-      <c r="G51" s="10" t="n"/>
-      <c r="H51" s="10" t="n"/>
+      <c r="A51" s="10" t="inlineStr">
+        <is>
+          <t>31.</t>
+        </is>
+      </c>
+      <c r="B51" s="10" t="inlineStr">
+        <is>
+          <t>Jazreel Sadio De Vera</t>
+        </is>
+      </c>
+      <c r="C51" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D51" s="10" t="inlineStr"/>
+      <c r="E51" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F51" s="10" t="n">
+        <v>396.7</v>
+      </c>
+      <c r="G51" s="11" t="n">
+        <v>1.6953</v>
+      </c>
+      <c r="H51" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="10" t="n"/>
-      <c r="B52" s="10" t="n"/>
-      <c r="C52" s="10" t="n"/>
-      <c r="D52" s="10" t="n"/>
-      <c r="E52" s="10" t="n"/>
-      <c r="F52" s="10" t="n"/>
-      <c r="G52" s="10" t="n"/>
-      <c r="H52" s="10" t="n"/>
+      <c r="A52" s="10" t="inlineStr">
+        <is>
+          <t>32.</t>
+        </is>
+      </c>
+      <c r="B52" s="10" t="inlineStr">
+        <is>
+          <t>Bea Ativo Malejana</t>
+        </is>
+      </c>
+      <c r="C52" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D52" s="10" t="inlineStr"/>
+      <c r="E52" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F52" s="10" t="n">
+        <v>397.6</v>
+      </c>
+      <c r="G52" s="11" t="n">
+        <v>1.6991</v>
+      </c>
+      <c r="H52" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" s="10" t="n"/>
-      <c r="B53" s="10" t="n"/>
-      <c r="C53" s="10" t="n"/>
-      <c r="D53" s="10" t="n"/>
-      <c r="E53" s="10" t="n"/>
-      <c r="F53" s="10" t="n"/>
-      <c r="G53" s="10" t="n"/>
-      <c r="H53" s="10" t="n"/>
+      <c r="A53" s="10" t="inlineStr">
+        <is>
+          <t>33.</t>
+        </is>
+      </c>
+      <c r="B53" s="10" t="inlineStr">
+        <is>
+          <t>Rowena Mendez Nuñez</t>
+        </is>
+      </c>
+      <c r="C53" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D53" s="10" t="inlineStr"/>
+      <c r="E53" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F53" s="10" t="n">
+        <v>398.3</v>
+      </c>
+      <c r="G53" s="11" t="n">
+        <v>1.7021</v>
+      </c>
+      <c r="H53" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" s="10" t="n"/>
-      <c r="B54" s="10" t="n"/>
-      <c r="C54" s="10" t="n"/>
-      <c r="D54" s="10" t="n"/>
-      <c r="E54" s="10" t="n"/>
-      <c r="F54" s="10" t="n"/>
-      <c r="G54" s="10" t="n"/>
-      <c r="H54" s="10" t="n"/>
+      <c r="A54" s="10" t="inlineStr">
+        <is>
+          <t>34.</t>
+        </is>
+      </c>
+      <c r="B54" s="10" t="inlineStr">
+        <is>
+          <t>Irish Diane Buates Belleza</t>
+        </is>
+      </c>
+      <c r="C54" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D54" s="10" t="inlineStr"/>
+      <c r="E54" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F54" s="10" t="n">
+        <v>398.7</v>
+      </c>
+      <c r="G54" s="11" t="n">
+        <v>1.7038</v>
+      </c>
+      <c r="H54" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" s="10" t="n"/>
-      <c r="B55" s="10" t="n"/>
-      <c r="C55" s="10" t="n"/>
-      <c r="D55" s="10" t="n"/>
-      <c r="E55" s="10" t="n"/>
-      <c r="F55" s="10" t="n"/>
-      <c r="G55" s="10" t="n"/>
-      <c r="H55" s="10" t="n"/>
+      <c r="A55" s="10" t="inlineStr">
+        <is>
+          <t>35.</t>
+        </is>
+      </c>
+      <c r="B55" s="10" t="inlineStr">
+        <is>
+          <t>Angelica Dichoso Escalante</t>
+        </is>
+      </c>
+      <c r="C55" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D55" s="10" t="inlineStr"/>
+      <c r="E55" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F55" s="10" t="n">
+        <v>399.3</v>
+      </c>
+      <c r="G55" s="11" t="n">
+        <v>1.7064</v>
+      </c>
+      <c r="H55" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" s="10" t="n"/>
-      <c r="B56" s="10" t="n"/>
-      <c r="C56" s="10" t="n"/>
-      <c r="D56" s="10" t="n"/>
-      <c r="E56" s="10" t="n"/>
-      <c r="F56" s="10" t="n"/>
-      <c r="G56" s="10" t="n"/>
-      <c r="H56" s="10" t="n"/>
+      <c r="A56" s="10" t="inlineStr">
+        <is>
+          <t>36.</t>
+        </is>
+      </c>
+      <c r="B56" s="10" t="inlineStr">
+        <is>
+          <t>Catherine Belgica Babasa</t>
+        </is>
+      </c>
+      <c r="C56" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D56" s="10" t="inlineStr"/>
+      <c r="E56" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F56" s="10" t="n">
+        <v>400.3</v>
+      </c>
+      <c r="G56" s="11" t="n">
+        <v>1.7107</v>
+      </c>
+      <c r="H56" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" s="10" t="n"/>
-      <c r="B57" s="10" t="n"/>
-      <c r="C57" s="10" t="n"/>
-      <c r="D57" s="10" t="n"/>
-      <c r="E57" s="10" t="n"/>
-      <c r="F57" s="10" t="n"/>
-      <c r="G57" s="10" t="n"/>
-      <c r="H57" s="10" t="n"/>
+      <c r="A57" s="10" t="inlineStr">
+        <is>
+          <t>37.</t>
+        </is>
+      </c>
+      <c r="B57" s="10" t="inlineStr">
+        <is>
+          <t>Aira Vianca Vibar Dayto</t>
+        </is>
+      </c>
+      <c r="C57" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D57" s="10" t="inlineStr"/>
+      <c r="E57" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F57" s="10" t="n">
+        <v>401.1</v>
+      </c>
+      <c r="G57" s="11" t="n">
+        <v>1.7141</v>
+      </c>
+      <c r="H57" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" s="10" t="n"/>
-      <c r="B58" s="10" t="n"/>
-      <c r="C58" s="10" t="n"/>
-      <c r="D58" s="10" t="n"/>
-      <c r="E58" s="10" t="n"/>
-      <c r="F58" s="10" t="n"/>
-      <c r="G58" s="10" t="n"/>
-      <c r="H58" s="10" t="n"/>
+      <c r="A58" s="10" t="inlineStr">
+        <is>
+          <t>38.</t>
+        </is>
+      </c>
+      <c r="B58" s="10" t="inlineStr">
+        <is>
+          <t>Veronica Supeña Evangelio</t>
+        </is>
+      </c>
+      <c r="C58" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D58" s="10" t="inlineStr"/>
+      <c r="E58" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F58" s="10" t="n">
+        <v>401.3</v>
+      </c>
+      <c r="G58" s="11" t="n">
+        <v>1.715</v>
+      </c>
+      <c r="H58" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" s="10" t="n"/>
-      <c r="B59" s="10" t="n"/>
-      <c r="C59" s="10" t="n"/>
-      <c r="D59" s="10" t="n"/>
-      <c r="E59" s="10" t="n"/>
-      <c r="F59" s="10" t="n"/>
-      <c r="G59" s="10" t="n"/>
-      <c r="H59" s="10" t="n"/>
+      <c r="A59" s="10" t="inlineStr">
+        <is>
+          <t>39.</t>
+        </is>
+      </c>
+      <c r="B59" s="10" t="inlineStr">
+        <is>
+          <t>Kathleen Alexa Dasco Aspe</t>
+        </is>
+      </c>
+      <c r="C59" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D59" s="10" t="inlineStr"/>
+      <c r="E59" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F59" s="10" t="n">
+        <v>401.4</v>
+      </c>
+      <c r="G59" s="11" t="n">
+        <v>1.7154</v>
+      </c>
+      <c r="H59" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" s="10" t="n"/>
-      <c r="B60" s="10" t="n"/>
-      <c r="C60" s="10" t="n"/>
-      <c r="D60" s="10" t="n"/>
-      <c r="E60" s="10" t="n"/>
-      <c r="F60" s="10" t="n"/>
-      <c r="G60" s="10" t="n"/>
-      <c r="H60" s="10" t="n"/>
+      <c r="A60" s="10" t="inlineStr">
+        <is>
+          <t>40.</t>
+        </is>
+      </c>
+      <c r="B60" s="10" t="inlineStr">
+        <is>
+          <t>Norlissa Rose Vargas Callo</t>
+        </is>
+      </c>
+      <c r="C60" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D60" s="10" t="inlineStr"/>
+      <c r="E60" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F60" s="10" t="n">
+        <v>401.9</v>
+      </c>
+      <c r="G60" s="11" t="n">
+        <v>1.7175</v>
+      </c>
+      <c r="H60" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" s="10" t="n"/>
-      <c r="B61" s="10" t="n"/>
-      <c r="C61" s="10" t="n"/>
-      <c r="D61" s="10" t="n"/>
-      <c r="E61" s="10" t="n"/>
-      <c r="F61" s="10" t="n"/>
-      <c r="G61" s="10" t="n"/>
-      <c r="H61" s="10" t="n"/>
+      <c r="A61" s="10" t="inlineStr">
+        <is>
+          <t>41.</t>
+        </is>
+      </c>
+      <c r="B61" s="10" t="inlineStr">
+        <is>
+          <t>Airene Mesina Pagarigan</t>
+        </is>
+      </c>
+      <c r="C61" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D61" s="10" t="inlineStr"/>
+      <c r="E61" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F61" s="10" t="n">
+        <v>401.9</v>
+      </c>
+      <c r="G61" s="11" t="n">
+        <v>1.7175</v>
+      </c>
+      <c r="H61" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" s="10" t="n"/>
-      <c r="B62" s="10" t="n"/>
-      <c r="C62" s="10" t="n"/>
-      <c r="D62" s="10" t="n"/>
-      <c r="E62" s="10" t="n"/>
-      <c r="F62" s="10" t="n"/>
-      <c r="G62" s="10" t="n"/>
-      <c r="H62" s="10" t="n"/>
+      <c r="A62" s="10" t="inlineStr">
+        <is>
+          <t>42.</t>
+        </is>
+      </c>
+      <c r="B62" s="10" t="inlineStr">
+        <is>
+          <t>Oscar Calag Nota</t>
+        </is>
+      </c>
+      <c r="C62" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D62" s="10" t="inlineStr"/>
+      <c r="E62" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F62" s="10" t="n">
+        <v>401.9</v>
+      </c>
+      <c r="G62" s="11" t="n">
+        <v>1.7175</v>
+      </c>
+      <c r="H62" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="10" t="n"/>
-      <c r="B63" s="10" t="n"/>
-      <c r="C63" s="10" t="n"/>
-      <c r="D63" s="10" t="n"/>
-      <c r="E63" s="10" t="n"/>
-      <c r="F63" s="10" t="n"/>
-      <c r="G63" s="10" t="n"/>
-      <c r="H63" s="10" t="n"/>
+      <c r="A63" s="10" t="inlineStr">
+        <is>
+          <t>43.</t>
+        </is>
+      </c>
+      <c r="B63" s="10" t="inlineStr">
+        <is>
+          <t>Walter Nebreja Tolosa</t>
+        </is>
+      </c>
+      <c r="C63" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D63" s="10" t="inlineStr"/>
+      <c r="E63" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F63" s="10" t="n">
+        <v>402</v>
+      </c>
+      <c r="G63" s="11" t="n">
+        <v>1.7179</v>
+      </c>
+      <c r="H63" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" s="10" t="n"/>
-      <c r="B64" s="10" t="n"/>
-      <c r="C64" s="10" t="n"/>
-      <c r="D64" s="10" t="n"/>
-      <c r="E64" s="10" t="n"/>
-      <c r="F64" s="10" t="n"/>
-      <c r="G64" s="10" t="n"/>
-      <c r="H64" s="10" t="n"/>
+      <c r="A64" s="10" t="inlineStr">
+        <is>
+          <t>44.</t>
+        </is>
+      </c>
+      <c r="B64" s="10" t="inlineStr">
+        <is>
+          <t>Ana Margarita Pollante Perez</t>
+        </is>
+      </c>
+      <c r="C64" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D64" s="10" t="inlineStr"/>
+      <c r="E64" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F64" s="10" t="n">
+        <v>402.5</v>
+      </c>
+      <c r="G64" s="11" t="n">
+        <v>1.7201</v>
+      </c>
+      <c r="H64" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" s="10" t="n"/>
-      <c r="B65" s="10" t="n"/>
-      <c r="C65" s="10" t="n"/>
-      <c r="D65" s="10" t="n"/>
-      <c r="E65" s="10" t="n"/>
-      <c r="F65" s="10" t="n"/>
-      <c r="G65" s="10" t="n"/>
-      <c r="H65" s="10" t="n"/>
+      <c r="A65" s="10" t="inlineStr">
+        <is>
+          <t>45.</t>
+        </is>
+      </c>
+      <c r="B65" s="10" t="inlineStr">
+        <is>
+          <t>Gerald Jebulan Go</t>
+        </is>
+      </c>
+      <c r="C65" s="10" t="inlineStr"/>
+      <c r="D65" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="E65" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F65" s="10" t="n">
+        <v>402.7</v>
+      </c>
+      <c r="G65" s="11" t="n">
+        <v>1.7209</v>
+      </c>
+      <c r="H65" s="10" t="inlineStr">
+        <is>
+          <t>with Academic Distinction</t>
+        </is>
+      </c>
     </row>
     <row r="66">
-      <c r="A66" s="10" t="n"/>
-      <c r="B66" s="10" t="n"/>
-      <c r="C66" s="10" t="n"/>
-      <c r="D66" s="10" t="n"/>
-      <c r="E66" s="10" t="n"/>
-      <c r="F66" s="10" t="n"/>
-      <c r="G66" s="10" t="n"/>
-      <c r="H66" s="10" t="n"/>
+      <c r="A66" s="10" t="inlineStr">
+        <is>
+          <t>46.</t>
+        </is>
+      </c>
+      <c r="B66" s="10" t="inlineStr">
+        <is>
+          <t>Lizelle Anne Magno Arnado</t>
+        </is>
+      </c>
+      <c r="C66" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D66" s="10" t="inlineStr"/>
+      <c r="E66" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F66" s="10" t="n">
+        <v>404.9</v>
+      </c>
+      <c r="G66" s="11" t="n">
+        <v>1.7303</v>
+      </c>
+      <c r="H66" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="67">
-      <c r="A67" s="10" t="n"/>
-      <c r="B67" s="10" t="n"/>
-      <c r="C67" s="10" t="n"/>
-      <c r="D67" s="10" t="n"/>
-      <c r="E67" s="10" t="n"/>
-      <c r="F67" s="10" t="n"/>
-      <c r="G67" s="10" t="n"/>
-      <c r="H67" s="10" t="n"/>
+      <c r="A67" s="10" t="inlineStr">
+        <is>
+          <t>47.</t>
+        </is>
+      </c>
+      <c r="B67" s="10" t="inlineStr">
+        <is>
+          <t>Virgette Mae Leosala Tee</t>
+        </is>
+      </c>
+      <c r="C67" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D67" s="10" t="inlineStr"/>
+      <c r="E67" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F67" s="10" t="n">
+        <v>405.3</v>
+      </c>
+      <c r="G67" s="11" t="n">
+        <v>1.7321</v>
+      </c>
+      <c r="H67" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="68">
-      <c r="A68" s="10" t="n"/>
-      <c r="B68" s="10" t="n"/>
-      <c r="C68" s="10" t="n"/>
-      <c r="D68" s="10" t="n"/>
-      <c r="E68" s="10" t="n"/>
-      <c r="F68" s="10" t="n"/>
-      <c r="G68" s="10" t="n"/>
-      <c r="H68" s="10" t="n"/>
+      <c r="A68" s="10" t="inlineStr">
+        <is>
+          <t>48.</t>
+        </is>
+      </c>
+      <c r="B68" s="10" t="inlineStr">
+        <is>
+          <t>April Cyron Borromeo Salivio</t>
+        </is>
+      </c>
+      <c r="C68" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D68" s="10" t="inlineStr"/>
+      <c r="E68" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F68" s="10" t="n">
+        <v>405.5</v>
+      </c>
+      <c r="G68" s="11" t="n">
+        <v>1.7329</v>
+      </c>
+      <c r="H68" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="69">
-      <c r="A69" s="10" t="n"/>
-      <c r="B69" s="10" t="n"/>
-      <c r="C69" s="10" t="n"/>
-      <c r="D69" s="10" t="n"/>
-      <c r="E69" s="10" t="n"/>
-      <c r="F69" s="10" t="n"/>
-      <c r="G69" s="10" t="n"/>
-      <c r="H69" s="10" t="n"/>
+      <c r="A69" s="10" t="inlineStr">
+        <is>
+          <t>49.</t>
+        </is>
+      </c>
+      <c r="B69" s="10" t="inlineStr">
+        <is>
+          <t>Trixy Quinn Serrano Miranda</t>
+        </is>
+      </c>
+      <c r="C69" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D69" s="10" t="inlineStr"/>
+      <c r="E69" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F69" s="10" t="n">
+        <v>405.7</v>
+      </c>
+      <c r="G69" s="11" t="n">
+        <v>1.7338</v>
+      </c>
+      <c r="H69" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="70">
-      <c r="A70" s="10" t="n"/>
-      <c r="B70" s="10" t="n"/>
-      <c r="C70" s="10" t="n"/>
-      <c r="D70" s="10" t="n"/>
-      <c r="E70" s="10" t="n"/>
-      <c r="F70" s="10" t="n"/>
-      <c r="G70" s="10" t="n"/>
-      <c r="H70" s="10" t="n"/>
+      <c r="A70" s="10" t="inlineStr">
+        <is>
+          <t>50.</t>
+        </is>
+      </c>
+      <c r="B70" s="10" t="inlineStr">
+        <is>
+          <t>Jaymee Rose Chan Gonzales</t>
+        </is>
+      </c>
+      <c r="C70" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D70" s="10" t="inlineStr"/>
+      <c r="E70" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F70" s="10" t="n">
+        <v>406.3</v>
+      </c>
+      <c r="G70" s="11" t="n">
+        <v>1.7363</v>
+      </c>
+      <c r="H70" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="71">
-      <c r="A71" s="10" t="n"/>
-      <c r="B71" s="10" t="n"/>
-      <c r="C71" s="10" t="n"/>
-      <c r="D71" s="10" t="n"/>
-      <c r="E71" s="10" t="n"/>
-      <c r="F71" s="10" t="n"/>
-      <c r="G71" s="10" t="n"/>
-      <c r="H71" s="10" t="n"/>
+      <c r="A71" s="10" t="inlineStr">
+        <is>
+          <t>51.</t>
+        </is>
+      </c>
+      <c r="B71" s="10" t="inlineStr">
+        <is>
+          <t>Tessa Denissa Gelua Hipolito</t>
+        </is>
+      </c>
+      <c r="C71" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D71" s="10" t="inlineStr"/>
+      <c r="E71" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F71" s="10" t="n">
+        <v>407.3</v>
+      </c>
+      <c r="G71" s="11" t="n">
+        <v>1.7406</v>
+      </c>
+      <c r="H71" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="72">
-      <c r="A72" s="10" t="n"/>
-      <c r="B72" s="10" t="n"/>
-      <c r="C72" s="10" t="n"/>
-      <c r="D72" s="10" t="n"/>
-      <c r="E72" s="10" t="n"/>
-      <c r="F72" s="10" t="n"/>
-      <c r="G72" s="10" t="n"/>
-      <c r="H72" s="10" t="n"/>
+      <c r="A72" s="10" t="inlineStr">
+        <is>
+          <t>52.</t>
+        </is>
+      </c>
+      <c r="B72" s="10" t="inlineStr">
+        <is>
+          <t>Syra Tomagan Maloles</t>
+        </is>
+      </c>
+      <c r="C72" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D72" s="10" t="inlineStr"/>
+      <c r="E72" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F72" s="10" t="n">
+        <v>407.6</v>
+      </c>
+      <c r="G72" s="11" t="n">
+        <v>1.7419</v>
+      </c>
+      <c r="H72" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="73">
-      <c r="A73" s="10" t="n"/>
-      <c r="B73" s="10" t="n"/>
-      <c r="C73" s="10" t="n"/>
-      <c r="D73" s="10" t="n"/>
-      <c r="E73" s="10" t="n"/>
-      <c r="F73" s="10" t="n"/>
-      <c r="G73" s="10" t="n"/>
-      <c r="H73" s="10" t="n"/>
+      <c r="A73" s="10" t="inlineStr">
+        <is>
+          <t>53.</t>
+        </is>
+      </c>
+      <c r="B73" s="10" t="inlineStr">
+        <is>
+          <t>Bernardine Ella Tolosa Millena</t>
+        </is>
+      </c>
+      <c r="C73" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D73" s="10" t="inlineStr"/>
+      <c r="E73" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F73" s="10" t="n">
+        <v>407.7</v>
+      </c>
+      <c r="G73" s="11" t="n">
+        <v>1.7423</v>
+      </c>
+      <c r="H73" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="74">
-      <c r="A74" s="10" t="n"/>
-      <c r="B74" s="10" t="n"/>
-      <c r="C74" s="10" t="n"/>
-      <c r="D74" s="10" t="n"/>
-      <c r="E74" s="10" t="n"/>
-      <c r="F74" s="10" t="n"/>
-      <c r="G74" s="10" t="n"/>
-      <c r="H74" s="10" t="n"/>
+      <c r="A74" s="10" t="inlineStr">
+        <is>
+          <t>54.</t>
+        </is>
+      </c>
+      <c r="B74" s="10" t="inlineStr">
+        <is>
+          <t>Mary Joy Rebellon Reparip</t>
+        </is>
+      </c>
+      <c r="C74" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D74" s="10" t="inlineStr"/>
+      <c r="E74" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F74" s="10" t="n">
+        <v>408.2</v>
+      </c>
+      <c r="G74" s="11" t="n">
+        <v>1.7444</v>
+      </c>
+      <c r="H74" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="75">
-      <c r="A75" s="10" t="n"/>
-      <c r="B75" s="10" t="n"/>
-      <c r="C75" s="10" t="n"/>
-      <c r="D75" s="10" t="n"/>
-      <c r="E75" s="10" t="n"/>
-      <c r="F75" s="10" t="n"/>
-      <c r="G75" s="10" t="n"/>
-      <c r="H75" s="10" t="n"/>
+      <c r="A75" s="10" t="inlineStr">
+        <is>
+          <t>55.</t>
+        </is>
+      </c>
+      <c r="B75" s="10" t="inlineStr">
+        <is>
+          <t>Mark Joseph Granadillos Carretero</t>
+        </is>
+      </c>
+      <c r="C75" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D75" s="10" t="inlineStr"/>
+      <c r="E75" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F75" s="10" t="n">
+        <v>408.3</v>
+      </c>
+      <c r="G75" s="11" t="n">
+        <v>1.7449</v>
+      </c>
+      <c r="H75" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="76">
-      <c r="A76" s="10" t="n"/>
-      <c r="B76" s="10" t="n"/>
-      <c r="C76" s="10" t="n"/>
-      <c r="D76" s="10" t="n"/>
-      <c r="E76" s="10" t="n"/>
-      <c r="F76" s="10" t="n"/>
-      <c r="G76" s="10" t="n"/>
-      <c r="H76" s="10" t="n"/>
+      <c r="A76" s="10" t="inlineStr">
+        <is>
+          <t>56.</t>
+        </is>
+      </c>
+      <c r="B76" s="10" t="inlineStr">
+        <is>
+          <t>Joceline Ann Ayende Lozada</t>
+        </is>
+      </c>
+      <c r="C76" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D76" s="10" t="inlineStr"/>
+      <c r="E76" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F76" s="10" t="n">
+        <v>408.8</v>
+      </c>
+      <c r="G76" s="11" t="n">
+        <v>1.747</v>
+      </c>
+      <c r="H76" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="77">
-      <c r="A77" s="10" t="n"/>
-      <c r="B77" s="10" t="n"/>
-      <c r="C77" s="10" t="n"/>
-      <c r="D77" s="10" t="n"/>
-      <c r="E77" s="10" t="n"/>
-      <c r="F77" s="10" t="n"/>
-      <c r="G77" s="10" t="n"/>
-      <c r="H77" s="10" t="n"/>
+      <c r="A77" s="10" t="inlineStr">
+        <is>
+          <t>57.</t>
+        </is>
+      </c>
+      <c r="B77" s="10" t="inlineStr">
+        <is>
+          <t>Kate Louise Cadag Aviso</t>
+        </is>
+      </c>
+      <c r="C77" s="10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="D77" s="10" t="inlineStr"/>
+      <c r="E77" s="10" t="n">
+        <v>234</v>
+      </c>
+      <c r="F77" s="10" t="n">
+        <v>409.1</v>
+      </c>
+      <c r="G77" s="11" t="n">
+        <v>1.7483</v>
+      </c>
+      <c r="H77" s="10" t="inlineStr">
+        <is>
+          <t>Cum Laude</t>
+        </is>
+      </c>
     </row>
     <row r="78">
-      <c r="A78" s="11" t="n"/>
-      <c r="B78" s="11" t="n"/>
-      <c r="C78" s="11" t="n"/>
-      <c r="D78" s="11" t="n"/>
-      <c r="E78" s="11" t="n"/>
-      <c r="F78" s="11" t="n"/>
-      <c r="G78" s="11" t="n"/>
-      <c r="H78" s="11" t="n"/>
+      <c r="A78" s="12" t="n"/>
+      <c r="B78" s="12" t="n"/>
+      <c r="C78" s="12" t="n"/>
+      <c r="D78" s="12" t="n"/>
+      <c r="E78" s="12" t="n"/>
+      <c r="F78" s="12" t="n"/>
+      <c r="G78" s="12" t="n"/>
+      <c r="H78" s="12" t="n"/>
     </row>
     <row r="79">
-      <c r="A79" s="12" t="inlineStr">
+      <c r="A79" s="13" t="inlineStr">
         <is>
           <t>EVALUATION COMMITTEE:</t>
         </is>
       </c>
-      <c r="C79" s="11" t="n"/>
-      <c r="D79" s="11" t="n"/>
-      <c r="E79" s="11" t="n"/>
-      <c r="F79" s="11" t="n"/>
-      <c r="G79" s="11" t="n"/>
-      <c r="H79" s="11" t="n"/>
+      <c r="C79" s="12" t="n"/>
+      <c r="D79" s="12" t="n"/>
+      <c r="E79" s="12" t="n"/>
+      <c r="F79" s="12" t="n"/>
+      <c r="G79" s="12" t="n"/>
+      <c r="H79" s="12" t="n"/>
     </row>
     <row r="80">
-      <c r="A80" s="11" t="n"/>
-      <c r="B80" s="11" t="n"/>
-      <c r="C80" s="11" t="n"/>
-      <c r="D80" s="11" t="n"/>
-      <c r="E80" s="11" t="n"/>
-      <c r="F80" s="11" t="n"/>
-      <c r="G80" s="11" t="n"/>
-      <c r="H80" s="11" t="n"/>
+      <c r="A80" s="12" t="n"/>
+      <c r="B80" s="12" t="n"/>
+      <c r="C80" s="12" t="n"/>
+      <c r="D80" s="12" t="n"/>
+      <c r="E80" s="12" t="n"/>
+      <c r="F80" s="12" t="n"/>
+      <c r="G80" s="12" t="n"/>
+      <c r="H80" s="12" t="n"/>
     </row>
     <row r="81">
-      <c r="A81" s="11" t="n"/>
-      <c r="B81" s="11" t="inlineStr">
+      <c r="A81" s="12" t="n"/>
+      <c r="B81" s="12" t="inlineStr">
         <is>
           <t>_________________________</t>
         </is>
       </c>
-      <c r="D81" s="11" t="n"/>
-      <c r="E81" s="11" t="n"/>
-      <c r="F81" s="11" t="inlineStr">
+      <c r="D81" s="12" t="n"/>
+      <c r="E81" s="12" t="n"/>
+      <c r="F81" s="12" t="inlineStr">
         <is>
           <t>_________________________</t>
         </is>
       </c>
-      <c r="H81" s="11" t="n"/>
+      <c r="H81" s="12" t="n"/>
     </row>
     <row r="82">
-      <c r="A82" s="11" t="n"/>
+      <c r="A82" s="12" t="n"/>
       <c r="B82" s="2" t="inlineStr">
         <is>
           <t>Committee</t>
         </is>
       </c>
-      <c r="D82" s="11" t="n"/>
-      <c r="E82" s="11" t="n"/>
+      <c r="D82" s="12" t="n"/>
+      <c r="E82" s="12" t="n"/>
       <c r="F82" s="2" t="inlineStr">
         <is>
           <t>Committee</t>
         </is>
       </c>
-      <c r="H82" s="11" t="n"/>
+      <c r="H82" s="12" t="n"/>
     </row>
     <row r="83">
-      <c r="A83" s="11" t="n"/>
-      <c r="B83" s="13" t="inlineStr">
+      <c r="A83" s="12" t="n"/>
+      <c r="B83" s="14" t="inlineStr">
         <is>
           <t>Position</t>
         </is>
       </c>
-      <c r="D83" s="11" t="n"/>
-      <c r="E83" s="11" t="n"/>
-      <c r="F83" s="13" t="inlineStr">
+      <c r="D83" s="12" t="n"/>
+      <c r="E83" s="12" t="n"/>
+      <c r="F83" s="14" t="inlineStr">
         <is>
           <t>Position</t>
         </is>
       </c>
-      <c r="H83" s="11" t="n"/>
+      <c r="H83" s="12" t="n"/>
     </row>
     <row r="84">
-      <c r="A84" s="11" t="n"/>
-      <c r="B84" s="11" t="n"/>
-      <c r="C84" s="11" t="n"/>
-      <c r="D84" s="11" t="n"/>
-      <c r="E84" s="11" t="n"/>
-      <c r="F84" s="11" t="n"/>
-      <c r="G84" s="11" t="n"/>
-      <c r="H84" s="11" t="n"/>
+      <c r="A84" s="12" t="n"/>
+      <c r="B84" s="12" t="n"/>
+      <c r="C84" s="12" t="n"/>
+      <c r="D84" s="12" t="n"/>
+      <c r="E84" s="12" t="n"/>
+      <c r="F84" s="12" t="n"/>
+      <c r="G84" s="12" t="n"/>
+      <c r="H84" s="12" t="n"/>
     </row>
     <row r="85">
-      <c r="A85" s="11" t="n"/>
-      <c r="B85" s="11" t="n"/>
-      <c r="C85" s="11" t="n"/>
-      <c r="D85" s="11" t="n"/>
-      <c r="E85" s="11" t="n"/>
-      <c r="F85" s="11" t="n"/>
-      <c r="G85" s="11" t="n"/>
-      <c r="H85" s="11" t="n"/>
+      <c r="A85" s="12" t="n"/>
+      <c r="B85" s="12" t="n"/>
+      <c r="C85" s="12" t="n"/>
+      <c r="D85" s="12" t="n"/>
+      <c r="E85" s="12" t="n"/>
+      <c r="F85" s="12" t="n"/>
+      <c r="G85" s="12" t="n"/>
+      <c r="H85" s="12" t="n"/>
     </row>
     <row r="86">
-      <c r="A86" s="11" t="n"/>
-      <c r="B86" s="11" t="inlineStr">
+      <c r="A86" s="12" t="n"/>
+      <c r="B86" s="12" t="inlineStr">
         <is>
           <t>_________________________</t>
         </is>
       </c>
-      <c r="D86" s="11" t="n"/>
-      <c r="E86" s="11" t="n"/>
-      <c r="F86" s="11" t="inlineStr">
+      <c r="D86" s="12" t="n"/>
+      <c r="E86" s="12" t="n"/>
+      <c r="F86" s="12" t="inlineStr">
         <is>
           <t>_________________________</t>
         </is>
       </c>
-      <c r="H86" s="11" t="n"/>
+      <c r="H86" s="12" t="n"/>
     </row>
     <row r="87">
-      <c r="A87" s="11" t="n"/>
+      <c r="A87" s="12" t="n"/>
       <c r="B87" s="2" t="inlineStr">
         <is>
           <t>Committee</t>
         </is>
       </c>
-      <c r="D87" s="11" t="n"/>
-      <c r="E87" s="11" t="n"/>
+      <c r="D87" s="12" t="n"/>
+      <c r="E87" s="12" t="n"/>
       <c r="F87" s="2" t="inlineStr">
         <is>
           <t>Committee</t>
         </is>
       </c>
-      <c r="H87" s="11" t="n"/>
+      <c r="H87" s="12" t="n"/>
     </row>
     <row r="88">
-      <c r="A88" s="11" t="n"/>
-      <c r="B88" s="13" t="inlineStr">
+      <c r="A88" s="12" t="n"/>
+      <c r="B88" s="14" t="inlineStr">
         <is>
           <t>Position</t>
         </is>
       </c>
-      <c r="D88" s="11" t="n"/>
-      <c r="E88" s="11" t="n"/>
-      <c r="F88" s="13" t="inlineStr">
+      <c r="D88" s="12" t="n"/>
+      <c r="E88" s="12" t="n"/>
+      <c r="F88" s="14" t="inlineStr">
         <is>
           <t>Position</t>
         </is>
       </c>
-      <c r="H88" s="11" t="n"/>
+      <c r="H88" s="12" t="n"/>
     </row>
     <row r="89">
-      <c r="A89" s="11" t="n"/>
-      <c r="B89" s="11" t="n"/>
-      <c r="C89" s="11" t="n"/>
-      <c r="D89" s="11" t="n"/>
-      <c r="E89" s="11" t="n"/>
-      <c r="F89" s="11" t="n"/>
-      <c r="G89" s="11" t="n"/>
-      <c r="H89" s="11" t="n"/>
+      <c r="A89" s="12" t="n"/>
+      <c r="B89" s="12" t="n"/>
+      <c r="C89" s="12" t="n"/>
+      <c r="D89" s="12" t="n"/>
+      <c r="E89" s="12" t="n"/>
+      <c r="F89" s="12" t="n"/>
+      <c r="G89" s="12" t="n"/>
+      <c r="H89" s="12" t="n"/>
     </row>
     <row r="90">
-      <c r="A90" s="11" t="n"/>
-      <c r="B90" s="11" t="n"/>
-      <c r="C90" s="11" t="n"/>
-      <c r="D90" s="11" t="n"/>
-      <c r="E90" s="11" t="n"/>
-      <c r="F90" s="11" t="n"/>
-      <c r="G90" s="11" t="n"/>
-      <c r="H90" s="11" t="n"/>
+      <c r="A90" s="12" t="n"/>
+      <c r="B90" s="12" t="n"/>
+      <c r="C90" s="12" t="n"/>
+      <c r="D90" s="12" t="n"/>
+      <c r="E90" s="12" t="n"/>
+      <c r="F90" s="12" t="n"/>
+      <c r="G90" s="12" t="n"/>
+      <c r="H90" s="12" t="n"/>
     </row>
     <row r="91">
-      <c r="A91" s="11" t="n"/>
-      <c r="B91" s="11" t="n"/>
-      <c r="C91" s="11" t="inlineStr">
+      <c r="A91" s="12" t="n"/>
+      <c r="B91" s="12" t="n"/>
+      <c r="C91" s="12" t="inlineStr">
         <is>
           <t>Note:</t>
         </is>
       </c>
-      <c r="D91" s="11" t="n"/>
-      <c r="E91" s="11" t="n"/>
-      <c r="F91" s="11" t="n"/>
-      <c r="G91" s="11" t="n"/>
-      <c r="H91" s="11" t="n"/>
+      <c r="D91" s="12" t="n"/>
+      <c r="E91" s="12" t="n"/>
+      <c r="F91" s="12" t="n"/>
+      <c r="G91" s="12" t="n"/>
+      <c r="H91" s="12" t="n"/>
     </row>
     <row r="92">
-      <c r="A92" s="11" t="n"/>
-      <c r="B92" s="11" t="n"/>
-      <c r="C92" s="11" t="n"/>
-      <c r="D92" s="11" t="inlineStr">
+      <c r="A92" s="12" t="n"/>
+      <c r="B92" s="12" t="n"/>
+      <c r="C92" s="12" t="n"/>
+      <c r="D92" s="12" t="inlineStr">
         <is>
           <t>_________________________</t>
         </is>
       </c>
-      <c r="F92" s="11" t="n"/>
-      <c r="G92" s="11" t="n"/>
-      <c r="H92" s="11" t="n"/>
+      <c r="F92" s="12" t="n"/>
+      <c r="G92" s="12" t="n"/>
+      <c r="H92" s="12" t="n"/>
     </row>
     <row r="93">
-      <c r="A93" s="11" t="n"/>
-      <c r="B93" s="11" t="n"/>
-      <c r="C93" s="11" t="n"/>
+      <c r="A93" s="12" t="n"/>
+      <c r="B93" s="12" t="n"/>
+      <c r="C93" s="12" t="n"/>
       <c r="D93" s="2" t="inlineStr">
         <is>
           <t>Committee</t>
         </is>
       </c>
-      <c r="F93" s="11" t="n"/>
-      <c r="G93" s="11" t="n"/>
-      <c r="H93" s="11" t="n"/>
+      <c r="F93" s="12" t="n"/>
+      <c r="G93" s="12" t="n"/>
+      <c r="H93" s="12" t="n"/>
     </row>
     <row r="94">
-      <c r="A94" s="11" t="n"/>
-      <c r="B94" s="11" t="n"/>
-      <c r="C94" s="11" t="n"/>
-      <c r="D94" s="13" t="inlineStr">
+      <c r="A94" s="12" t="n"/>
+      <c r="B94" s="12" t="n"/>
+      <c r="C94" s="12" t="n"/>
+      <c r="D94" s="14" t="inlineStr">
         <is>
           <t>Position</t>
         </is>
       </c>
-      <c r="F94" s="11" t="n"/>
-      <c r="G94" s="11" t="n"/>
-      <c r="H94" s="11" t="n"/>
+      <c r="F94" s="12" t="n"/>
+      <c r="G94" s="12" t="n"/>
+      <c r="H94" s="12" t="n"/>
     </row>
     <row r="95">
-      <c r="A95" s="11" t="n"/>
-      <c r="B95" s="11" t="n"/>
-      <c r="C95" s="11" t="n"/>
-      <c r="D95" s="11" t="n"/>
-      <c r="E95" s="11" t="n"/>
-      <c r="F95" s="11" t="n"/>
-      <c r="G95" s="11" t="n"/>
-      <c r="H95" s="11" t="n"/>
+      <c r="A95" s="12" t="n"/>
+      <c r="B95" s="12" t="n"/>
+      <c r="C95" s="12" t="n"/>
+      <c r="D95" s="12" t="n"/>
+      <c r="E95" s="12" t="n"/>
+      <c r="F95" s="12" t="n"/>
+      <c r="G95" s="12" t="n"/>
+      <c r="H95" s="12" t="n"/>
     </row>
     <row r="96">
-      <c r="A96" s="11" t="n"/>
-      <c r="B96" s="11" t="n"/>
-      <c r="C96" s="11" t="n"/>
-      <c r="D96" s="11" t="n"/>
-      <c r="E96" s="11" t="n"/>
-      <c r="F96" s="11" t="n"/>
-      <c r="G96" s="11" t="n"/>
-      <c r="H96" s="11" t="n"/>
+      <c r="A96" s="12" t="n"/>
+      <c r="B96" s="12" t="n"/>
+      <c r="C96" s="12" t="n"/>
+      <c r="D96" s="12" t="n"/>
+      <c r="E96" s="12" t="n"/>
+      <c r="F96" s="12" t="n"/>
+      <c r="G96" s="12" t="n"/>
+      <c r="H96" s="12" t="n"/>
     </row>
     <row r="97">
-      <c r="A97" s="11" t="n"/>
-      <c r="B97" s="11" t="n"/>
-      <c r="C97" s="11" t="n"/>
-      <c r="D97" s="11" t="n"/>
-      <c r="E97" s="11" t="n"/>
-      <c r="F97" s="11" t="n"/>
-      <c r="G97" s="11" t="n"/>
-      <c r="H97" s="11" t="n"/>
+      <c r="A97" s="12" t="n"/>
+      <c r="B97" s="12" t="n"/>
+      <c r="C97" s="12" t="n"/>
+      <c r="D97" s="12" t="n"/>
+      <c r="E97" s="12" t="n"/>
+      <c r="F97" s="12" t="n"/>
+      <c r="G97" s="12" t="n"/>
+      <c r="H97" s="12" t="n"/>
     </row>
     <row r="98">
-      <c r="A98" s="11" t="n"/>
-      <c r="B98" s="11" t="n"/>
-      <c r="C98" s="11" t="n"/>
-      <c r="D98" s="11" t="n"/>
-      <c r="E98" s="11" t="n"/>
-      <c r="F98" s="11" t="n"/>
-      <c r="G98" s="11" t="n"/>
-      <c r="H98" s="11" t="n"/>
+      <c r="A98" s="12" t="n"/>
+      <c r="B98" s="12" t="n"/>
+      <c r="C98" s="12" t="n"/>
+      <c r="D98" s="12" t="n"/>
+      <c r="E98" s="12" t="n"/>
+      <c r="F98" s="12" t="n"/>
+      <c r="G98" s="12" t="n"/>
+      <c r="H98" s="12" t="n"/>
     </row>
     <row r="99">
-      <c r="A99" s="11" t="n"/>
-      <c r="B99" s="11" t="n"/>
-      <c r="C99" s="11" t="n"/>
-      <c r="D99" s="11" t="n"/>
-      <c r="E99" s="11" t="n"/>
-      <c r="F99" s="11" t="n"/>
-      <c r="G99" s="11" t="n"/>
-      <c r="H99" s="11" t="n"/>
+      <c r="A99" s="12" t="n"/>
+      <c r="B99" s="12" t="n"/>
+      <c r="C99" s="12" t="n"/>
+      <c r="D99" s="12" t="n"/>
+      <c r="E99" s="12" t="n"/>
+      <c r="F99" s="12" t="n"/>
+      <c r="G99" s="12" t="n"/>
+      <c r="H99" s="12" t="n"/>
     </row>
     <row r="100">
-      <c r="A100" s="11" t="n"/>
-      <c r="B100" s="11" t="n"/>
-      <c r="C100" s="11" t="n"/>
-      <c r="D100" s="11" t="n"/>
-      <c r="E100" s="11" t="n"/>
-      <c r="F100" s="11" t="n"/>
-      <c r="G100" s="11" t="n"/>
-      <c r="H100" s="11" t="n"/>
+      <c r="A100" s="12" t="n"/>
+      <c r="B100" s="12" t="n"/>
+      <c r="C100" s="12" t="n"/>
+      <c r="D100" s="12" t="n"/>
+      <c r="E100" s="12" t="n"/>
+      <c r="F100" s="12" t="n"/>
+      <c r="G100" s="12" t="n"/>
+      <c r="H100" s="12" t="n"/>
     </row>
     <row r="101">
-      <c r="A101" s="11" t="n"/>
-      <c r="B101" s="11" t="n"/>
-      <c r="C101" s="11" t="n"/>
-      <c r="D101" s="11" t="n"/>
-      <c r="E101" s="11" t="n"/>
-      <c r="F101" s="11" t="n"/>
-      <c r="G101" s="11" t="n"/>
-      <c r="H101" s="11" t="n"/>
+      <c r="A101" s="12" t="n"/>
+      <c r="B101" s="12" t="n"/>
+      <c r="C101" s="12" t="n"/>
+      <c r="D101" s="12" t="n"/>
+      <c r="E101" s="12" t="n"/>
+      <c r="F101" s="12" t="n"/>
+      <c r="G101" s="12" t="n"/>
+      <c r="H101" s="12" t="n"/>
     </row>
     <row r="102">
-      <c r="A102" s="11" t="n"/>
-      <c r="B102" s="11" t="n"/>
-      <c r="C102" s="11" t="n"/>
-      <c r="D102" s="11" t="n"/>
-      <c r="E102" s="11" t="n"/>
-      <c r="F102" s="11" t="n"/>
-      <c r="G102" s="11" t="n"/>
-      <c r="H102" s="11" t="n"/>
+      <c r="A102" s="12" t="n"/>
+      <c r="B102" s="12" t="n"/>
+      <c r="C102" s="12" t="n"/>
+      <c r="D102" s="12" t="n"/>
+      <c r="E102" s="12" t="n"/>
+      <c r="F102" s="12" t="n"/>
+      <c r="G102" s="12" t="n"/>
+      <c r="H102" s="12" t="n"/>
     </row>
     <row r="103">
-      <c r="A103" s="11" t="n"/>
-      <c r="B103" s="11" t="n"/>
-      <c r="C103" s="11" t="n"/>
-      <c r="D103" s="11" t="n"/>
-      <c r="E103" s="11" t="n"/>
-      <c r="F103" s="11" t="n"/>
-      <c r="G103" s="11" t="n"/>
-      <c r="H103" s="11" t="n"/>
+      <c r="A103" s="12" t="n"/>
+      <c r="B103" s="12" t="n"/>
+      <c r="C103" s="12" t="n"/>
+      <c r="D103" s="12" t="n"/>
+      <c r="E103" s="12" t="n"/>
+      <c r="F103" s="12" t="n"/>
+      <c r="G103" s="12" t="n"/>
+      <c r="H103" s="12" t="n"/>
     </row>
     <row r="104">
-      <c r="A104" s="11" t="n"/>
-      <c r="B104" s="14" t="inlineStr">
+      <c r="A104" s="12" t="n"/>
+      <c r="B104" s="15" t="inlineStr">
         <is>
           <t>Note: Subject for verification/recommendation/approval by the University Evaluation/Review Committee</t>
         </is>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="11" t="n"/>
-      <c r="B105" s="14" t="inlineStr">
+      <c r="A105" s="12" t="n"/>
+      <c r="B105" s="15" t="inlineStr">
         <is>
           <t>on Honor Graduates</t>
         </is>
       </c>
-      <c r="D105" s="11" t="n"/>
-      <c r="E105" s="11" t="n"/>
-      <c r="F105" s="11" t="n"/>
-      <c r="G105" s="11" t="n"/>
-      <c r="H105" s="11" t="n"/>
+      <c r="D105" s="12" t="n"/>
+      <c r="E105" s="12" t="n"/>
+      <c r="F105" s="12" t="n"/>
+      <c r="G105" s="12" t="n"/>
+      <c r="H105" s="12" t="n"/>
     </row>
     <row r="106">
-      <c r="A106" s="11" t="n"/>
-      <c r="B106" s="11" t="n"/>
-      <c r="C106" s="11" t="n"/>
-      <c r="D106" s="11" t="n"/>
-      <c r="E106" s="11" t="n"/>
-      <c r="F106" s="11" t="n"/>
-      <c r="G106" s="11" t="n"/>
-      <c r="H106" s="11" t="n"/>
+      <c r="A106" s="12" t="n"/>
+      <c r="B106" s="12" t="n"/>
+      <c r="C106" s="12" t="n"/>
+      <c r="D106" s="12" t="n"/>
+      <c r="E106" s="12" t="n"/>
+      <c r="F106" s="12" t="n"/>
+      <c r="G106" s="12" t="n"/>
+      <c r="H106" s="12" t="n"/>
     </row>
     <row r="107">
-      <c r="A107" s="11" t="n"/>
-      <c r="B107" s="14" t="inlineStr">
+      <c r="A107" s="12" t="n"/>
+      <c r="B107" s="15" t="inlineStr">
         <is>
           <t>Attached are the individual collegiate student's permanent record with the individual computation of grades</t>
         </is>
@@ -1809,284 +3066,656 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="15" t="n"/>
-      <c r="B126" s="15" t="n"/>
-      <c r="C126" s="15" t="n"/>
-      <c r="D126" s="15" t="n"/>
-      <c r="E126" s="15" t="n"/>
-      <c r="F126" s="15" t="n"/>
-      <c r="G126" s="15" t="n"/>
-      <c r="H126" s="15" t="n"/>
+      <c r="A126" s="16" t="inlineStr">
+        <is>
+          <t>58.</t>
+        </is>
+      </c>
+      <c r="B126" s="16" t="inlineStr">
+        <is>
+          <t>Ian Mediavillo Llaneta</t>
+        </is>
+      </c>
+      <c r="C126" s="16" t="inlineStr"/>
+      <c r="D126" s="16" t="inlineStr"/>
+      <c r="E126" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F126" s="16" t="n">
+        <v>409.1</v>
+      </c>
+      <c r="G126" s="16" t="n">
+        <v>1.7483</v>
+      </c>
+      <c r="H126" s="16" t="n"/>
     </row>
     <row r="127">
-      <c r="A127" s="15" t="n"/>
-      <c r="B127" s="15" t="n"/>
-      <c r="C127" s="15" t="n"/>
-      <c r="D127" s="15" t="n"/>
-      <c r="E127" s="15" t="n"/>
-      <c r="F127" s="15" t="n"/>
-      <c r="G127" s="15" t="n"/>
-      <c r="H127" s="15" t="n"/>
+      <c r="A127" s="16" t="inlineStr">
+        <is>
+          <t>59.</t>
+        </is>
+      </c>
+      <c r="B127" s="16" t="inlineStr">
+        <is>
+          <t>Charlene Bellen Baroso</t>
+        </is>
+      </c>
+      <c r="C127" s="16" t="inlineStr"/>
+      <c r="D127" s="16" t="inlineStr"/>
+      <c r="E127" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F127" s="16" t="n">
+        <v>411.7</v>
+      </c>
+      <c r="G127" s="16" t="n">
+        <v>1.7594</v>
+      </c>
+      <c r="H127" s="16" t="n"/>
     </row>
     <row r="128">
-      <c r="A128" s="15" t="n"/>
-      <c r="B128" s="15" t="n"/>
-      <c r="C128" s="15" t="n"/>
-      <c r="D128" s="15" t="n"/>
-      <c r="E128" s="15" t="n"/>
-      <c r="F128" s="15" t="n"/>
-      <c r="G128" s="15" t="n"/>
-      <c r="H128" s="15" t="n"/>
+      <c r="A128" s="16" t="inlineStr">
+        <is>
+          <t>60.</t>
+        </is>
+      </c>
+      <c r="B128" s="16" t="inlineStr">
+        <is>
+          <t>Lyka Marie Escurel Fullente</t>
+        </is>
+      </c>
+      <c r="C128" s="16" t="inlineStr"/>
+      <c r="D128" s="16" t="inlineStr"/>
+      <c r="E128" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F128" s="16" t="n">
+        <v>412</v>
+      </c>
+      <c r="G128" s="16" t="n">
+        <v>1.7607</v>
+      </c>
+      <c r="H128" s="16" t="n"/>
     </row>
     <row r="129">
-      <c r="A129" s="15" t="n"/>
-      <c r="B129" s="15" t="n"/>
-      <c r="C129" s="15" t="n"/>
-      <c r="D129" s="15" t="n"/>
-      <c r="E129" s="15" t="n"/>
-      <c r="F129" s="15" t="n"/>
-      <c r="G129" s="15" t="n"/>
-      <c r="H129" s="15" t="n"/>
+      <c r="A129" s="16" t="inlineStr">
+        <is>
+          <t>61.</t>
+        </is>
+      </c>
+      <c r="B129" s="16" t="inlineStr">
+        <is>
+          <t>Jhon Christian Grimpluma Biñas</t>
+        </is>
+      </c>
+      <c r="C129" s="16" t="inlineStr"/>
+      <c r="D129" s="16" t="inlineStr"/>
+      <c r="E129" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F129" s="16" t="n">
+        <v>414.3</v>
+      </c>
+      <c r="G129" s="16" t="n">
+        <v>1.7705</v>
+      </c>
+      <c r="H129" s="16" t="n"/>
     </row>
     <row r="130">
-      <c r="A130" s="15" t="n"/>
-      <c r="B130" s="15" t="n"/>
-      <c r="C130" s="15" t="n"/>
-      <c r="D130" s="15" t="n"/>
-      <c r="E130" s="15" t="n"/>
-      <c r="F130" s="15" t="n"/>
-      <c r="G130" s="15" t="n"/>
-      <c r="H130" s="15" t="n"/>
+      <c r="A130" s="16" t="inlineStr">
+        <is>
+          <t>63.</t>
+        </is>
+      </c>
+      <c r="B130" s="16" t="inlineStr">
+        <is>
+          <t>Alizza May Cantillo Salando</t>
+        </is>
+      </c>
+      <c r="C130" s="16" t="inlineStr"/>
+      <c r="D130" s="16" t="inlineStr"/>
+      <c r="E130" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F130" s="16" t="n">
+        <v>417.3</v>
+      </c>
+      <c r="G130" s="16" t="n">
+        <v>1.7833</v>
+      </c>
+      <c r="H130" s="16" t="n"/>
     </row>
     <row r="131">
-      <c r="A131" s="15" t="n"/>
-      <c r="B131" s="15" t="n"/>
-      <c r="C131" s="15" t="n"/>
-      <c r="D131" s="15" t="n"/>
-      <c r="E131" s="15" t="n"/>
-      <c r="F131" s="15" t="n"/>
-      <c r="G131" s="15" t="n"/>
-      <c r="H131" s="15" t="n"/>
+      <c r="A131" s="16" t="inlineStr">
+        <is>
+          <t>64.</t>
+        </is>
+      </c>
+      <c r="B131" s="16" t="inlineStr">
+        <is>
+          <t>Merari Deborah Falabi Catorce</t>
+        </is>
+      </c>
+      <c r="C131" s="16" t="inlineStr"/>
+      <c r="D131" s="16" t="inlineStr"/>
+      <c r="E131" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F131" s="16" t="n">
+        <v>422.2</v>
+      </c>
+      <c r="G131" s="16" t="n">
+        <v>1.8043</v>
+      </c>
+      <c r="H131" s="16" t="n"/>
     </row>
     <row r="132">
-      <c r="A132" s="15" t="n"/>
-      <c r="B132" s="15" t="n"/>
-      <c r="C132" s="15" t="n"/>
-      <c r="D132" s="15" t="n"/>
-      <c r="E132" s="15" t="n"/>
-      <c r="F132" s="15" t="n"/>
-      <c r="G132" s="15" t="n"/>
-      <c r="H132" s="15" t="n"/>
+      <c r="A132" s="16" t="inlineStr">
+        <is>
+          <t>65.</t>
+        </is>
+      </c>
+      <c r="B132" s="16" t="inlineStr">
+        <is>
+          <t>Carla Jae Bitancur Barela</t>
+        </is>
+      </c>
+      <c r="C132" s="16" t="inlineStr"/>
+      <c r="D132" s="16" t="inlineStr"/>
+      <c r="E132" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F132" s="16" t="n">
+        <v>417.9</v>
+      </c>
+      <c r="G132" s="16" t="n">
+        <v>1.7859</v>
+      </c>
+      <c r="H132" s="16" t="n"/>
     </row>
     <row r="133">
-      <c r="A133" s="15" t="n"/>
-      <c r="B133" s="15" t="n"/>
-      <c r="C133" s="15" t="n"/>
-      <c r="D133" s="15" t="n"/>
-      <c r="E133" s="15" t="n"/>
-      <c r="F133" s="15" t="n"/>
-      <c r="G133" s="15" t="n"/>
-      <c r="H133" s="15" t="n"/>
+      <c r="A133" s="16" t="inlineStr">
+        <is>
+          <t>66.</t>
+        </is>
+      </c>
+      <c r="B133" s="16" t="inlineStr">
+        <is>
+          <t>Stacy Kate Yuson Guerrero</t>
+        </is>
+      </c>
+      <c r="C133" s="16" t="inlineStr"/>
+      <c r="D133" s="16" t="inlineStr"/>
+      <c r="E133" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F133" s="16" t="n">
+        <v>418.2</v>
+      </c>
+      <c r="G133" s="16" t="n">
+        <v>1.7872</v>
+      </c>
+      <c r="H133" s="16" t="n"/>
     </row>
     <row r="134">
-      <c r="A134" s="15" t="n"/>
-      <c r="B134" s="15" t="n"/>
-      <c r="C134" s="15" t="n"/>
-      <c r="D134" s="15" t="n"/>
-      <c r="E134" s="15" t="n"/>
-      <c r="F134" s="15" t="n"/>
-      <c r="G134" s="15" t="n"/>
-      <c r="H134" s="15" t="n"/>
+      <c r="A134" s="16" t="inlineStr">
+        <is>
+          <t>67.</t>
+        </is>
+      </c>
+      <c r="B134" s="16" t="inlineStr">
+        <is>
+          <t>Justine Lorilla Daria</t>
+        </is>
+      </c>
+      <c r="C134" s="16" t="inlineStr"/>
+      <c r="D134" s="16" t="inlineStr"/>
+      <c r="E134" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F134" s="16" t="n">
+        <v>419</v>
+      </c>
+      <c r="G134" s="16" t="n">
+        <v>1.7906</v>
+      </c>
+      <c r="H134" s="16" t="n"/>
     </row>
     <row r="135">
-      <c r="A135" s="15" t="n"/>
-      <c r="B135" s="15" t="n"/>
-      <c r="C135" s="15" t="n"/>
-      <c r="D135" s="15" t="n"/>
-      <c r="E135" s="15" t="n"/>
-      <c r="F135" s="15" t="n"/>
-      <c r="G135" s="15" t="n"/>
-      <c r="H135" s="15" t="n"/>
+      <c r="A135" s="16" t="inlineStr">
+        <is>
+          <t>68.</t>
+        </is>
+      </c>
+      <c r="B135" s="16" t="inlineStr">
+        <is>
+          <t>Cianiah Kaela Mimay Apurado</t>
+        </is>
+      </c>
+      <c r="C135" s="16" t="inlineStr"/>
+      <c r="D135" s="16" t="inlineStr"/>
+      <c r="E135" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F135" s="16" t="n">
+        <v>420</v>
+      </c>
+      <c r="G135" s="16" t="n">
+        <v>1.7949</v>
+      </c>
+      <c r="H135" s="16" t="n"/>
     </row>
     <row r="136">
-      <c r="A136" s="15" t="n"/>
-      <c r="B136" s="15" t="n"/>
-      <c r="C136" s="15" t="n"/>
-      <c r="D136" s="15" t="n"/>
-      <c r="E136" s="15" t="n"/>
-      <c r="F136" s="15" t="n"/>
-      <c r="G136" s="15" t="n"/>
-      <c r="H136" s="15" t="n"/>
+      <c r="A136" s="16" t="inlineStr">
+        <is>
+          <t>69.</t>
+        </is>
+      </c>
+      <c r="B136" s="16" t="inlineStr">
+        <is>
+          <t>Hans Christian Gonzales Imperial</t>
+        </is>
+      </c>
+      <c r="C136" s="16" t="inlineStr"/>
+      <c r="D136" s="16" t="inlineStr"/>
+      <c r="E136" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F136" s="16" t="n">
+        <v>420.1</v>
+      </c>
+      <c r="G136" s="16" t="n">
+        <v>1.7953</v>
+      </c>
+      <c r="H136" s="16" t="n"/>
     </row>
     <row r="137">
-      <c r="A137" s="15" t="n"/>
-      <c r="B137" s="15" t="n"/>
-      <c r="C137" s="15" t="n"/>
-      <c r="D137" s="15" t="n"/>
-      <c r="E137" s="15" t="n"/>
-      <c r="F137" s="15" t="n"/>
-      <c r="G137" s="15" t="n"/>
-      <c r="H137" s="15" t="n"/>
+      <c r="A137" s="16" t="inlineStr">
+        <is>
+          <t>70.</t>
+        </is>
+      </c>
+      <c r="B137" s="16" t="inlineStr">
+        <is>
+          <t>Ma. Elaine Jacob Abejo</t>
+        </is>
+      </c>
+      <c r="C137" s="16" t="inlineStr"/>
+      <c r="D137" s="16" t="inlineStr"/>
+      <c r="E137" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F137" s="16" t="n">
+        <v>420.9</v>
+      </c>
+      <c r="G137" s="16" t="n">
+        <v>1.7987</v>
+      </c>
+      <c r="H137" s="16" t="n"/>
     </row>
     <row r="138">
-      <c r="A138" s="15" t="n"/>
-      <c r="B138" s="15" t="n"/>
-      <c r="C138" s="15" t="n"/>
-      <c r="D138" s="15" t="n"/>
-      <c r="E138" s="15" t="n"/>
-      <c r="F138" s="15" t="n"/>
-      <c r="G138" s="15" t="n"/>
-      <c r="H138" s="15" t="n"/>
+      <c r="A138" s="16" t="inlineStr">
+        <is>
+          <t>71.</t>
+        </is>
+      </c>
+      <c r="B138" s="16" t="inlineStr">
+        <is>
+          <t>Ella Mae Patiño Suruiz</t>
+        </is>
+      </c>
+      <c r="C138" s="16" t="inlineStr"/>
+      <c r="D138" s="16" t="inlineStr"/>
+      <c r="E138" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F138" s="16" t="n">
+        <v>421.3</v>
+      </c>
+      <c r="G138" s="16" t="n">
+        <v>1.8004</v>
+      </c>
+      <c r="H138" s="16" t="n"/>
     </row>
     <row r="139">
-      <c r="A139" s="15" t="n"/>
-      <c r="B139" s="15" t="n"/>
-      <c r="C139" s="15" t="n"/>
-      <c r="D139" s="15" t="n"/>
-      <c r="E139" s="15" t="n"/>
-      <c r="F139" s="15" t="n"/>
-      <c r="G139" s="15" t="n"/>
-      <c r="H139" s="15" t="n"/>
+      <c r="A139" s="16" t="inlineStr">
+        <is>
+          <t>72.</t>
+        </is>
+      </c>
+      <c r="B139" s="16" t="inlineStr">
+        <is>
+          <t>China Araya Goyena</t>
+        </is>
+      </c>
+      <c r="C139" s="16" t="inlineStr"/>
+      <c r="D139" s="16" t="inlineStr"/>
+      <c r="E139" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F139" s="16" t="n">
+        <v>422.9</v>
+      </c>
+      <c r="G139" s="16" t="n">
+        <v>1.8073</v>
+      </c>
+      <c r="H139" s="16" t="n"/>
     </row>
     <row r="140">
-      <c r="A140" s="15" t="n"/>
-      <c r="B140" s="15" t="n"/>
-      <c r="C140" s="15" t="n"/>
-      <c r="D140" s="15" t="n"/>
-      <c r="E140" s="15" t="n"/>
-      <c r="F140" s="15" t="n"/>
-      <c r="G140" s="15" t="n"/>
-      <c r="H140" s="15" t="n"/>
+      <c r="A140" s="17" t="inlineStr">
+        <is>
+          <t>73.</t>
+        </is>
+      </c>
+      <c r="B140" s="17" t="inlineStr">
+        <is>
+          <t>Joanne Karla Caldit Consuelo</t>
+        </is>
+      </c>
+      <c r="C140" s="17" t="inlineStr"/>
+      <c r="D140" s="17" t="inlineStr"/>
+      <c r="E140" s="17" t="n">
+        <v>216</v>
+      </c>
+      <c r="F140" s="17" t="n">
+        <v>363</v>
+      </c>
+      <c r="G140" s="11" t="n">
+        <v>1.6806</v>
+      </c>
+      <c r="H140" s="16" t="n"/>
     </row>
     <row r="141">
-      <c r="A141" s="15" t="n"/>
-      <c r="B141" s="15" t="n"/>
-      <c r="C141" s="15" t="n"/>
-      <c r="D141" s="15" t="n"/>
-      <c r="E141" s="15" t="n"/>
-      <c r="F141" s="15" t="n"/>
-      <c r="G141" s="15" t="n"/>
-      <c r="H141" s="15" t="n"/>
+      <c r="A141" s="16" t="inlineStr">
+        <is>
+          <t>74.</t>
+        </is>
+      </c>
+      <c r="B141" s="16" t="inlineStr">
+        <is>
+          <t>Christine Joy Belano Deona</t>
+        </is>
+      </c>
+      <c r="C141" s="16" t="inlineStr"/>
+      <c r="D141" s="16" t="inlineStr"/>
+      <c r="E141" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F141" s="16" t="n">
+        <v>425.6</v>
+      </c>
+      <c r="G141" s="16" t="n">
+        <v>1.8188</v>
+      </c>
+      <c r="H141" s="16" t="n"/>
     </row>
     <row r="142">
-      <c r="A142" s="15" t="n"/>
-      <c r="B142" s="15" t="n"/>
-      <c r="C142" s="15" t="n"/>
-      <c r="D142" s="15" t="n"/>
-      <c r="E142" s="15" t="n"/>
-      <c r="F142" s="15" t="n"/>
-      <c r="G142" s="15" t="n"/>
-      <c r="H142" s="15" t="n"/>
+      <c r="A142" s="16" t="inlineStr">
+        <is>
+          <t>75.</t>
+        </is>
+      </c>
+      <c r="B142" s="16" t="inlineStr">
+        <is>
+          <t>Ignacio Rodriguez Juaquera</t>
+        </is>
+      </c>
+      <c r="C142" s="16" t="inlineStr"/>
+      <c r="D142" s="16" t="inlineStr"/>
+      <c r="E142" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F142" s="16" t="n">
+        <v>426.5</v>
+      </c>
+      <c r="G142" s="16" t="n">
+        <v>1.8226</v>
+      </c>
+      <c r="H142" s="16" t="n"/>
     </row>
     <row r="143">
-      <c r="A143" s="15" t="n"/>
-      <c r="B143" s="15" t="n"/>
-      <c r="C143" s="15" t="n"/>
-      <c r="D143" s="15" t="n"/>
-      <c r="E143" s="15" t="n"/>
-      <c r="F143" s="15" t="n"/>
-      <c r="G143" s="15" t="n"/>
-      <c r="H143" s="15" t="n"/>
+      <c r="A143" s="16" t="inlineStr">
+        <is>
+          <t>76.</t>
+        </is>
+      </c>
+      <c r="B143" s="16" t="inlineStr">
+        <is>
+          <t>Vanessa Alemania Leosala</t>
+        </is>
+      </c>
+      <c r="C143" s="16" t="inlineStr"/>
+      <c r="D143" s="16" t="inlineStr"/>
+      <c r="E143" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F143" s="16" t="n">
+        <v>427.2</v>
+      </c>
+      <c r="G143" s="16" t="n">
+        <v>1.8256</v>
+      </c>
+      <c r="H143" s="16" t="n"/>
     </row>
     <row r="144">
-      <c r="A144" s="15" t="n"/>
-      <c r="B144" s="15" t="n"/>
-      <c r="C144" s="15" t="n"/>
-      <c r="D144" s="15" t="n"/>
-      <c r="E144" s="15" t="n"/>
-      <c r="F144" s="15" t="n"/>
-      <c r="G144" s="15" t="n"/>
-      <c r="H144" s="15" t="n"/>
+      <c r="A144" s="16" t="inlineStr">
+        <is>
+          <t>77.</t>
+        </is>
+      </c>
+      <c r="B144" s="16" t="inlineStr">
+        <is>
+          <t>Vanessa Mae Sia Cañete</t>
+        </is>
+      </c>
+      <c r="C144" s="16" t="inlineStr"/>
+      <c r="D144" s="16" t="inlineStr"/>
+      <c r="E144" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F144" s="16" t="n">
+        <v>430.2</v>
+      </c>
+      <c r="G144" s="16" t="n">
+        <v>1.8385</v>
+      </c>
+      <c r="H144" s="16" t="n"/>
     </row>
     <row r="145">
-      <c r="A145" s="15" t="n"/>
-      <c r="B145" s="15" t="n"/>
-      <c r="C145" s="15" t="n"/>
-      <c r="D145" s="15" t="n"/>
-      <c r="E145" s="15" t="n"/>
-      <c r="F145" s="15" t="n"/>
-      <c r="G145" s="15" t="n"/>
-      <c r="H145" s="15" t="n"/>
+      <c r="A145" s="16" t="inlineStr">
+        <is>
+          <t>78.</t>
+        </is>
+      </c>
+      <c r="B145" s="16" t="inlineStr">
+        <is>
+          <t>Jazmin Shane Adlaon Calisin</t>
+        </is>
+      </c>
+      <c r="C145" s="16" t="inlineStr"/>
+      <c r="D145" s="16" t="inlineStr"/>
+      <c r="E145" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F145" s="16" t="n">
+        <v>430.6</v>
+      </c>
+      <c r="G145" s="16" t="n">
+        <v>1.8402</v>
+      </c>
+      <c r="H145" s="16" t="n"/>
     </row>
     <row r="146">
-      <c r="A146" s="15" t="n"/>
-      <c r="B146" s="15" t="n"/>
-      <c r="C146" s="15" t="n"/>
-      <c r="D146" s="15" t="n"/>
-      <c r="E146" s="15" t="n"/>
-      <c r="F146" s="15" t="n"/>
-      <c r="G146" s="15" t="n"/>
-      <c r="H146" s="15" t="n"/>
+      <c r="A146" s="16" t="inlineStr">
+        <is>
+          <t>79.</t>
+        </is>
+      </c>
+      <c r="B146" s="16" t="inlineStr">
+        <is>
+          <t>Rev Neo Pavilando</t>
+        </is>
+      </c>
+      <c r="C146" s="16" t="inlineStr"/>
+      <c r="D146" s="16" t="inlineStr"/>
+      <c r="E146" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F146" s="16" t="n">
+        <v>431.8</v>
+      </c>
+      <c r="G146" s="16" t="n">
+        <v>1.8453</v>
+      </c>
+      <c r="H146" s="16" t="n"/>
     </row>
     <row r="147">
-      <c r="A147" s="15" t="n"/>
-      <c r="B147" s="15" t="n"/>
-      <c r="C147" s="15" t="n"/>
-      <c r="D147" s="15" t="n"/>
-      <c r="E147" s="15" t="n"/>
-      <c r="F147" s="15" t="n"/>
-      <c r="G147" s="15" t="n"/>
-      <c r="H147" s="15" t="n"/>
+      <c r="A147" s="16" t="inlineStr">
+        <is>
+          <t>80.</t>
+        </is>
+      </c>
+      <c r="B147" s="16" t="inlineStr">
+        <is>
+          <t>Glenn Homer Polo Naparam</t>
+        </is>
+      </c>
+      <c r="C147" s="16" t="inlineStr"/>
+      <c r="D147" s="16" t="inlineStr"/>
+      <c r="E147" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F147" s="16" t="n">
+        <v>432.3</v>
+      </c>
+      <c r="G147" s="16" t="n">
+        <v>1.8474</v>
+      </c>
+      <c r="H147" s="16" t="n"/>
     </row>
     <row r="148">
-      <c r="A148" s="15" t="n"/>
-      <c r="B148" s="15" t="n"/>
-      <c r="C148" s="15" t="n"/>
-      <c r="D148" s="15" t="n"/>
-      <c r="E148" s="15" t="n"/>
-      <c r="F148" s="15" t="n"/>
-      <c r="G148" s="15" t="n"/>
-      <c r="H148" s="15" t="n"/>
+      <c r="A148" s="16" t="inlineStr">
+        <is>
+          <t>81.</t>
+        </is>
+      </c>
+      <c r="B148" s="16" t="inlineStr">
+        <is>
+          <t>Christine Reocasa Paguio</t>
+        </is>
+      </c>
+      <c r="C148" s="16" t="inlineStr"/>
+      <c r="D148" s="16" t="inlineStr"/>
+      <c r="E148" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F148" s="16" t="n">
+        <v>433.5</v>
+      </c>
+      <c r="G148" s="16" t="n">
+        <v>1.8526</v>
+      </c>
+      <c r="H148" s="16" t="n"/>
     </row>
     <row r="149">
-      <c r="A149" s="15" t="n"/>
-      <c r="B149" s="15" t="n"/>
-      <c r="C149" s="15" t="n"/>
-      <c r="D149" s="15" t="n"/>
-      <c r="E149" s="15" t="n"/>
-      <c r="F149" s="15" t="n"/>
-      <c r="G149" s="15" t="n"/>
-      <c r="H149" s="15" t="n"/>
+      <c r="A149" s="16" t="inlineStr">
+        <is>
+          <t>82.</t>
+        </is>
+      </c>
+      <c r="B149" s="16" t="inlineStr">
+        <is>
+          <t>Renee Lynne Maquiñiana Camposano</t>
+        </is>
+      </c>
+      <c r="C149" s="16" t="inlineStr"/>
+      <c r="D149" s="16" t="inlineStr"/>
+      <c r="E149" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F149" s="16" t="n">
+        <v>439.2</v>
+      </c>
+      <c r="G149" s="16" t="n">
+        <v>1.8769</v>
+      </c>
+      <c r="H149" s="16" t="n"/>
     </row>
     <row r="150">
-      <c r="A150" s="15" t="n"/>
-      <c r="B150" s="15" t="n"/>
-      <c r="C150" s="15" t="n"/>
-      <c r="D150" s="15" t="n"/>
-      <c r="E150" s="15" t="n"/>
-      <c r="F150" s="15" t="n"/>
-      <c r="G150" s="15" t="n"/>
-      <c r="H150" s="15" t="n"/>
+      <c r="A150" s="16" t="inlineStr">
+        <is>
+          <t>83.</t>
+        </is>
+      </c>
+      <c r="B150" s="16" t="inlineStr">
+        <is>
+          <t>Pauline Anne Vibar Balilo</t>
+        </is>
+      </c>
+      <c r="C150" s="16" t="inlineStr"/>
+      <c r="D150" s="16" t="inlineStr"/>
+      <c r="E150" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F150" s="16" t="n">
+        <v>440.4</v>
+      </c>
+      <c r="G150" s="16" t="n">
+        <v>1.8821</v>
+      </c>
+      <c r="H150" s="16" t="n"/>
     </row>
     <row r="151">
-      <c r="A151" s="15" t="n"/>
-      <c r="B151" s="15" t="n"/>
-      <c r="C151" s="15" t="n"/>
-      <c r="D151" s="15" t="n"/>
-      <c r="E151" s="15" t="n"/>
-      <c r="F151" s="15" t="n"/>
-      <c r="G151" s="15" t="n"/>
-      <c r="H151" s="15" t="n"/>
+      <c r="A151" s="16" t="inlineStr">
+        <is>
+          <t>84.</t>
+        </is>
+      </c>
+      <c r="B151" s="16" t="inlineStr">
+        <is>
+          <t>Francis Edrian Bien Cellona</t>
+        </is>
+      </c>
+      <c r="C151" s="16" t="inlineStr"/>
+      <c r="D151" s="16" t="inlineStr"/>
+      <c r="E151" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F151" s="16" t="n">
+        <v>456.6</v>
+      </c>
+      <c r="G151" s="16" t="n">
+        <v>1.9513</v>
+      </c>
+      <c r="H151" s="16" t="n"/>
     </row>
     <row r="152">
-      <c r="A152" s="15" t="n"/>
-      <c r="B152" s="15" t="n"/>
-      <c r="C152" s="15" t="n"/>
-      <c r="D152" s="15" t="n"/>
-      <c r="E152" s="15" t="n"/>
-      <c r="F152" s="15" t="n"/>
-      <c r="G152" s="15" t="n"/>
-      <c r="H152" s="15" t="n"/>
+      <c r="A152" s="16" t="inlineStr">
+        <is>
+          <t>85.</t>
+        </is>
+      </c>
+      <c r="B152" s="16" t="inlineStr">
+        <is>
+          <t>Johann Patrick Beli Dela Cruz</t>
+        </is>
+      </c>
+      <c r="C152" s="16" t="inlineStr"/>
+      <c r="D152" s="16" t="inlineStr"/>
+      <c r="E152" s="16" t="n"/>
+      <c r="F152" s="16" t="n"/>
+      <c r="G152" s="16" t="n"/>
+      <c r="H152" s="16" t="n"/>
     </row>
     <row r="153">
-      <c r="A153" s="15" t="n"/>
-      <c r="B153" s="15" t="n"/>
-      <c r="C153" s="15" t="n"/>
-      <c r="D153" s="15" t="n"/>
-      <c r="E153" s="15" t="n"/>
-      <c r="F153" s="15" t="n"/>
-      <c r="G153" s="15" t="n"/>
-      <c r="H153" s="15" t="n"/>
+      <c r="A153" s="16" t="n"/>
+      <c r="B153" s="16" t="n"/>
+      <c r="C153" s="16" t="n"/>
+      <c r="D153" s="16" t="n"/>
+      <c r="E153" s="16" t="n"/>
+      <c r="F153" s="16" t="n"/>
+      <c r="G153" s="16" t="n"/>
+      <c r="H153" s="16" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="45">
@@ -2269,7 +3898,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="16" t="inlineStr">
+      <c r="A16" s="18" t="inlineStr">
         <is>
           <t xml:space="preserve">Herewith are the Official List of Candidates for Graduation with Honors under the different degree </t>
         </is>
@@ -2327,16 +3956,16 @@
       <c r="F20" s="9" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="17" t="inlineStr">
+      <c r="A21" s="19" t="inlineStr">
         <is>
           <t>MALE</t>
         </is>
       </c>
-      <c r="B21" s="18" t="n"/>
-      <c r="C21" s="18" t="n"/>
-      <c r="D21" s="18" t="n"/>
-      <c r="E21" s="18" t="n"/>
-      <c r="F21" s="19" t="n"/>
+      <c r="B21" s="20" t="n"/>
+      <c r="C21" s="20" t="n"/>
+      <c r="D21" s="20" t="n"/>
+      <c r="E21" s="20" t="n"/>
+      <c r="F21" s="21" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="10" t="n">
@@ -2353,7 +3982,7 @@
       <c r="D22" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E22" s="17" t="n">
+      <c r="E22" s="19" t="n">
         <v>1.7705</v>
       </c>
       <c r="F22" s="10" t="n"/>
@@ -2373,7 +4002,7 @@
       <c r="D23" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E23" s="20" t="n">
+      <c r="E23" s="11" t="n">
         <v>1.7449</v>
       </c>
       <c r="F23" s="10" t="inlineStr">
@@ -2397,7 +4026,7 @@
       <c r="D24" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E24" s="17" t="n">
+      <c r="E24" s="19" t="n">
         <v>1.9513</v>
       </c>
       <c r="F24" s="10" t="n"/>
@@ -2431,7 +4060,7 @@
       <c r="D26" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E26" s="20" t="n">
+      <c r="E26" s="11" t="n">
         <v>1.7209</v>
       </c>
       <c r="F26" s="10" t="inlineStr">
@@ -2455,7 +4084,7 @@
       <c r="D27" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E27" s="20" t="n">
+      <c r="E27" s="11" t="n">
         <v>1.5675</v>
       </c>
       <c r="F27" s="10" t="inlineStr">
@@ -2479,7 +4108,7 @@
       <c r="D28" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E28" s="17" t="n">
+      <c r="E28" s="19" t="n">
         <v>1.7953</v>
       </c>
       <c r="F28" s="10" t="n"/>
@@ -2499,7 +4128,7 @@
       <c r="D29" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E29" s="20" t="n">
+      <c r="E29" s="11" t="n">
         <v>1.4962</v>
       </c>
       <c r="F29" s="10" t="inlineStr">
@@ -2523,7 +4152,7 @@
       <c r="D30" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E30" s="17" t="n">
+      <c r="E30" s="19" t="n">
         <v>1.8226</v>
       </c>
       <c r="F30" s="10" t="n"/>
@@ -2543,7 +4172,7 @@
       <c r="D31" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E31" s="17" t="n">
+      <c r="E31" s="19" t="n">
         <v>1.7594</v>
       </c>
       <c r="F31" s="10" t="n"/>
@@ -2563,7 +4192,7 @@
       <c r="D32" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E32" s="17" t="n">
+      <c r="E32" s="19" t="n">
         <v>1.8474</v>
       </c>
       <c r="F32" s="10" t="n"/>
@@ -2583,7 +4212,7 @@
       <c r="D33" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E33" s="20" t="n">
+      <c r="E33" s="11" t="n">
         <v>1.5368</v>
       </c>
       <c r="F33" s="10" t="inlineStr">
@@ -2607,7 +4236,7 @@
       <c r="D34" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E34" s="20" t="n">
+      <c r="E34" s="11" t="n">
         <v>1.7175</v>
       </c>
       <c r="F34" s="10" t="inlineStr">
@@ -2631,7 +4260,7 @@
       <c r="D35" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E35" s="20" t="n">
+      <c r="E35" s="11" t="n">
         <v>1.6312</v>
       </c>
       <c r="F35" s="10" t="inlineStr">
@@ -2655,7 +4284,7 @@
       <c r="D36" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E36" s="17" t="n">
+      <c r="E36" s="19" t="n">
         <v>1.8453</v>
       </c>
       <c r="F36" s="10" t="n"/>
@@ -2675,7 +4304,7 @@
       <c r="D37" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E37" s="20" t="n">
+      <c r="E37" s="11" t="n">
         <v>1.4509</v>
       </c>
       <c r="F37" s="10" t="inlineStr">
@@ -2699,7 +4328,7 @@
       <c r="D38" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E38" s="20" t="n">
+      <c r="E38" s="11" t="n">
         <v>1.5047</v>
       </c>
       <c r="F38" s="10" t="inlineStr">
@@ -2723,7 +4352,7 @@
       <c r="D39" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E39" s="20" t="n">
+      <c r="E39" s="11" t="n">
         <v>1.5184</v>
       </c>
       <c r="F39" s="10" t="inlineStr">
@@ -2747,7 +4376,7 @@
       <c r="D40" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E40" s="20" t="n">
+      <c r="E40" s="11" t="n">
         <v>1.6171</v>
       </c>
       <c r="F40" s="10" t="inlineStr">
@@ -2771,7 +4400,7 @@
       <c r="D41" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E41" s="20" t="n">
+      <c r="E41" s="11" t="n">
         <v>1.7179</v>
       </c>
       <c r="F41" s="10" t="inlineStr">
@@ -2781,16 +4410,16 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="17" t="inlineStr">
+      <c r="A42" s="19" t="inlineStr">
         <is>
           <t>FEMALE</t>
         </is>
       </c>
-      <c r="B42" s="18" t="n"/>
-      <c r="C42" s="18" t="n"/>
-      <c r="D42" s="18" t="n"/>
-      <c r="E42" s="18" t="n"/>
-      <c r="F42" s="19" t="n"/>
+      <c r="B42" s="20" t="n"/>
+      <c r="C42" s="20" t="n"/>
+      <c r="D42" s="20" t="n"/>
+      <c r="E42" s="20" t="n"/>
+      <c r="F42" s="21" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="10" t="n">
@@ -2807,7 +4436,7 @@
       <c r="D43" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E43" s="20" t="n">
+      <c r="E43" s="11" t="n">
         <v>1.6188</v>
       </c>
       <c r="F43" s="10" t="inlineStr">
@@ -2831,7 +4460,7 @@
       <c r="D44" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E44" s="17" t="n">
+      <c r="E44" s="19" t="n">
         <v>1.7987</v>
       </c>
       <c r="F44" s="10" t="n"/>
@@ -2851,7 +4480,7 @@
       <c r="D45" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E45" s="20" t="n">
+      <c r="E45" s="11" t="n">
         <v>1.6372</v>
       </c>
       <c r="F45" s="10" t="inlineStr">
@@ -2875,7 +4504,7 @@
       <c r="D46" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E46" s="20" t="n">
+      <c r="E46" s="11" t="n">
         <v>1.6709</v>
       </c>
       <c r="F46" s="10" t="inlineStr">
@@ -2899,7 +4528,7 @@
       <c r="D47" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E47" s="20" t="n">
+      <c r="E47" s="11" t="n">
         <v>1.6179</v>
       </c>
       <c r="F47" s="10" t="inlineStr">
@@ -2923,7 +4552,7 @@
       <c r="D48" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E48" s="17" t="n">
+      <c r="E48" s="19" t="n">
         <v>1.7949</v>
       </c>
       <c r="F48" s="10" t="n"/>
@@ -2943,7 +4572,7 @@
       <c r="D49" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E49" s="20" t="n">
+      <c r="E49" s="11" t="n">
         <v>1.7303</v>
       </c>
       <c r="F49" s="10" t="inlineStr">
@@ -2967,7 +4596,7 @@
       <c r="D50" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E50" s="20" t="n">
+      <c r="E50" s="11" t="n">
         <v>1.7154</v>
       </c>
       <c r="F50" s="10" t="inlineStr">
@@ -2991,7 +4620,7 @@
       <c r="D51" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E51" s="20" t="n">
+      <c r="E51" s="11" t="n">
         <v>1.6799</v>
       </c>
       <c r="F51" s="10" t="inlineStr">
@@ -3015,7 +4644,7 @@
       <c r="D52" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E52" s="20" t="n">
+      <c r="E52" s="11" t="n">
         <v>1.7483</v>
       </c>
       <c r="F52" s="10" t="inlineStr">
@@ -3039,7 +4668,7 @@
       <c r="D53" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E53" s="20" t="n">
+      <c r="E53" s="11" t="n">
         <v>1.7107</v>
       </c>
       <c r="F53" s="10" t="inlineStr">
@@ -3063,7 +4692,7 @@
       <c r="D54" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E54" s="17" t="n">
+      <c r="E54" s="19" t="n">
         <v>1.8821</v>
       </c>
       <c r="F54" s="10" t="n"/>
@@ -3083,7 +4712,7 @@
       <c r="D55" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E55" s="17" t="n">
+      <c r="E55" s="19" t="n">
         <v>1.7859</v>
       </c>
       <c r="F55" s="10" t="n"/>
@@ -3103,7 +4732,7 @@
       <c r="D56" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E56" s="17" t="n">
+      <c r="E56" s="19" t="n">
         <v>1.7607</v>
       </c>
       <c r="F56" s="10" t="n"/>
@@ -3123,7 +4752,7 @@
       <c r="D57" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E57" s="20" t="n">
+      <c r="E57" s="11" t="n">
         <v>1.6175</v>
       </c>
       <c r="F57" s="10" t="inlineStr">
@@ -3147,7 +4776,7 @@
       <c r="D58" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E58" s="20" t="n">
+      <c r="E58" s="11" t="n">
         <v>1.6556</v>
       </c>
       <c r="F58" s="10" t="inlineStr">
@@ -3171,7 +4800,7 @@
       <c r="D59" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E59" s="20" t="n">
+      <c r="E59" s="11" t="n">
         <v>1.7038</v>
       </c>
       <c r="F59" s="10" t="inlineStr">
@@ -3195,7 +4824,7 @@
       <c r="D60" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E60" s="17" t="n">
+      <c r="E60" s="19" t="n">
         <v>1.8402</v>
       </c>
       <c r="F60" s="10" t="n"/>
@@ -3215,7 +4844,7 @@
       <c r="D61" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E61" s="20" t="n">
+      <c r="E61" s="11" t="n">
         <v>1.7175</v>
       </c>
       <c r="F61" s="10" t="inlineStr">
@@ -3239,7 +4868,7 @@
       <c r="D62" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E62" s="20" t="n">
+      <c r="E62" s="11" t="n">
         <v>1.6457</v>
       </c>
       <c r="F62" s="10" t="inlineStr">
@@ -3263,7 +4892,7 @@
       <c r="D63" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E63" s="17" t="n">
+      <c r="E63" s="19" t="n">
         <v>1.8769</v>
       </c>
       <c r="F63" s="10" t="n"/>
@@ -3283,7 +4912,7 @@
       <c r="D64" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E64" s="17" t="n">
+      <c r="E64" s="19" t="n">
         <v>1.8385</v>
       </c>
       <c r="F64" s="10" t="n"/>
@@ -3303,7 +4932,7 @@
       <c r="D65" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E65" s="20" t="n">
+      <c r="E65" s="11" t="n">
         <v>1.4141</v>
       </c>
       <c r="F65" s="10" t="inlineStr">
@@ -3327,30 +4956,30 @@
       <c r="D66" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E66" s="17" t="n">
+      <c r="E66" s="19" t="n">
         <v>1.8043</v>
       </c>
       <c r="F66" s="10" t="n"/>
     </row>
     <row r="67">
-      <c r="A67" s="21" t="n">
+      <c r="A67" s="22" t="n">
         <v>25</v>
       </c>
-      <c r="B67" s="21" t="inlineStr">
+      <c r="B67" s="22" t="inlineStr">
         <is>
           <t>Joanne Karla Caldit Consuelo</t>
         </is>
       </c>
-      <c r="C67" s="21" t="n">
+      <c r="C67" s="22" t="n">
         <v>363</v>
       </c>
-      <c r="D67" s="21" t="n">
+      <c r="D67" s="22" t="n">
         <v>216</v>
       </c>
-      <c r="E67" s="20" t="n">
+      <c r="E67" s="11" t="n">
         <v>1.6806</v>
       </c>
-      <c r="F67" s="21" t="n"/>
+      <c r="F67" s="22" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="10" t="n">
@@ -3367,7 +4996,7 @@
       <c r="D68" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E68" s="17" t="n">
+      <c r="E68" s="19" t="n">
         <v>1.7906</v>
       </c>
       <c r="F68" s="10" t="n"/>
@@ -3387,7 +5016,7 @@
       <c r="D69" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E69" s="20" t="n">
+      <c r="E69" s="11" t="n">
         <v>1.7141</v>
       </c>
       <c r="F69" s="10" t="inlineStr">
@@ -3411,7 +5040,7 @@
       <c r="D70" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E70" s="20" t="n">
+      <c r="E70" s="11" t="n">
         <v>1.6953</v>
       </c>
       <c r="F70" s="10" t="inlineStr">
@@ -3435,7 +5064,7 @@
       <c r="D71" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E71" s="17" t="n">
+      <c r="E71" s="19" t="n">
         <v>1.8188</v>
       </c>
       <c r="F71" s="10" t="n"/>
@@ -3455,7 +5084,7 @@
       <c r="D72" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E72" s="20" t="n">
+      <c r="E72" s="11" t="n">
         <v>1.7064</v>
       </c>
       <c r="F72" s="10" t="inlineStr">
@@ -3479,7 +5108,7 @@
       <c r="D73" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E73" s="20" t="n">
+      <c r="E73" s="11" t="n">
         <v>1.656</v>
       </c>
       <c r="F73" s="10" t="inlineStr">
@@ -3503,7 +5132,7 @@
       <c r="D74" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E74" s="20" t="n">
+      <c r="E74" s="11" t="n">
         <v>1.715</v>
       </c>
       <c r="F74" s="10" t="inlineStr">
@@ -3527,7 +5156,7 @@
       <c r="D75" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E75" s="20" t="n">
+      <c r="E75" s="11" t="n">
         <v>1.6846</v>
       </c>
       <c r="F75" s="10" t="inlineStr">
@@ -3551,7 +5180,7 @@
       <c r="D76" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E76" s="20" t="n">
+      <c r="E76" s="11" t="n">
         <v>1.6671</v>
       </c>
       <c r="F76" s="10" t="inlineStr">
@@ -3575,7 +5204,7 @@
       <c r="D77" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E77" s="17" t="n">
+      <c r="E77" s="19" t="n">
         <v>1.7628</v>
       </c>
       <c r="F77" s="10" t="n"/>
@@ -3595,7 +5224,7 @@
       <c r="D78" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E78" s="20" t="n">
+      <c r="E78" s="11" t="n">
         <v>1.6171</v>
       </c>
       <c r="F78" s="10" t="inlineStr">
@@ -3619,7 +5248,7 @@
       <c r="D79" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E79" s="20" t="n">
+      <c r="E79" s="11" t="n">
         <v>1.7363</v>
       </c>
       <c r="F79" s="10" t="inlineStr">
@@ -3643,7 +5272,7 @@
       <c r="D80" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E80" s="17" t="n">
+      <c r="E80" s="19" t="n">
         <v>1.8073</v>
       </c>
       <c r="F80" s="10" t="n"/>
@@ -3663,7 +5292,7 @@
       <c r="D81" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E81" s="17" t="n">
+      <c r="E81" s="19" t="n">
         <v>1.7872</v>
       </c>
       <c r="F81" s="10" t="n"/>
@@ -3683,7 +5312,7 @@
       <c r="D82" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E82" s="20" t="n">
+      <c r="E82" s="11" t="n">
         <v>1.7406</v>
       </c>
       <c r="F82" s="10" t="inlineStr">
@@ -3707,7 +5336,7 @@
       <c r="D83" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E83" s="20" t="n">
+      <c r="E83" s="11" t="n">
         <v>1.5479</v>
       </c>
       <c r="F83" s="10" t="inlineStr">
@@ -3731,7 +5360,7 @@
       <c r="D84" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E84" s="20" t="n">
+      <c r="E84" s="11" t="n">
         <v>1.6722</v>
       </c>
       <c r="F84" s="10" t="inlineStr">
@@ -3755,7 +5384,7 @@
       <c r="D85" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E85" s="17" t="n">
+      <c r="E85" s="19" t="n">
         <v>1.8256</v>
       </c>
       <c r="F85" s="10" t="n"/>
@@ -3775,7 +5404,7 @@
       <c r="D86" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E86" s="20" t="n">
+      <c r="E86" s="11" t="n">
         <v>1.6902</v>
       </c>
       <c r="F86" s="10" t="inlineStr">
@@ -3799,7 +5428,7 @@
       <c r="D87" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E87" s="20" t="n">
+      <c r="E87" s="11" t="n">
         <v>1.747</v>
       </c>
       <c r="F87" s="10" t="inlineStr">
@@ -3823,7 +5452,7 @@
       <c r="D88" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E88" s="20" t="n">
+      <c r="E88" s="11" t="n">
         <v>1.6991</v>
       </c>
       <c r="F88" s="10" t="inlineStr">
@@ -3847,7 +5476,7 @@
       <c r="D89" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E89" s="20" t="n">
+      <c r="E89" s="11" t="n">
         <v>1.7419</v>
       </c>
       <c r="F89" s="10" t="inlineStr">
@@ -3871,7 +5500,7 @@
       <c r="D90" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E90" s="20" t="n">
+      <c r="E90" s="11" t="n">
         <v>1.7423</v>
       </c>
       <c r="F90" s="10" t="inlineStr">
@@ -3895,7 +5524,7 @@
       <c r="D91" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E91" s="20" t="n">
+      <c r="E91" s="11" t="n">
         <v>1.7338</v>
       </c>
       <c r="F91" s="10" t="inlineStr">
@@ -3919,7 +5548,7 @@
       <c r="D92" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E92" s="20" t="n">
+      <c r="E92" s="11" t="n">
         <v>1.691</v>
       </c>
       <c r="F92" s="10" t="inlineStr">
@@ -3943,7 +5572,7 @@
       <c r="D93" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E93" s="20" t="n">
+      <c r="E93" s="11" t="n">
         <v>1.7021</v>
       </c>
       <c r="F93" s="10" t="inlineStr">
@@ -3967,7 +5596,7 @@
       <c r="D94" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E94" s="20" t="n">
+      <c r="E94" s="11" t="n">
         <v>1.7175</v>
       </c>
       <c r="F94" s="10" t="inlineStr">
@@ -3991,7 +5620,7 @@
       <c r="D95" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E95" s="17" t="n">
+      <c r="E95" s="19" t="n">
         <v>1.8526</v>
       </c>
       <c r="F95" s="10" t="n"/>
@@ -4011,7 +5640,7 @@
       <c r="D96" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E96" s="20" t="n">
+      <c r="E96" s="11" t="n">
         <v>1.7201</v>
       </c>
       <c r="F96" s="10" t="inlineStr">
@@ -4035,7 +5664,7 @@
       <c r="D97" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E97" s="20" t="n">
+      <c r="E97" s="11" t="n">
         <v>1.653</v>
       </c>
       <c r="F97" s="10" t="inlineStr">
@@ -4059,7 +5688,7 @@
       <c r="D98" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E98" s="20" t="n">
+      <c r="E98" s="11" t="n">
         <v>1.6731</v>
       </c>
       <c r="F98" s="10" t="inlineStr">
@@ -4083,7 +5712,7 @@
       <c r="D99" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E99" s="20" t="n">
+      <c r="E99" s="11" t="n">
         <v>1.6457</v>
       </c>
       <c r="F99" s="10" t="inlineStr">
@@ -4107,7 +5736,7 @@
       <c r="D100" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E100" s="17" t="n">
+      <c r="E100" s="19" t="n">
         <v>1.7641</v>
       </c>
       <c r="F100" s="10" t="n"/>
@@ -4127,7 +5756,7 @@
       <c r="D101" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E101" s="20" t="n">
+      <c r="E101" s="11" t="n">
         <v>1.7444</v>
       </c>
       <c r="F101" s="10" t="inlineStr">
@@ -4151,7 +5780,7 @@
       <c r="D102" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E102" s="17" t="n">
+      <c r="E102" s="19" t="n">
         <v>1.7833</v>
       </c>
       <c r="F102" s="10" t="n"/>
@@ -4171,7 +5800,7 @@
       <c r="D103" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E103" s="20" t="n">
+      <c r="E103" s="11" t="n">
         <v>1.7329</v>
       </c>
       <c r="F103" s="10" t="inlineStr">
@@ -4195,7 +5824,7 @@
       <c r="D104" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E104" s="20" t="n">
+      <c r="E104" s="11" t="n">
         <v>1.635</v>
       </c>
       <c r="F104" s="10" t="inlineStr">
@@ -4219,7 +5848,7 @@
       <c r="D105" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E105" s="17" t="n">
+      <c r="E105" s="19" t="n">
         <v>1.8004</v>
       </c>
       <c r="F105" s="10" t="n"/>
@@ -4239,7 +5868,7 @@
       <c r="D106" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E106" s="20" t="n">
+      <c r="E106" s="11" t="n">
         <v>1.7321</v>
       </c>
       <c r="F106" s="10" t="inlineStr">
@@ -4263,7 +5892,7 @@
       <c r="D107" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E107" s="20" t="n">
+      <c r="E107" s="11" t="n">
         <v>1.5175</v>
       </c>
       <c r="F107" s="10" t="inlineStr">
@@ -4273,21 +5902,21 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="16" t="inlineStr">
+      <c r="A109" s="18" t="inlineStr">
         <is>
           <t>Note: Subject for verification/recommendation/approval by the University Evaluation/Review</t>
         </is>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="22" t="inlineStr">
+      <c r="A110" s="23" t="inlineStr">
         <is>
           <t>Committee on Honor Graduates</t>
         </is>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="16" t="inlineStr">
+      <c r="A112" s="18" t="inlineStr">
         <is>
           <t xml:space="preserve">Attached are the individual collegiate student's permanent record with the individual computation of </t>
         </is>
@@ -4308,83 +5937,83 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="23" t="inlineStr">
+      <c r="A116" s="24" t="inlineStr">
         <is>
           <t>COLLEGE/CAMPUS EVALUATION/REVIEW COMMITTEE</t>
         </is>
       </c>
     </row>
     <row r="118">
-      <c r="B118" s="23" t="inlineStr">
+      <c r="B118" s="24" t="inlineStr">
         <is>
           <t>Member N. Name</t>
         </is>
       </c>
-      <c r="F118" s="23" t="inlineStr">
+      <c r="F118" s="24" t="inlineStr">
         <is>
           <t>Member N. Name</t>
         </is>
       </c>
     </row>
     <row r="119">
-      <c r="B119" s="24" t="inlineStr">
+      <c r="B119" s="25" t="inlineStr">
         <is>
           <t>Member</t>
         </is>
       </c>
-      <c r="F119" s="24" t="inlineStr">
+      <c r="F119" s="25" t="inlineStr">
         <is>
           <t>Member</t>
         </is>
       </c>
     </row>
     <row r="122">
-      <c r="B122" s="23" t="inlineStr">
+      <c r="B122" s="24" t="inlineStr">
         <is>
           <t>Member N. Name</t>
         </is>
       </c>
-      <c r="F122" s="23" t="inlineStr">
+      <c r="F122" s="24" t="inlineStr">
         <is>
           <t>Member N. Name</t>
         </is>
       </c>
     </row>
     <row r="123">
-      <c r="B123" s="24" t="inlineStr">
+      <c r="B123" s="25" t="inlineStr">
         <is>
           <t>Member</t>
         </is>
       </c>
-      <c r="F123" s="24" t="inlineStr">
+      <c r="F123" s="25" t="inlineStr">
         <is>
           <t>Member</t>
         </is>
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="23" t="inlineStr">
+      <c r="A125" s="24" t="inlineStr">
         <is>
           <t>Co-chair N. Name</t>
         </is>
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="24" t="inlineStr">
+      <c r="A126" s="25" t="inlineStr">
         <is>
           <t>Co-Chairman</t>
         </is>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="23" t="inlineStr">
+      <c r="A128" s="24" t="inlineStr">
         <is>
           <t>Chairperson N. Name</t>
         </is>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="24" t="inlineStr">
+      <c r="A129" s="25" t="inlineStr">
         <is>
           <t>Chairperson</t>
         </is>

</xml_diff>

<commit_message>
rank sheet column width fix, th font fix
</commit_message>
<xml_diff>
--- a/static/Honors.xlsx
+++ b/static/Honors.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -44,6 +44,11 @@
       <b val="1"/>
       <color rgb="009d0008"/>
       <sz val="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="4">
@@ -167,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -184,12 +189,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -210,9 +215,18 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -603,12 +617,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="5" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="25" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="7" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="7" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="9" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="9" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="9" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -807,7 +823,7 @@
     <row r="21">
       <c r="A21" s="10" t="inlineStr">
         <is>
-          <t>1.</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B21" s="10" t="inlineStr">
@@ -839,7 +855,7 @@
     <row r="22">
       <c r="A22" s="10" t="inlineStr">
         <is>
-          <t>2.</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B22" s="10" t="inlineStr">
@@ -871,7 +887,7 @@
     <row r="23">
       <c r="A23" s="10" t="inlineStr">
         <is>
-          <t>3.</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B23" s="10" t="inlineStr">
@@ -903,7 +919,7 @@
     <row r="24">
       <c r="A24" s="10" t="inlineStr">
         <is>
-          <t>4.</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B24" s="10" t="inlineStr">
@@ -935,7 +951,7 @@
     <row r="25">
       <c r="A25" s="10" t="inlineStr">
         <is>
-          <t>5.</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B25" s="10" t="inlineStr">
@@ -967,7 +983,7 @@
     <row r="26">
       <c r="A26" s="10" t="inlineStr">
         <is>
-          <t>6.</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B26" s="10" t="inlineStr">
@@ -999,7 +1015,7 @@
     <row r="27">
       <c r="A27" s="10" t="inlineStr">
         <is>
-          <t>7.</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B27" s="10" t="inlineStr">
@@ -1031,7 +1047,7 @@
     <row r="28">
       <c r="A28" s="10" t="inlineStr">
         <is>
-          <t>8.</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B28" s="10" t="inlineStr">
@@ -1063,7 +1079,7 @@
     <row r="29">
       <c r="A29" s="10" t="inlineStr">
         <is>
-          <t>9.</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B29" s="10" t="inlineStr">
@@ -1095,7 +1111,7 @@
     <row r="30">
       <c r="A30" s="10" t="inlineStr">
         <is>
-          <t>10.</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B30" s="10" t="inlineStr">
@@ -1127,7 +1143,7 @@
     <row r="31">
       <c r="A31" s="10" t="inlineStr">
         <is>
-          <t>11.</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B31" s="10" t="inlineStr">
@@ -1159,7 +1175,7 @@
     <row r="32">
       <c r="A32" s="10" t="inlineStr">
         <is>
-          <t>12.</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B32" s="10" t="inlineStr">
@@ -1191,7 +1207,7 @@
     <row r="33">
       <c r="A33" s="10" t="inlineStr">
         <is>
-          <t>13.</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B33" s="10" t="inlineStr">
@@ -1223,7 +1239,7 @@
     <row r="34">
       <c r="A34" s="10" t="inlineStr">
         <is>
-          <t>14.</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B34" s="10" t="inlineStr">
@@ -1255,7 +1271,7 @@
     <row r="35">
       <c r="A35" s="10" t="inlineStr">
         <is>
-          <t>15.</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B35" s="10" t="inlineStr">
@@ -1287,7 +1303,7 @@
     <row r="36">
       <c r="A36" s="10" t="inlineStr">
         <is>
-          <t>16.</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B36" s="10" t="inlineStr">
@@ -1319,7 +1335,7 @@
     <row r="37">
       <c r="A37" s="10" t="inlineStr">
         <is>
-          <t>17.</t>
+          <t>17</t>
         </is>
       </c>
       <c r="B37" s="10" t="inlineStr">
@@ -1351,7 +1367,7 @@
     <row r="38">
       <c r="A38" s="10" t="inlineStr">
         <is>
-          <t>18.</t>
+          <t>18</t>
         </is>
       </c>
       <c r="B38" s="10" t="inlineStr">
@@ -1383,7 +1399,7 @@
     <row r="39">
       <c r="A39" s="10" t="inlineStr">
         <is>
-          <t>19.</t>
+          <t>19</t>
         </is>
       </c>
       <c r="B39" s="10" t="inlineStr">
@@ -1415,7 +1431,7 @@
     <row r="40">
       <c r="A40" s="10" t="inlineStr">
         <is>
-          <t>20.</t>
+          <t>20</t>
         </is>
       </c>
       <c r="B40" s="10" t="inlineStr">
@@ -1447,7 +1463,7 @@
     <row r="41">
       <c r="A41" s="10" t="inlineStr">
         <is>
-          <t>21.</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B41" s="10" t="inlineStr">
@@ -1479,7 +1495,7 @@
     <row r="42">
       <c r="A42" s="10" t="inlineStr">
         <is>
-          <t>22.</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B42" s="10" t="inlineStr">
@@ -1511,7 +1527,7 @@
     <row r="43">
       <c r="A43" s="10" t="inlineStr">
         <is>
-          <t>23.</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B43" s="10" t="inlineStr">
@@ -1543,7 +1559,7 @@
     <row r="44">
       <c r="A44" s="10" t="inlineStr">
         <is>
-          <t>24.</t>
+          <t>24</t>
         </is>
       </c>
       <c r="B44" s="10" t="inlineStr">
@@ -1575,7 +1591,7 @@
     <row r="45">
       <c r="A45" s="10" t="inlineStr">
         <is>
-          <t>25.</t>
+          <t>25</t>
         </is>
       </c>
       <c r="B45" s="10" t="inlineStr">
@@ -1607,7 +1623,7 @@
     <row r="46">
       <c r="A46" s="10" t="inlineStr">
         <is>
-          <t>26.</t>
+          <t>26</t>
         </is>
       </c>
       <c r="B46" s="10" t="inlineStr">
@@ -1639,7 +1655,7 @@
     <row r="47">
       <c r="A47" s="10" t="inlineStr">
         <is>
-          <t>27.</t>
+          <t>27</t>
         </is>
       </c>
       <c r="B47" s="10" t="inlineStr">
@@ -1671,7 +1687,7 @@
     <row r="48">
       <c r="A48" s="10" t="inlineStr">
         <is>
-          <t>28.</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B48" s="10" t="inlineStr">
@@ -1703,7 +1719,7 @@
     <row r="49">
       <c r="A49" s="10" t="inlineStr">
         <is>
-          <t>29.</t>
+          <t>29</t>
         </is>
       </c>
       <c r="B49" s="10" t="inlineStr">
@@ -1735,7 +1751,7 @@
     <row r="50">
       <c r="A50" s="10" t="inlineStr">
         <is>
-          <t>30.</t>
+          <t>30</t>
         </is>
       </c>
       <c r="B50" s="10" t="inlineStr">
@@ -1767,7 +1783,7 @@
     <row r="51">
       <c r="A51" s="10" t="inlineStr">
         <is>
-          <t>31.</t>
+          <t>31</t>
         </is>
       </c>
       <c r="B51" s="10" t="inlineStr">
@@ -1799,7 +1815,7 @@
     <row r="52">
       <c r="A52" s="10" t="inlineStr">
         <is>
-          <t>32.</t>
+          <t>32</t>
         </is>
       </c>
       <c r="B52" s="10" t="inlineStr">
@@ -1831,7 +1847,7 @@
     <row r="53">
       <c r="A53" s="10" t="inlineStr">
         <is>
-          <t>33.</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B53" s="10" t="inlineStr">
@@ -1863,7 +1879,7 @@
     <row r="54">
       <c r="A54" s="10" t="inlineStr">
         <is>
-          <t>34.</t>
+          <t>34</t>
         </is>
       </c>
       <c r="B54" s="10" t="inlineStr">
@@ -1895,7 +1911,7 @@
     <row r="55">
       <c r="A55" s="10" t="inlineStr">
         <is>
-          <t>35.</t>
+          <t>35</t>
         </is>
       </c>
       <c r="B55" s="10" t="inlineStr">
@@ -1927,7 +1943,7 @@
     <row r="56">
       <c r="A56" s="10" t="inlineStr">
         <is>
-          <t>36.</t>
+          <t>36</t>
         </is>
       </c>
       <c r="B56" s="10" t="inlineStr">
@@ -1959,7 +1975,7 @@
     <row r="57">
       <c r="A57" s="10" t="inlineStr">
         <is>
-          <t>37.</t>
+          <t>37</t>
         </is>
       </c>
       <c r="B57" s="10" t="inlineStr">
@@ -1991,7 +2007,7 @@
     <row r="58">
       <c r="A58" s="10" t="inlineStr">
         <is>
-          <t>38.</t>
+          <t>38</t>
         </is>
       </c>
       <c r="B58" s="10" t="inlineStr">
@@ -2023,7 +2039,7 @@
     <row r="59">
       <c r="A59" s="10" t="inlineStr">
         <is>
-          <t>39.</t>
+          <t>39</t>
         </is>
       </c>
       <c r="B59" s="10" t="inlineStr">
@@ -2055,7 +2071,7 @@
     <row r="60">
       <c r="A60" s="10" t="inlineStr">
         <is>
-          <t>40.</t>
+          <t>40</t>
         </is>
       </c>
       <c r="B60" s="10" t="inlineStr">
@@ -2087,7 +2103,7 @@
     <row r="61">
       <c r="A61" s="10" t="inlineStr">
         <is>
-          <t>41.</t>
+          <t>41</t>
         </is>
       </c>
       <c r="B61" s="10" t="inlineStr">
@@ -2119,7 +2135,7 @@
     <row r="62">
       <c r="A62" s="10" t="inlineStr">
         <is>
-          <t>42.</t>
+          <t>42</t>
         </is>
       </c>
       <c r="B62" s="10" t="inlineStr">
@@ -2151,7 +2167,7 @@
     <row r="63">
       <c r="A63" s="10" t="inlineStr">
         <is>
-          <t>43.</t>
+          <t>43</t>
         </is>
       </c>
       <c r="B63" s="10" t="inlineStr">
@@ -2183,7 +2199,7 @@
     <row r="64">
       <c r="A64" s="10" t="inlineStr">
         <is>
-          <t>44.</t>
+          <t>44</t>
         </is>
       </c>
       <c r="B64" s="10" t="inlineStr">
@@ -2215,7 +2231,7 @@
     <row r="65">
       <c r="A65" s="10" t="inlineStr">
         <is>
-          <t>45.</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B65" s="10" t="inlineStr">
@@ -2247,7 +2263,7 @@
     <row r="66">
       <c r="A66" s="10" t="inlineStr">
         <is>
-          <t>46.</t>
+          <t>46</t>
         </is>
       </c>
       <c r="B66" s="10" t="inlineStr">
@@ -2279,7 +2295,7 @@
     <row r="67">
       <c r="A67" s="10" t="inlineStr">
         <is>
-          <t>47.</t>
+          <t>47</t>
         </is>
       </c>
       <c r="B67" s="10" t="inlineStr">
@@ -2311,7 +2327,7 @@
     <row r="68">
       <c r="A68" s="10" t="inlineStr">
         <is>
-          <t>48.</t>
+          <t>48</t>
         </is>
       </c>
       <c r="B68" s="10" t="inlineStr">
@@ -2343,7 +2359,7 @@
     <row r="69">
       <c r="A69" s="10" t="inlineStr">
         <is>
-          <t>49.</t>
+          <t>49</t>
         </is>
       </c>
       <c r="B69" s="10" t="inlineStr">
@@ -2375,7 +2391,7 @@
     <row r="70">
       <c r="A70" s="10" t="inlineStr">
         <is>
-          <t>50.</t>
+          <t>50</t>
         </is>
       </c>
       <c r="B70" s="10" t="inlineStr">
@@ -2407,7 +2423,7 @@
     <row r="71">
       <c r="A71" s="10" t="inlineStr">
         <is>
-          <t>51.</t>
+          <t>51</t>
         </is>
       </c>
       <c r="B71" s="10" t="inlineStr">
@@ -2439,7 +2455,7 @@
     <row r="72">
       <c r="A72" s="10" t="inlineStr">
         <is>
-          <t>52.</t>
+          <t>52</t>
         </is>
       </c>
       <c r="B72" s="10" t="inlineStr">
@@ -2471,7 +2487,7 @@
     <row r="73">
       <c r="A73" s="10" t="inlineStr">
         <is>
-          <t>53.</t>
+          <t>53</t>
         </is>
       </c>
       <c r="B73" s="10" t="inlineStr">
@@ -2503,7 +2519,7 @@
     <row r="74">
       <c r="A74" s="10" t="inlineStr">
         <is>
-          <t>54.</t>
+          <t>54</t>
         </is>
       </c>
       <c r="B74" s="10" t="inlineStr">
@@ -2535,7 +2551,7 @@
     <row r="75">
       <c r="A75" s="10" t="inlineStr">
         <is>
-          <t>55.</t>
+          <t>55</t>
         </is>
       </c>
       <c r="B75" s="10" t="inlineStr">
@@ -2567,7 +2583,7 @@
     <row r="76">
       <c r="A76" s="10" t="inlineStr">
         <is>
-          <t>56.</t>
+          <t>56</t>
         </is>
       </c>
       <c r="B76" s="10" t="inlineStr">
@@ -2599,7 +2615,7 @@
     <row r="77">
       <c r="A77" s="10" t="inlineStr">
         <is>
-          <t>57.</t>
+          <t>57</t>
         </is>
       </c>
       <c r="B77" s="10" t="inlineStr">
@@ -3068,7 +3084,7 @@
     <row r="126">
       <c r="A126" s="16" t="inlineStr">
         <is>
-          <t>58.</t>
+          <t>58</t>
         </is>
       </c>
       <c r="B126" s="16" t="inlineStr">
@@ -3092,7 +3108,7 @@
     <row r="127">
       <c r="A127" s="16" t="inlineStr">
         <is>
-          <t>59.</t>
+          <t>59</t>
         </is>
       </c>
       <c r="B127" s="16" t="inlineStr">
@@ -3116,7 +3132,7 @@
     <row r="128">
       <c r="A128" s="16" t="inlineStr">
         <is>
-          <t>60.</t>
+          <t>60</t>
         </is>
       </c>
       <c r="B128" s="16" t="inlineStr">
@@ -3140,7 +3156,7 @@
     <row r="129">
       <c r="A129" s="16" t="inlineStr">
         <is>
-          <t>61.</t>
+          <t>61</t>
         </is>
       </c>
       <c r="B129" s="16" t="inlineStr">
@@ -3164,12 +3180,12 @@
     <row r="130">
       <c r="A130" s="16" t="inlineStr">
         <is>
-          <t>63.</t>
+          <t>62</t>
         </is>
       </c>
       <c r="B130" s="16" t="inlineStr">
         <is>
-          <t>Alizza May Cantillo Salando</t>
+          <t>Diana Alcaldeza Relorcasa</t>
         </is>
       </c>
       <c r="C130" s="16" t="inlineStr"/>
@@ -3178,22 +3194,22 @@
         <v>234</v>
       </c>
       <c r="F130" s="16" t="n">
-        <v>417.3</v>
+        <v>412.8</v>
       </c>
       <c r="G130" s="16" t="n">
-        <v>1.7833</v>
+        <v>1.7641</v>
       </c>
       <c r="H130" s="16" t="n"/>
     </row>
     <row r="131">
       <c r="A131" s="16" t="inlineStr">
         <is>
-          <t>64.</t>
+          <t>63</t>
         </is>
       </c>
       <c r="B131" s="16" t="inlineStr">
         <is>
-          <t>Merari Deborah Falabi Catorce</t>
+          <t>Alizza May Cantillo Salando</t>
         </is>
       </c>
       <c r="C131" s="16" t="inlineStr"/>
@@ -3202,22 +3218,22 @@
         <v>234</v>
       </c>
       <c r="F131" s="16" t="n">
-        <v>422.2</v>
+        <v>417.3</v>
       </c>
       <c r="G131" s="16" t="n">
-        <v>1.8043</v>
+        <v>1.7833</v>
       </c>
       <c r="H131" s="16" t="n"/>
     </row>
     <row r="132">
       <c r="A132" s="16" t="inlineStr">
         <is>
-          <t>65.</t>
+          <t>64</t>
         </is>
       </c>
       <c r="B132" s="16" t="inlineStr">
         <is>
-          <t>Carla Jae Bitancur Barela</t>
+          <t>Merari Deborah Falabi Catorce</t>
         </is>
       </c>
       <c r="C132" s="16" t="inlineStr"/>
@@ -3226,22 +3242,22 @@
         <v>234</v>
       </c>
       <c r="F132" s="16" t="n">
-        <v>417.9</v>
+        <v>422.2</v>
       </c>
       <c r="G132" s="16" t="n">
-        <v>1.7859</v>
+        <v>1.8043</v>
       </c>
       <c r="H132" s="16" t="n"/>
     </row>
     <row r="133">
       <c r="A133" s="16" t="inlineStr">
         <is>
-          <t>66.</t>
+          <t>65</t>
         </is>
       </c>
       <c r="B133" s="16" t="inlineStr">
         <is>
-          <t>Stacy Kate Yuson Guerrero</t>
+          <t>Carla Jae Bitancur Barela</t>
         </is>
       </c>
       <c r="C133" s="16" t="inlineStr"/>
@@ -3250,22 +3266,22 @@
         <v>234</v>
       </c>
       <c r="F133" s="16" t="n">
-        <v>418.2</v>
+        <v>417.9</v>
       </c>
       <c r="G133" s="16" t="n">
-        <v>1.7872</v>
+        <v>1.7859</v>
       </c>
       <c r="H133" s="16" t="n"/>
     </row>
     <row r="134">
       <c r="A134" s="16" t="inlineStr">
         <is>
-          <t>67.</t>
+          <t>66</t>
         </is>
       </c>
       <c r="B134" s="16" t="inlineStr">
         <is>
-          <t>Justine Lorilla Daria</t>
+          <t>Stacy Kate Yuson Guerrero</t>
         </is>
       </c>
       <c r="C134" s="16" t="inlineStr"/>
@@ -3274,22 +3290,22 @@
         <v>234</v>
       </c>
       <c r="F134" s="16" t="n">
-        <v>419</v>
+        <v>418.2</v>
       </c>
       <c r="G134" s="16" t="n">
-        <v>1.7906</v>
+        <v>1.7872</v>
       </c>
       <c r="H134" s="16" t="n"/>
     </row>
     <row r="135">
       <c r="A135" s="16" t="inlineStr">
         <is>
-          <t>68.</t>
+          <t>67</t>
         </is>
       </c>
       <c r="B135" s="16" t="inlineStr">
         <is>
-          <t>Cianiah Kaela Mimay Apurado</t>
+          <t>Justine Lorilla Daria</t>
         </is>
       </c>
       <c r="C135" s="16" t="inlineStr"/>
@@ -3298,22 +3314,22 @@
         <v>234</v>
       </c>
       <c r="F135" s="16" t="n">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G135" s="16" t="n">
-        <v>1.7949</v>
+        <v>1.7906</v>
       </c>
       <c r="H135" s="16" t="n"/>
     </row>
     <row r="136">
       <c r="A136" s="16" t="inlineStr">
         <is>
-          <t>69.</t>
+          <t>68</t>
         </is>
       </c>
       <c r="B136" s="16" t="inlineStr">
         <is>
-          <t>Hans Christian Gonzales Imperial</t>
+          <t>Cianiah Kaela Mimay Apurado</t>
         </is>
       </c>
       <c r="C136" s="16" t="inlineStr"/>
@@ -3322,22 +3338,22 @@
         <v>234</v>
       </c>
       <c r="F136" s="16" t="n">
-        <v>420.1</v>
+        <v>420</v>
       </c>
       <c r="G136" s="16" t="n">
-        <v>1.7953</v>
+        <v>1.7949</v>
       </c>
       <c r="H136" s="16" t="n"/>
     </row>
     <row r="137">
       <c r="A137" s="16" t="inlineStr">
         <is>
-          <t>70.</t>
+          <t>69</t>
         </is>
       </c>
       <c r="B137" s="16" t="inlineStr">
         <is>
-          <t>Ma. Elaine Jacob Abejo</t>
+          <t>Hans Christian Gonzales Imperial</t>
         </is>
       </c>
       <c r="C137" s="16" t="inlineStr"/>
@@ -3346,22 +3362,22 @@
         <v>234</v>
       </c>
       <c r="F137" s="16" t="n">
-        <v>420.9</v>
+        <v>420.1</v>
       </c>
       <c r="G137" s="16" t="n">
-        <v>1.7987</v>
+        <v>1.7953</v>
       </c>
       <c r="H137" s="16" t="n"/>
     </row>
     <row r="138">
       <c r="A138" s="16" t="inlineStr">
         <is>
-          <t>71.</t>
+          <t>70</t>
         </is>
       </c>
       <c r="B138" s="16" t="inlineStr">
         <is>
-          <t>Ella Mae Patiño Suruiz</t>
+          <t>Ma. Elaine Jacob Abejo</t>
         </is>
       </c>
       <c r="C138" s="16" t="inlineStr"/>
@@ -3370,22 +3386,22 @@
         <v>234</v>
       </c>
       <c r="F138" s="16" t="n">
-        <v>421.3</v>
+        <v>420.9</v>
       </c>
       <c r="G138" s="16" t="n">
-        <v>1.8004</v>
+        <v>1.7987</v>
       </c>
       <c r="H138" s="16" t="n"/>
     </row>
     <row r="139">
       <c r="A139" s="16" t="inlineStr">
         <is>
-          <t>72.</t>
+          <t>71</t>
         </is>
       </c>
       <c r="B139" s="16" t="inlineStr">
         <is>
-          <t>China Araya Goyena</t>
+          <t>Ella Mae Patiño Suruiz</t>
         </is>
       </c>
       <c r="C139" s="16" t="inlineStr"/>
@@ -3394,70 +3410,70 @@
         <v>234</v>
       </c>
       <c r="F139" s="16" t="n">
+        <v>421.3</v>
+      </c>
+      <c r="G139" s="16" t="n">
+        <v>1.8004</v>
+      </c>
+      <c r="H139" s="16" t="n"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="16" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="B140" s="16" t="inlineStr">
+        <is>
+          <t>China Araya Goyena</t>
+        </is>
+      </c>
+      <c r="C140" s="16" t="inlineStr"/>
+      <c r="D140" s="16" t="inlineStr"/>
+      <c r="E140" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F140" s="16" t="n">
         <v>422.9</v>
       </c>
-      <c r="G139" s="16" t="n">
+      <c r="G140" s="16" t="n">
         <v>1.8073</v>
       </c>
-      <c r="H139" s="16" t="n"/>
-    </row>
-    <row r="140">
-      <c r="A140" s="17" t="inlineStr">
-        <is>
-          <t>73.</t>
-        </is>
-      </c>
-      <c r="B140" s="17" t="inlineStr">
+      <c r="H140" s="16" t="n"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="17" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B141" s="17" t="inlineStr">
         <is>
           <t>Joanne Karla Caldit Consuelo</t>
         </is>
       </c>
-      <c r="C140" s="17" t="inlineStr"/>
-      <c r="D140" s="17" t="inlineStr"/>
-      <c r="E140" s="17" t="n">
+      <c r="C141" s="17" t="inlineStr"/>
+      <c r="D141" s="17" t="inlineStr"/>
+      <c r="E141" s="17" t="n">
         <v>216</v>
       </c>
-      <c r="F140" s="17" t="n">
+      <c r="F141" s="17" t="n">
         <v>363</v>
       </c>
-      <c r="G140" s="11" t="n">
+      <c r="G141" s="11" t="n">
         <v>1.6806</v>
       </c>
-      <c r="H140" s="16" t="n"/>
-    </row>
-    <row r="141">
-      <c r="A141" s="16" t="inlineStr">
-        <is>
-          <t>74.</t>
-        </is>
-      </c>
-      <c r="B141" s="16" t="inlineStr">
-        <is>
-          <t>Christine Joy Belano Deona</t>
-        </is>
-      </c>
-      <c r="C141" s="16" t="inlineStr"/>
-      <c r="D141" s="16" t="inlineStr"/>
-      <c r="E141" s="16" t="n">
-        <v>234</v>
-      </c>
-      <c r="F141" s="16" t="n">
-        <v>425.6</v>
-      </c>
-      <c r="G141" s="16" t="n">
-        <v>1.8188</v>
-      </c>
-      <c r="H141" s="16" t="n"/>
+      <c r="H141" s="18" t="n"/>
     </row>
     <row r="142">
       <c r="A142" s="16" t="inlineStr">
         <is>
-          <t>75.</t>
+          <t>74</t>
         </is>
       </c>
       <c r="B142" s="16" t="inlineStr">
         <is>
-          <t>Ignacio Rodriguez Juaquera</t>
+          <t>Christine Joy Belano Deona</t>
         </is>
       </c>
       <c r="C142" s="16" t="inlineStr"/>
@@ -3466,22 +3482,22 @@
         <v>234</v>
       </c>
       <c r="F142" s="16" t="n">
-        <v>426.5</v>
+        <v>425.6</v>
       </c>
       <c r="G142" s="16" t="n">
-        <v>1.8226</v>
+        <v>1.8188</v>
       </c>
       <c r="H142" s="16" t="n"/>
     </row>
     <row r="143">
       <c r="A143" s="16" t="inlineStr">
         <is>
-          <t>76.</t>
+          <t>75</t>
         </is>
       </c>
       <c r="B143" s="16" t="inlineStr">
         <is>
-          <t>Vanessa Alemania Leosala</t>
+          <t>Ignacio Rodriguez Juaquera</t>
         </is>
       </c>
       <c r="C143" s="16" t="inlineStr"/>
@@ -3490,22 +3506,22 @@
         <v>234</v>
       </c>
       <c r="F143" s="16" t="n">
-        <v>427.2</v>
+        <v>426.5</v>
       </c>
       <c r="G143" s="16" t="n">
-        <v>1.8256</v>
+        <v>1.8226</v>
       </c>
       <c r="H143" s="16" t="n"/>
     </row>
     <row r="144">
       <c r="A144" s="16" t="inlineStr">
         <is>
-          <t>77.</t>
+          <t>76</t>
         </is>
       </c>
       <c r="B144" s="16" t="inlineStr">
         <is>
-          <t>Vanessa Mae Sia Cañete</t>
+          <t>Vanessa Alemania Leosala</t>
         </is>
       </c>
       <c r="C144" s="16" t="inlineStr"/>
@@ -3514,22 +3530,22 @@
         <v>234</v>
       </c>
       <c r="F144" s="16" t="n">
-        <v>430.2</v>
+        <v>427.2</v>
       </c>
       <c r="G144" s="16" t="n">
-        <v>1.8385</v>
+        <v>1.8256</v>
       </c>
       <c r="H144" s="16" t="n"/>
     </row>
     <row r="145">
       <c r="A145" s="16" t="inlineStr">
         <is>
-          <t>78.</t>
+          <t>77</t>
         </is>
       </c>
       <c r="B145" s="16" t="inlineStr">
         <is>
-          <t>Jazmin Shane Adlaon Calisin</t>
+          <t>Vanessa Mae Sia Cañete</t>
         </is>
       </c>
       <c r="C145" s="16" t="inlineStr"/>
@@ -3538,22 +3554,22 @@
         <v>234</v>
       </c>
       <c r="F145" s="16" t="n">
-        <v>430.6</v>
+        <v>430.2</v>
       </c>
       <c r="G145" s="16" t="n">
-        <v>1.8402</v>
+        <v>1.8385</v>
       </c>
       <c r="H145" s="16" t="n"/>
     </row>
     <row r="146">
       <c r="A146" s="16" t="inlineStr">
         <is>
-          <t>79.</t>
+          <t>78</t>
         </is>
       </c>
       <c r="B146" s="16" t="inlineStr">
         <is>
-          <t>Rev Neo Pavilando</t>
+          <t>Jazmin Shane Adlaon Calisin</t>
         </is>
       </c>
       <c r="C146" s="16" t="inlineStr"/>
@@ -3562,22 +3578,22 @@
         <v>234</v>
       </c>
       <c r="F146" s="16" t="n">
-        <v>431.8</v>
+        <v>430.6</v>
       </c>
       <c r="G146" s="16" t="n">
-        <v>1.8453</v>
+        <v>1.8402</v>
       </c>
       <c r="H146" s="16" t="n"/>
     </row>
     <row r="147">
       <c r="A147" s="16" t="inlineStr">
         <is>
-          <t>80.</t>
+          <t>79</t>
         </is>
       </c>
       <c r="B147" s="16" t="inlineStr">
         <is>
-          <t>Glenn Homer Polo Naparam</t>
+          <t>Rev Neo Pavilando</t>
         </is>
       </c>
       <c r="C147" s="16" t="inlineStr"/>
@@ -3586,22 +3602,22 @@
         <v>234</v>
       </c>
       <c r="F147" s="16" t="n">
-        <v>432.3</v>
+        <v>431.8</v>
       </c>
       <c r="G147" s="16" t="n">
-        <v>1.8474</v>
+        <v>1.8453</v>
       </c>
       <c r="H147" s="16" t="n"/>
     </row>
     <row r="148">
       <c r="A148" s="16" t="inlineStr">
         <is>
-          <t>81.</t>
+          <t>80</t>
         </is>
       </c>
       <c r="B148" s="16" t="inlineStr">
         <is>
-          <t>Christine Reocasa Paguio</t>
+          <t>Glenn Homer Polo Naparam</t>
         </is>
       </c>
       <c r="C148" s="16" t="inlineStr"/>
@@ -3610,22 +3626,22 @@
         <v>234</v>
       </c>
       <c r="F148" s="16" t="n">
-        <v>433.5</v>
+        <v>432.3</v>
       </c>
       <c r="G148" s="16" t="n">
-        <v>1.8526</v>
+        <v>1.8474</v>
       </c>
       <c r="H148" s="16" t="n"/>
     </row>
     <row r="149">
       <c r="A149" s="16" t="inlineStr">
         <is>
-          <t>82.</t>
+          <t>81</t>
         </is>
       </c>
       <c r="B149" s="16" t="inlineStr">
         <is>
-          <t>Renee Lynne Maquiñiana Camposano</t>
+          <t>Christine Reocasa Paguio</t>
         </is>
       </c>
       <c r="C149" s="16" t="inlineStr"/>
@@ -3634,22 +3650,22 @@
         <v>234</v>
       </c>
       <c r="F149" s="16" t="n">
-        <v>439.2</v>
+        <v>433.5</v>
       </c>
       <c r="G149" s="16" t="n">
-        <v>1.8769</v>
+        <v>1.8526</v>
       </c>
       <c r="H149" s="16" t="n"/>
     </row>
     <row r="150">
       <c r="A150" s="16" t="inlineStr">
         <is>
-          <t>83.</t>
+          <t>82</t>
         </is>
       </c>
       <c r="B150" s="16" t="inlineStr">
         <is>
-          <t>Pauline Anne Vibar Balilo</t>
+          <t>Renee Lynne Maquiñiana Camposano</t>
         </is>
       </c>
       <c r="C150" s="16" t="inlineStr"/>
@@ -3658,22 +3674,22 @@
         <v>234</v>
       </c>
       <c r="F150" s="16" t="n">
-        <v>440.4</v>
+        <v>439.2</v>
       </c>
       <c r="G150" s="16" t="n">
-        <v>1.8821</v>
+        <v>1.8769</v>
       </c>
       <c r="H150" s="16" t="n"/>
     </row>
     <row r="151">
       <c r="A151" s="16" t="inlineStr">
         <is>
-          <t>84.</t>
+          <t>83</t>
         </is>
       </c>
       <c r="B151" s="16" t="inlineStr">
         <is>
-          <t>Francis Edrian Bien Cellona</t>
+          <t>Pauline Anne Vibar Balilo</t>
         </is>
       </c>
       <c r="C151" s="16" t="inlineStr"/>
@@ -3682,36 +3698,50 @@
         <v>234</v>
       </c>
       <c r="F151" s="16" t="n">
-        <v>456.6</v>
+        <v>440.4</v>
       </c>
       <c r="G151" s="16" t="n">
-        <v>1.9513</v>
+        <v>1.8821</v>
       </c>
       <c r="H151" s="16" t="n"/>
     </row>
     <row r="152">
       <c r="A152" s="16" t="inlineStr">
         <is>
-          <t>85.</t>
+          <t>84</t>
         </is>
       </c>
       <c r="B152" s="16" t="inlineStr">
         <is>
-          <t>Johann Patrick Beli Dela Cruz</t>
+          <t>Francis Edrian Bien Cellona</t>
         </is>
       </c>
       <c r="C152" s="16" t="inlineStr"/>
       <c r="D152" s="16" t="inlineStr"/>
-      <c r="E152" s="16" t="n"/>
-      <c r="F152" s="16" t="n"/>
-      <c r="G152" s="16" t="n"/>
+      <c r="E152" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F152" s="16" t="n">
+        <v>456.6</v>
+      </c>
+      <c r="G152" s="16" t="n">
+        <v>1.9513</v>
+      </c>
       <c r="H152" s="16" t="n"/>
     </row>
     <row r="153">
-      <c r="A153" s="16" t="n"/>
-      <c r="B153" s="16" t="n"/>
-      <c r="C153" s="16" t="n"/>
-      <c r="D153" s="16" t="n"/>
+      <c r="A153" s="16" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="B153" s="16" t="inlineStr">
+        <is>
+          <t>Johann Patrick Beli Dela Cruz</t>
+        </is>
+      </c>
+      <c r="C153" s="16" t="inlineStr"/>
+      <c r="D153" s="16" t="inlineStr"/>
       <c r="E153" s="16" t="n"/>
       <c r="F153" s="16" t="n"/>
       <c r="G153" s="16" t="n"/>
@@ -3898,7 +3928,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="18" t="inlineStr">
+      <c r="A16" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">Herewith are the Official List of Candidates for Graduation with Honors under the different degree </t>
         </is>
@@ -3912,60 +3942,60 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="inlineStr">
+      <c r="A19" s="20" t="inlineStr">
         <is>
           <t>NO.</t>
         </is>
       </c>
-      <c r="B19" s="6" t="inlineStr">
+      <c r="B19" s="20" t="inlineStr">
         <is>
           <t>NAME</t>
         </is>
       </c>
-      <c r="C19" s="6" t="inlineStr">
+      <c r="C19" s="20" t="inlineStr">
         <is>
           <t>RATING</t>
         </is>
       </c>
-      <c r="D19" s="8" t="n"/>
-      <c r="E19" s="7" t="n"/>
-      <c r="F19" s="6" t="inlineStr">
+      <c r="D19" s="21" t="n"/>
+      <c r="E19" s="22" t="n"/>
+      <c r="F19" s="20" t="inlineStr">
         <is>
           <t>AWARD</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="9" t="n"/>
-      <c r="B20" s="9" t="n"/>
-      <c r="C20" s="6" t="inlineStr">
+      <c r="A20" s="23" t="n"/>
+      <c r="B20" s="23" t="n"/>
+      <c r="C20" s="20" t="inlineStr">
         <is>
           <t>Sum of Grades</t>
         </is>
       </c>
-      <c r="D20" s="6" t="inlineStr">
+      <c r="D20" s="20" t="inlineStr">
         <is>
           <t>Total Units</t>
         </is>
       </c>
-      <c r="E20" s="6" t="inlineStr">
+      <c r="E20" s="20" t="inlineStr">
         <is>
           <t>Final GWA</t>
         </is>
       </c>
-      <c r="F20" s="9" t="n"/>
+      <c r="F20" s="23" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="19" t="inlineStr">
+      <c r="A21" s="24" t="inlineStr">
         <is>
           <t>MALE</t>
         </is>
       </c>
-      <c r="B21" s="20" t="n"/>
-      <c r="C21" s="20" t="n"/>
-      <c r="D21" s="20" t="n"/>
-      <c r="E21" s="20" t="n"/>
-      <c r="F21" s="21" t="n"/>
+      <c r="B21" s="25" t="n"/>
+      <c r="C21" s="25" t="n"/>
+      <c r="D21" s="25" t="n"/>
+      <c r="E21" s="25" t="n"/>
+      <c r="F21" s="26" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="10" t="n">
@@ -3982,7 +4012,7 @@
       <c r="D22" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E22" s="19" t="n">
+      <c r="E22" s="24" t="n">
         <v>1.7705</v>
       </c>
       <c r="F22" s="10" t="n"/>
@@ -4026,7 +4056,7 @@
       <c r="D24" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E24" s="19" t="n">
+      <c r="E24" s="24" t="n">
         <v>1.9513</v>
       </c>
       <c r="F24" s="10" t="n"/>
@@ -4108,7 +4138,7 @@
       <c r="D28" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E28" s="19" t="n">
+      <c r="E28" s="24" t="n">
         <v>1.7953</v>
       </c>
       <c r="F28" s="10" t="n"/>
@@ -4152,7 +4182,7 @@
       <c r="D30" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E30" s="19" t="n">
+      <c r="E30" s="24" t="n">
         <v>1.8226</v>
       </c>
       <c r="F30" s="10" t="n"/>
@@ -4172,7 +4202,7 @@
       <c r="D31" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E31" s="19" t="n">
+      <c r="E31" s="24" t="n">
         <v>1.7594</v>
       </c>
       <c r="F31" s="10" t="n"/>
@@ -4192,7 +4222,7 @@
       <c r="D32" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E32" s="19" t="n">
+      <c r="E32" s="24" t="n">
         <v>1.8474</v>
       </c>
       <c r="F32" s="10" t="n"/>
@@ -4284,7 +4314,7 @@
       <c r="D36" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E36" s="19" t="n">
+      <c r="E36" s="24" t="n">
         <v>1.8453</v>
       </c>
       <c r="F36" s="10" t="n"/>
@@ -4410,16 +4440,16 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="19" t="inlineStr">
+      <c r="A42" s="24" t="inlineStr">
         <is>
           <t>FEMALE</t>
         </is>
       </c>
-      <c r="B42" s="20" t="n"/>
-      <c r="C42" s="20" t="n"/>
-      <c r="D42" s="20" t="n"/>
-      <c r="E42" s="20" t="n"/>
-      <c r="F42" s="21" t="n"/>
+      <c r="B42" s="25" t="n"/>
+      <c r="C42" s="25" t="n"/>
+      <c r="D42" s="25" t="n"/>
+      <c r="E42" s="25" t="n"/>
+      <c r="F42" s="26" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="10" t="n">
@@ -4460,7 +4490,7 @@
       <c r="D44" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E44" s="19" t="n">
+      <c r="E44" s="24" t="n">
         <v>1.7987</v>
       </c>
       <c r="F44" s="10" t="n"/>
@@ -4552,7 +4582,7 @@
       <c r="D48" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E48" s="19" t="n">
+      <c r="E48" s="24" t="n">
         <v>1.7949</v>
       </c>
       <c r="F48" s="10" t="n"/>
@@ -4692,7 +4722,7 @@
       <c r="D54" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E54" s="19" t="n">
+      <c r="E54" s="24" t="n">
         <v>1.8821</v>
       </c>
       <c r="F54" s="10" t="n"/>
@@ -4712,7 +4742,7 @@
       <c r="D55" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E55" s="19" t="n">
+      <c r="E55" s="24" t="n">
         <v>1.7859</v>
       </c>
       <c r="F55" s="10" t="n"/>
@@ -4732,7 +4762,7 @@
       <c r="D56" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E56" s="19" t="n">
+      <c r="E56" s="24" t="n">
         <v>1.7607</v>
       </c>
       <c r="F56" s="10" t="n"/>
@@ -4824,7 +4854,7 @@
       <c r="D60" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E60" s="19" t="n">
+      <c r="E60" s="24" t="n">
         <v>1.8402</v>
       </c>
       <c r="F60" s="10" t="n"/>
@@ -4892,7 +4922,7 @@
       <c r="D63" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E63" s="19" t="n">
+      <c r="E63" s="24" t="n">
         <v>1.8769</v>
       </c>
       <c r="F63" s="10" t="n"/>
@@ -4912,7 +4942,7 @@
       <c r="D64" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E64" s="19" t="n">
+      <c r="E64" s="24" t="n">
         <v>1.8385</v>
       </c>
       <c r="F64" s="10" t="n"/>
@@ -4956,30 +4986,30 @@
       <c r="D66" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E66" s="19" t="n">
+      <c r="E66" s="24" t="n">
         <v>1.8043</v>
       </c>
       <c r="F66" s="10" t="n"/>
     </row>
     <row r="67">
-      <c r="A67" s="22" t="n">
+      <c r="A67" s="27" t="n">
         <v>25</v>
       </c>
-      <c r="B67" s="22" t="inlineStr">
+      <c r="B67" s="27" t="inlineStr">
         <is>
           <t>Joanne Karla Caldit Consuelo</t>
         </is>
       </c>
-      <c r="C67" s="22" t="n">
+      <c r="C67" s="27" t="n">
         <v>363</v>
       </c>
-      <c r="D67" s="22" t="n">
+      <c r="D67" s="27" t="n">
         <v>216</v>
       </c>
       <c r="E67" s="11" t="n">
         <v>1.6806</v>
       </c>
-      <c r="F67" s="22" t="n"/>
+      <c r="F67" s="27" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="10" t="n">
@@ -4996,7 +5026,7 @@
       <c r="D68" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E68" s="19" t="n">
+      <c r="E68" s="24" t="n">
         <v>1.7906</v>
       </c>
       <c r="F68" s="10" t="n"/>
@@ -5064,7 +5094,7 @@
       <c r="D71" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E71" s="19" t="n">
+      <c r="E71" s="24" t="n">
         <v>1.8188</v>
       </c>
       <c r="F71" s="10" t="n"/>
@@ -5204,7 +5234,7 @@
       <c r="D77" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E77" s="19" t="n">
+      <c r="E77" s="24" t="n">
         <v>1.7628</v>
       </c>
       <c r="F77" s="10" t="n"/>
@@ -5272,7 +5302,7 @@
       <c r="D80" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E80" s="19" t="n">
+      <c r="E80" s="24" t="n">
         <v>1.8073</v>
       </c>
       <c r="F80" s="10" t="n"/>
@@ -5292,7 +5322,7 @@
       <c r="D81" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E81" s="19" t="n">
+      <c r="E81" s="24" t="n">
         <v>1.7872</v>
       </c>
       <c r="F81" s="10" t="n"/>
@@ -5384,7 +5414,7 @@
       <c r="D85" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E85" s="19" t="n">
+      <c r="E85" s="24" t="n">
         <v>1.8256</v>
       </c>
       <c r="F85" s="10" t="n"/>
@@ -5620,7 +5650,7 @@
       <c r="D95" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E95" s="19" t="n">
+      <c r="E95" s="24" t="n">
         <v>1.8526</v>
       </c>
       <c r="F95" s="10" t="n"/>
@@ -5736,7 +5766,7 @@
       <c r="D100" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E100" s="19" t="n">
+      <c r="E100" s="24" t="n">
         <v>1.7641</v>
       </c>
       <c r="F100" s="10" t="n"/>
@@ -5780,7 +5810,7 @@
       <c r="D102" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E102" s="19" t="n">
+      <c r="E102" s="24" t="n">
         <v>1.7833</v>
       </c>
       <c r="F102" s="10" t="n"/>
@@ -5848,7 +5878,7 @@
       <c r="D105" s="10" t="n">
         <v>234</v>
       </c>
-      <c r="E105" s="19" t="n">
+      <c r="E105" s="24" t="n">
         <v>1.8004</v>
       </c>
       <c r="F105" s="10" t="n"/>
@@ -5902,21 +5932,21 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="18" t="inlineStr">
+      <c r="A109" s="19" t="inlineStr">
         <is>
           <t>Note: Subject for verification/recommendation/approval by the University Evaluation/Review</t>
         </is>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="23" t="inlineStr">
+      <c r="A110" s="28" t="inlineStr">
         <is>
           <t>Committee on Honor Graduates</t>
         </is>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="18" t="inlineStr">
+      <c r="A112" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">Attached are the individual collegiate student's permanent record with the individual computation of </t>
         </is>
@@ -5937,83 +5967,83 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="24" t="inlineStr">
+      <c r="A116" s="29" t="inlineStr">
         <is>
           <t>COLLEGE/CAMPUS EVALUATION/REVIEW COMMITTEE</t>
         </is>
       </c>
     </row>
     <row r="118">
-      <c r="B118" s="24" t="inlineStr">
+      <c r="B118" s="29" t="inlineStr">
         <is>
           <t>Member N. Name</t>
         </is>
       </c>
-      <c r="F118" s="24" t="inlineStr">
+      <c r="F118" s="29" t="inlineStr">
         <is>
           <t>Member N. Name</t>
         </is>
       </c>
     </row>
     <row r="119">
-      <c r="B119" s="25" t="inlineStr">
+      <c r="B119" s="30" t="inlineStr">
         <is>
           <t>Member</t>
         </is>
       </c>
-      <c r="F119" s="25" t="inlineStr">
+      <c r="F119" s="30" t="inlineStr">
         <is>
           <t>Member</t>
         </is>
       </c>
     </row>
     <row r="122">
-      <c r="B122" s="24" t="inlineStr">
+      <c r="B122" s="29" t="inlineStr">
         <is>
           <t>Member N. Name</t>
         </is>
       </c>
-      <c r="F122" s="24" t="inlineStr">
+      <c r="F122" s="29" t="inlineStr">
         <is>
           <t>Member N. Name</t>
         </is>
       </c>
     </row>
     <row r="123">
-      <c r="B123" s="25" t="inlineStr">
+      <c r="B123" s="30" t="inlineStr">
         <is>
           <t>Member</t>
         </is>
       </c>
-      <c r="F123" s="25" t="inlineStr">
+      <c r="F123" s="30" t="inlineStr">
         <is>
           <t>Member</t>
         </is>
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="24" t="inlineStr">
+      <c r="A125" s="29" t="inlineStr">
         <is>
           <t>Co-chair N. Name</t>
         </is>
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="25" t="inlineStr">
+      <c r="A126" s="30" t="inlineStr">
         <is>
           <t>Co-Chairman</t>
         </is>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="24" t="inlineStr">
+      <c r="A128" s="29" t="inlineStr">
         <is>
           <t>Chairperson N. Name</t>
         </is>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="25" t="inlineStr">
+      <c r="A129" s="30" t="inlineStr">
         <is>
           <t>Chairperson</t>
         </is>

</xml_diff>

<commit_message>
column EFG size adjusted
</commit_message>
<xml_diff>
--- a/static/Honors.xlsx
+++ b/static/Honors.xlsx
@@ -621,9 +621,9 @@
     <col width="25" bestFit="1" customWidth="1" min="2" max="2"/>
     <col width="7" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="7" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="9" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="9" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="9" customWidth="1" min="7" max="7"/>
+    <col width="8" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="8" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
rank sheet col dimension update
</commit_message>
<xml_diff>
--- a/static/Honors.xlsx
+++ b/static/Honors.xlsx
@@ -627,13 +627,13 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="5" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="25" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="30" bestFit="1" customWidth="1" min="2" max="2"/>
     <col width="7" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="7" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="8" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="8" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="7" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="7" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>